<commit_message>
Apply a growth constraint for wave and tidal
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD00383-B3FD-47AE-BB8B-CFE5F7B330DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2659BC-D81E-4F42-8537-0173AB60FA72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="162">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -553,19 +553,28 @@
     <t>LGT-Maximum growth rate of NG-ICEs</t>
   </si>
   <si>
-    <t>UC-PWR_MaxGrowthCCS</t>
-  </si>
-  <si>
     <t>Max growth rate</t>
   </si>
   <si>
-    <t>PWR CCS maximum growth rate</t>
-  </si>
-  <si>
     <t>P*CCS*</t>
   </si>
   <si>
     <t>Starting value (GW)</t>
+  </si>
+  <si>
+    <t>CCS</t>
+  </si>
+  <si>
+    <t>Wave</t>
+  </si>
+  <si>
+    <t>Tidal</t>
+  </si>
+  <si>
+    <t>P*OCE*TID*</t>
+  </si>
+  <si>
+    <t>P*OCE*WAV*</t>
   </si>
 </sst>
 </file>
@@ -3669,18 +3678,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A87F6E-94AE-4E0F-A04E-E84AF9E35740}">
-  <dimension ref="B2:N12"/>
+  <dimension ref="A2:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:AD3)</f>
         <v>~UC_Sets: R_E: IE,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
@@ -3698,7 +3709,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -3715,7 +3726,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -3732,7 +3743,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -3773,9 +3784,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
-        <v>154</v>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="18" t="str">
+        <f>_xlfn.TEXTJOIN("",TRUE,"UC-PWR_MaxGrowth",A12)</f>
+        <v>UC-PWR_MaxGrowthCCS</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>13</v>
@@ -3784,7 +3796,7 @@
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H6" s="18">
         <v>2018</v>
@@ -3793,7 +3805,7 @@
         <v>15</v>
       </c>
       <c r="J6" s="29">
-        <f>1+$B$12</f>
+        <f>1+$B12</f>
         <v>1.2</v>
       </c>
       <c r="K6" s="18">
@@ -3806,24 +3818,122 @@
       <c r="M6" s="18">
         <v>5</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="N6" s="18" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,"PWR",A12, "maximum growth rate")</f>
+        <v>PWR CCS maximum growth rate</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="18" t="str">
+        <f t="shared" ref="B7:B8" si="0">_xlfn.TEXTJOIN("",TRUE,"UC-PWR_MaxGrowth",A13)</f>
+        <v>UC-PWR_MaxGrowthWave</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="H7">
+        <v>2035</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="29">
+        <f t="shared" ref="J7:J8" si="1">1+$B13</f>
+        <v>1.2</v>
+      </c>
+      <c r="K7" s="18">
+        <v>1</v>
+      </c>
+      <c r="L7" s="19">
+        <f t="shared" ref="L7:L8" si="2">-D13</f>
+        <v>-0.4</v>
+      </c>
+      <c r="M7" s="18">
+        <v>5</v>
+      </c>
+      <c r="N7" s="18" t="str">
+        <f t="shared" ref="N7:N8" si="3">_xlfn.TEXTJOIN(" ",TRUE,"PWR",A13, "maximum growth rate")</f>
+        <v>PWR Wave maximum growth rate</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-PWR_MaxGrowthTidal</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="H8">
+        <v>2035</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="29">
+        <f t="shared" si="1"/>
+        <v>1.2</v>
+      </c>
+      <c r="K8" s="18">
+        <v>1</v>
+      </c>
+      <c r="L8" s="19">
+        <f t="shared" si="2"/>
+        <v>-0.1</v>
+      </c>
+      <c r="M8" s="18">
+        <v>5</v>
+      </c>
+      <c r="N8" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>PWR Tidal maximum growth rate</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D11" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>155</v>
-      </c>
-      <c r="D11" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>157</v>
+      </c>
       <c r="B12" s="13">
         <v>0.2</v>
       </c>
       <c r="D12">
         <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D13">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B14" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D14">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -3832,21 +3942,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -4057,24 +4152,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4091,4 +4184,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Change UC_MaxGrowthRate for TRA
Increased growth rates and seed values for AFV
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\ccr-40\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2659BC-D81E-4F42-8537-0173AB60FA72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98366B3-8C1A-4028-9EFF-AAC00C655CAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="4530" yWindow="16050" windowWidth="19650" windowHeight="11070" activeTab="1" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="161">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -553,28 +553,25 @@
     <t>LGT-Maximum growth rate of NG-ICEs</t>
   </si>
   <si>
+    <t>UC-PWR_MaxGrowthCCS</t>
+  </si>
+  <si>
     <t>Max growth rate</t>
   </si>
   <si>
+    <t>PWR CCS maximum growth rate</t>
+  </si>
+  <si>
     <t>P*CCS*</t>
   </si>
   <si>
     <t>Starting value (GW)</t>
   </si>
   <si>
-    <t>CCS</t>
-  </si>
-  <si>
-    <t>Wave</t>
-  </si>
-  <si>
-    <t>Tidal</t>
-  </si>
-  <si>
-    <t>P*OCE*TID*</t>
-  </si>
-  <si>
-    <t>P*OCE*WAV*</t>
+    <t>Seed value (% of 2018 sales)</t>
+  </si>
+  <si>
+    <t>Total stock 2018</t>
   </si>
 </sst>
 </file>
@@ -984,7 +981,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1026,6 +1023,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="217">
     <cellStyle name="20% - Accent5 2" xfId="10" xr:uid="{72E8C261-0B7B-4154-8B6F-C9901D88251B}"/>
@@ -2387,10 +2385,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
-  <dimension ref="A2:O52"/>
+  <dimension ref="A2:P52"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2405,7 +2403,8 @@
     <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.5703125" customWidth="1"/>
     <col min="14" max="14" width="34" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
@@ -2527,14 +2526,14 @@
       </c>
       <c r="J6" s="29">
         <f t="shared" ref="J6:J23" si="0">1+$B$46</f>
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="K6" s="18">
         <v>1</v>
       </c>
       <c r="L6" s="19">
         <f>-C52/1000</f>
-        <v>-24.2242</v>
+        <v>-18.168149999999997</v>
       </c>
       <c r="M6" s="18">
         <v>5</v>
@@ -2566,14 +2565,14 @@
       </c>
       <c r="J7" s="29">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="K7" s="18">
         <v>1</v>
       </c>
       <c r="L7" s="19">
         <f>-C52/1000</f>
-        <v>-24.2242</v>
+        <v>-18.168149999999997</v>
       </c>
       <c r="M7" s="18">
         <v>5</v>
@@ -2605,14 +2604,14 @@
       </c>
       <c r="J8" s="29">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="K8" s="18">
         <v>1</v>
       </c>
       <c r="L8" s="19">
         <f>-C52/1000</f>
-        <v>-24.2242</v>
+        <v>-18.168149999999997</v>
       </c>
       <c r="M8" s="18">
         <v>5</v>
@@ -2644,14 +2643,14 @@
       </c>
       <c r="J9" s="30">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="K9" s="21">
         <v>1</v>
       </c>
       <c r="L9" s="22">
         <f>-C52/1000</f>
-        <v>-24.2242</v>
+        <v>-18.168149999999997</v>
       </c>
       <c r="M9" s="21">
         <v>5</v>
@@ -2683,14 +2682,14 @@
       </c>
       <c r="J10" s="29">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="K10" s="18">
         <v>1</v>
       </c>
       <c r="L10" s="19">
         <f>-C51/1000</f>
-        <v>-1.6539000000000001</v>
+        <v>-2.4808499999999998</v>
       </c>
       <c r="M10" s="18">
         <v>5</v>
@@ -2722,14 +2721,14 @@
       </c>
       <c r="J11" s="29">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="K11" s="18">
         <v>1</v>
       </c>
       <c r="L11" s="19">
         <f>-C51/1000</f>
-        <v>-1.6539000000000001</v>
+        <v>-2.4808499999999998</v>
       </c>
       <c r="M11" s="18">
         <v>5</v>
@@ -2761,14 +2760,14 @@
       </c>
       <c r="J12" s="29">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="K12" s="18">
         <v>1</v>
       </c>
       <c r="L12" s="19">
         <f>-C51/1000</f>
-        <v>-1.6539000000000001</v>
+        <v>-2.4808499999999998</v>
       </c>
       <c r="M12" s="18">
         <v>5</v>
@@ -2800,14 +2799,14 @@
       </c>
       <c r="J13" s="30">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="K13" s="21">
         <v>1</v>
       </c>
       <c r="L13" s="22">
         <f>-C51/1000</f>
-        <v>-1.6539000000000001</v>
+        <v>-2.4808499999999998</v>
       </c>
       <c r="M13" s="21">
         <v>5</v>
@@ -2839,14 +2838,14 @@
       </c>
       <c r="J14" s="29">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="K14" s="18">
         <v>1</v>
       </c>
       <c r="L14" s="19">
         <f>-C50/1000</f>
-        <v>-5.2999999999999999E-2</v>
+        <v>-7.9500000000000001E-2</v>
       </c>
       <c r="M14" s="18">
         <v>5</v>
@@ -2878,14 +2877,14 @@
       </c>
       <c r="J15" s="29">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="K15" s="18">
         <v>1</v>
       </c>
       <c r="L15" s="19">
         <f>-C50/1000</f>
-        <v>-5.2999999999999999E-2</v>
+        <v>-7.9500000000000001E-2</v>
       </c>
       <c r="M15" s="18">
         <v>5</v>
@@ -2917,14 +2916,14 @@
       </c>
       <c r="J16" s="29">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="K16" s="18">
         <v>1</v>
       </c>
       <c r="L16" s="19">
         <f>-C50/1000</f>
-        <v>-5.2999999999999999E-2</v>
+        <v>-7.9500000000000001E-2</v>
       </c>
       <c r="M16" s="18">
         <v>5</v>
@@ -2956,14 +2955,14 @@
       </c>
       <c r="J17" s="29">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="K17" s="18">
         <v>1</v>
       </c>
       <c r="L17" s="19">
         <f>-C50/1000</f>
-        <v>-5.2999999999999999E-2</v>
+        <v>-7.9500000000000001E-2</v>
       </c>
       <c r="M17" s="18">
         <v>5</v>
@@ -2995,14 +2994,14 @@
       </c>
       <c r="J18" s="30">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="K18" s="21">
         <v>1</v>
       </c>
       <c r="L18" s="22">
         <f>-C50/1000</f>
-        <v>-5.2999999999999999E-2</v>
+        <v>-7.9500000000000001E-2</v>
       </c>
       <c r="M18" s="21">
         <v>5</v>
@@ -3034,14 +3033,14 @@
       </c>
       <c r="J19" s="29">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="K19" s="18">
         <v>1</v>
       </c>
       <c r="L19" s="19">
         <f>-C49/1000</f>
-        <v>-0.15180000000000002</v>
+        <v>-0.22769999999999999</v>
       </c>
       <c r="M19" s="18">
         <v>5</v>
@@ -3073,14 +3072,14 @@
       </c>
       <c r="J20" s="29">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="K20" s="18">
         <v>1</v>
       </c>
       <c r="L20" s="19">
         <f>-C49/1000</f>
-        <v>-0.15180000000000002</v>
+        <v>-0.22769999999999999</v>
       </c>
       <c r="M20" s="18">
         <v>5</v>
@@ -3112,14 +3111,14 @@
       </c>
       <c r="J21" s="29">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="K21" s="18">
         <v>1</v>
       </c>
       <c r="L21" s="19">
         <f>-C49/1000</f>
-        <v>-0.15180000000000002</v>
+        <v>-0.22769999999999999</v>
       </c>
       <c r="M21" s="18">
         <v>5</v>
@@ -3151,14 +3150,14 @@
       </c>
       <c r="J22" s="29">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="K22" s="18">
         <v>1</v>
       </c>
       <c r="L22" s="19">
         <f>-C49/1000</f>
-        <v>-0.15180000000000002</v>
+        <v>-0.22769999999999999</v>
       </c>
       <c r="M22" s="18">
         <v>5</v>
@@ -3191,14 +3190,14 @@
       </c>
       <c r="J23" s="30">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="K23" s="21">
         <v>1</v>
       </c>
       <c r="L23" s="22">
         <f>-C49/1000</f>
-        <v>-0.15180000000000002</v>
+        <v>-0.22769999999999999</v>
       </c>
       <c r="M23" s="21">
         <v>5</v>
@@ -3291,7 +3290,7 @@
         <v>4.9391983185707852E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="31"/>
       <c r="B33" s="3" t="s">
         <v>22</v>
@@ -3307,7 +3306,7 @@
         <v>5.7573599240265907E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="31"/>
       <c r="B34" s="3" t="s">
         <v>21</v>
@@ -3323,7 +3322,7 @@
         <v>7.187086899046824E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>20</v>
       </c>
@@ -3338,7 +3337,7 @@
         <v>5.5865068892149296E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>19</v>
       </c>
@@ -3353,7 +3352,7 @@
         <v>6.1874562947601935E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>18</v>
       </c>
@@ -3368,7 +3367,7 @@
         <v>5.7044321200540614E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="7" t="s">
         <v>17</v>
@@ -3384,22 +3383,28 @@
         <v>4.9170087453150095E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B46" s="13">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="C46" s="13">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C47">
         <v>2018</v>
       </c>
@@ -3430,8 +3435,20 @@
       <c r="L47">
         <v>2027</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M47">
+        <v>2028</v>
+      </c>
+      <c r="N47">
+        <v>2029</v>
+      </c>
+      <c r="O47">
+        <v>2030</v>
+      </c>
+      <c r="P47" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>34</v>
       </c>
@@ -3465,8 +3482,17 @@
       <c r="L48">
         <v>10</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M48">
+        <v>10</v>
+      </c>
+      <c r="N48">
+        <v>10</v>
+      </c>
+      <c r="O48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -3475,48 +3501,63 @@
         <v>1518</v>
       </c>
       <c r="C49" s="14">
-        <f>B49/10</f>
-        <v>151.80000000000001</v>
+        <f>B49*$C$46</f>
+        <v>227.7</v>
       </c>
       <c r="D49" s="14">
-        <f t="shared" ref="D49:L49" si="3">C49*(1+$B$46)</f>
-        <v>182.16</v>
+        <f>C49*(1+$B$46)</f>
+        <v>341.54999999999995</v>
       </c>
       <c r="E49" s="20">
-        <f t="shared" si="3"/>
-        <v>218.59199999999998</v>
+        <f t="shared" ref="D49:L49" si="3">D49*(1+$B$46)</f>
+        <v>512.32499999999993</v>
       </c>
       <c r="F49" s="14">
         <f t="shared" si="3"/>
-        <v>262.31039999999996</v>
+        <v>768.48749999999995</v>
       </c>
       <c r="G49" s="14">
         <f t="shared" si="3"/>
-        <v>314.77247999999992</v>
+        <v>1152.7312499999998</v>
       </c>
       <c r="H49" s="14">
         <f t="shared" si="3"/>
-        <v>377.72697599999987</v>
+        <v>1729.0968749999997</v>
       </c>
       <c r="I49" s="14">
-        <f t="shared" si="3"/>
-        <v>453.27237119999984</v>
+        <f t="shared" ref="I49" si="4">H49*(1+$B$46)</f>
+        <v>2593.6453124999998</v>
       </c>
       <c r="J49" s="14">
-        <f t="shared" si="3"/>
-        <v>543.92684543999974</v>
+        <f t="shared" ref="J49" si="5">I49*(1+$B$46)</f>
+        <v>3890.4679687499997</v>
       </c>
       <c r="K49" s="14">
-        <f t="shared" si="3"/>
-        <v>652.71221452799966</v>
+        <f t="shared" ref="K49" si="6">J49*(1+$B$46)</f>
+        <v>5835.7019531249998</v>
       </c>
       <c r="L49" s="14">
-        <f t="shared" si="3"/>
-        <v>783.25465743359962</v>
-      </c>
-      <c r="M49" s="14"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" ref="L49" si="7">K49*(1+$B$46)</f>
+        <v>8753.5529296874993</v>
+      </c>
+      <c r="M49" s="14">
+        <f t="shared" ref="M49" si="8">L49*(1+$B$46)</f>
+        <v>13130.329394531249</v>
+      </c>
+      <c r="N49" s="14">
+        <f t="shared" ref="N49" si="9">M49*(1+$B$46)</f>
+        <v>19695.494091796874</v>
+      </c>
+      <c r="O49" s="32">
+        <f>N49*(1+$B$46)</f>
+        <v>29543.24113769531</v>
+      </c>
+      <c r="P49" s="15">
+        <f>C34+C33</f>
+        <v>22797</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>36</v>
       </c>
@@ -3525,48 +3566,63 @@
         <v>530</v>
       </c>
       <c r="C50" s="14">
-        <f>B50/10</f>
-        <v>53</v>
+        <f>B50*$C$46</f>
+        <v>79.5</v>
       </c>
       <c r="D50" s="14">
-        <f t="shared" ref="D50:L50" si="4">C50*(1+$B$46)</f>
-        <v>63.599999999999994</v>
+        <f t="shared" ref="D50:L50" si="10">C50*(1+$B$46)</f>
+        <v>119.25</v>
       </c>
       <c r="E50" s="20">
-        <f t="shared" si="4"/>
-        <v>76.319999999999993</v>
+        <f t="shared" si="10"/>
+        <v>178.875</v>
       </c>
       <c r="F50" s="14">
-        <f t="shared" si="4"/>
-        <v>91.583999999999989</v>
+        <f t="shared" si="10"/>
+        <v>268.3125</v>
       </c>
       <c r="G50" s="14">
-        <f t="shared" si="4"/>
-        <v>109.90079999999999</v>
+        <f t="shared" si="10"/>
+        <v>402.46875</v>
       </c>
       <c r="H50" s="14">
-        <f t="shared" si="4"/>
-        <v>131.88095999999999</v>
+        <f t="shared" si="10"/>
+        <v>603.703125</v>
       </c>
       <c r="I50" s="14">
-        <f t="shared" si="4"/>
-        <v>158.25715199999999</v>
+        <f t="shared" si="10"/>
+        <v>905.5546875</v>
       </c>
       <c r="J50" s="14">
-        <f t="shared" si="4"/>
-        <v>189.90858239999997</v>
+        <f t="shared" si="10"/>
+        <v>1358.33203125</v>
       </c>
       <c r="K50" s="14">
-        <f t="shared" si="4"/>
-        <v>227.89029887999996</v>
+        <f t="shared" si="10"/>
+        <v>2037.498046875</v>
       </c>
       <c r="L50" s="14">
-        <f t="shared" si="4"/>
-        <v>273.46835865599996</v>
-      </c>
-      <c r="M50" s="14"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="10"/>
+        <v>3056.2470703125</v>
+      </c>
+      <c r="M50" s="14">
+        <f t="shared" ref="M49:M52" si="11">L50*(1+$B$46)</f>
+        <v>4584.37060546875</v>
+      </c>
+      <c r="N50" s="14">
+        <f t="shared" ref="N49:N52" si="12">M50*(1+$B$46)</f>
+        <v>6876.555908203125</v>
+      </c>
+      <c r="O50" s="32">
+        <f t="shared" ref="O49:O52" si="13">N50*(1+$B$46)</f>
+        <v>10314.833862304688</v>
+      </c>
+      <c r="P50" s="15">
+        <f>C32+C31</f>
+        <v>11207</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>37</v>
       </c>
@@ -3575,48 +3631,63 @@
         <v>16539</v>
       </c>
       <c r="C51" s="14">
-        <f>B51/10</f>
-        <v>1653.9</v>
+        <f>B51*$C$46</f>
+        <v>2480.85</v>
       </c>
       <c r="D51" s="14">
         <f>C51*(1+$B$46)</f>
-        <v>1984.68</v>
+        <v>3721.2749999999996</v>
       </c>
       <c r="E51" s="20">
-        <f t="shared" ref="E51:L51" si="5">D51*(1+$B$46)</f>
-        <v>2381.616</v>
+        <f t="shared" ref="E51:L51" si="14">D51*(1+$B$46)</f>
+        <v>5581.9124999999995</v>
       </c>
       <c r="F51" s="14">
-        <f t="shared" si="5"/>
-        <v>2857.9391999999998</v>
+        <f t="shared" si="14"/>
+        <v>8372.8687499999996</v>
       </c>
       <c r="G51" s="14">
-        <f t="shared" si="5"/>
-        <v>3429.5270399999995</v>
+        <f t="shared" si="14"/>
+        <v>12559.303124999999</v>
       </c>
       <c r="H51" s="14">
-        <f t="shared" si="5"/>
-        <v>4115.4324479999996</v>
+        <f t="shared" si="14"/>
+        <v>18838.954687499998</v>
       </c>
       <c r="I51" s="14">
-        <f t="shared" si="5"/>
-        <v>4938.5189375999989</v>
+        <f t="shared" si="14"/>
+        <v>28258.432031249999</v>
       </c>
       <c r="J51" s="14">
-        <f t="shared" si="5"/>
-        <v>5926.2227251199984</v>
+        <f t="shared" si="14"/>
+        <v>42387.648046874994</v>
       </c>
       <c r="K51" s="14">
-        <f t="shared" si="5"/>
-        <v>7111.4672701439977</v>
+        <f t="shared" si="14"/>
+        <v>63581.472070312491</v>
       </c>
       <c r="L51" s="14">
-        <f t="shared" si="5"/>
-        <v>8533.7607241727965</v>
-      </c>
-      <c r="M51" s="14"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="14"/>
+        <v>95372.208105468744</v>
+      </c>
+      <c r="M51" s="14">
+        <f t="shared" si="11"/>
+        <v>143058.3121582031</v>
+      </c>
+      <c r="N51" s="14">
+        <f t="shared" si="12"/>
+        <v>214587.46823730465</v>
+      </c>
+      <c r="O51" s="32">
+        <f t="shared" si="13"/>
+        <v>321881.20235595701</v>
+      </c>
+      <c r="P51" s="15">
+        <f>C30+C29</f>
+        <v>328695</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>38</v>
       </c>
@@ -3625,46 +3696,61 @@
         <v>121121</v>
       </c>
       <c r="C52" s="14">
-        <f>B52/5</f>
-        <v>24224.2</v>
+        <f>B52*$C$46</f>
+        <v>18168.149999999998</v>
       </c>
       <c r="D52" s="14">
-        <f t="shared" ref="D52:L52" si="6">C52*(1+$B$46)</f>
-        <v>29069.040000000001</v>
+        <f t="shared" ref="D52:L52" si="15">C52*(1+$B$46)</f>
+        <v>27252.224999999999</v>
       </c>
       <c r="E52" s="20">
-        <f t="shared" si="6"/>
-        <v>34882.847999999998</v>
+        <f t="shared" si="15"/>
+        <v>40878.337499999994</v>
       </c>
       <c r="F52" s="14">
-        <f t="shared" si="6"/>
-        <v>41859.417599999993</v>
+        <f t="shared" si="15"/>
+        <v>61317.506249999991</v>
       </c>
       <c r="G52" s="14">
-        <f t="shared" si="6"/>
-        <v>50231.301119999989</v>
+        <f t="shared" si="15"/>
+        <v>91976.259374999994</v>
       </c>
       <c r="H52" s="14">
-        <f t="shared" si="6"/>
-        <v>60277.561343999987</v>
+        <f t="shared" si="15"/>
+        <v>137964.38906249998</v>
       </c>
       <c r="I52" s="14">
-        <f t="shared" si="6"/>
-        <v>72333.073612799984</v>
+        <f t="shared" si="15"/>
+        <v>206946.58359374997</v>
       </c>
       <c r="J52" s="14">
-        <f t="shared" si="6"/>
-        <v>86799.688335359984</v>
+        <f t="shared" si="15"/>
+        <v>310419.87539062498</v>
       </c>
       <c r="K52" s="14">
-        <f t="shared" si="6"/>
-        <v>104159.62600243198</v>
+        <f t="shared" si="15"/>
+        <v>465629.81308593747</v>
       </c>
       <c r="L52" s="14">
-        <f t="shared" si="6"/>
-        <v>124991.55120291837</v>
-      </c>
-      <c r="M52" s="14"/>
+        <f t="shared" si="15"/>
+        <v>698444.71962890623</v>
+      </c>
+      <c r="M52" s="14">
+        <f t="shared" si="11"/>
+        <v>1047667.0794433593</v>
+      </c>
+      <c r="N52" s="14">
+        <f t="shared" si="12"/>
+        <v>1571500.6191650389</v>
+      </c>
+      <c r="O52" s="32">
+        <f t="shared" si="13"/>
+        <v>2357250.9287475585</v>
+      </c>
+      <c r="P52" s="15">
+        <f>C35</f>
+        <v>2168099</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3678,20 +3764,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A87F6E-94AE-4E0F-A04E-E84AF9E35740}">
-  <dimension ref="A2:N14"/>
+  <dimension ref="B2:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:AD3)</f>
         <v>~UC_Sets: R_E: IE,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
@@ -3709,7 +3793,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -3726,7 +3810,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -3743,7 +3827,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -3784,10 +3868,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",TRUE,"UC-PWR_MaxGrowth",A12)</f>
-        <v>UC-PWR_MaxGrowthCCS</v>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="18" t="s">
+        <v>154</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>13</v>
@@ -3796,7 +3879,7 @@
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H6" s="18">
         <v>2018</v>
@@ -3805,7 +3888,7 @@
         <v>15</v>
       </c>
       <c r="J6" s="29">
-        <f>1+$B12</f>
+        <f>1+$B$12</f>
         <v>1.2</v>
       </c>
       <c r="K6" s="18">
@@ -3818,122 +3901,24 @@
       <c r="M6" s="18">
         <v>5</v>
       </c>
-      <c r="N6" s="18" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,"PWR",A12, "maximum growth rate")</f>
-        <v>PWR CCS maximum growth rate</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="str">
-        <f t="shared" ref="B7:B8" si="0">_xlfn.TEXTJOIN("",TRUE,"UC-PWR_MaxGrowth",A13)</f>
-        <v>UC-PWR_MaxGrowthWave</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="H7">
-        <v>2035</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="29">
-        <f t="shared" ref="J7:J8" si="1">1+$B13</f>
-        <v>1.2</v>
-      </c>
-      <c r="K7" s="18">
-        <v>1</v>
-      </c>
-      <c r="L7" s="19">
-        <f t="shared" ref="L7:L8" si="2">-D13</f>
-        <v>-0.4</v>
-      </c>
-      <c r="M7" s="18">
-        <v>5</v>
-      </c>
-      <c r="N7" s="18" t="str">
-        <f t="shared" ref="N7:N8" si="3">_xlfn.TEXTJOIN(" ",TRUE,"PWR",A13, "maximum growth rate")</f>
-        <v>PWR Wave maximum growth rate</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UC-PWR_MaxGrowthTidal</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="H8">
-        <v>2035</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="29">
-        <f t="shared" si="1"/>
-        <v>1.2</v>
-      </c>
-      <c r="K8" s="18">
-        <v>1</v>
-      </c>
-      <c r="L8" s="19">
-        <f t="shared" si="2"/>
-        <v>-0.1</v>
-      </c>
-      <c r="M8" s="18">
-        <v>5</v>
-      </c>
-      <c r="N8" s="18" t="str">
-        <f t="shared" si="3"/>
-        <v>PWR Tidal maximum growth rate</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N6" s="18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>157</v>
-      </c>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="13">
         <v>0.2</v>
       </c>
       <c r="D12">
         <v>0.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>158</v>
-      </c>
-      <c r="B13" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="D13">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>159</v>
-      </c>
-      <c r="B14" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="D14">
-        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reapply growth constraint for wave and tidal
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\ccr-40\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98366B3-8C1A-4028-9EFF-AAC00C655CAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87645595-8646-4B9E-9D14-B92A1A4C22D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4530" yWindow="16050" windowWidth="19650" windowHeight="11070" activeTab="1" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
-    <sheet name="TRA" sheetId="1" r:id="rId2"/>
-    <sheet name="PWR" sheetId="3" r:id="rId3"/>
+    <sheet name="PWR" sheetId="4" r:id="rId2"/>
+    <sheet name="TRA" sheetId="1" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <definedNames>
+    <definedName name="__123Graph_AEUMILKPN" localSheetId="1" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
+    <definedName name="_Regression_Y" localSheetId="1" hidden="1">#REF!</definedName>
     <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
+    <definedName name="aa" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="table6" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -69,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="164">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -553,15 +565,9 @@
     <t>LGT-Maximum growth rate of NG-ICEs</t>
   </si>
   <si>
-    <t>UC-PWR_MaxGrowthCCS</t>
-  </si>
-  <si>
     <t>Max growth rate</t>
   </si>
   <si>
-    <t>PWR CCS maximum growth rate</t>
-  </si>
-  <si>
     <t>P*CCS*</t>
   </si>
   <si>
@@ -572,6 +578,21 @@
   </si>
   <si>
     <t>Total stock 2018</t>
+  </si>
+  <si>
+    <t>P*OCE*TID*</t>
+  </si>
+  <si>
+    <t>P*OCE*WAV*</t>
+  </si>
+  <si>
+    <t>CCS</t>
+  </si>
+  <si>
+    <t>Wave</t>
+  </si>
+  <si>
+    <t>Tidal</t>
   </si>
 </sst>
 </file>
@@ -981,7 +1002,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1020,10 +1041,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="217">
     <cellStyle name="20% - Accent5 2" xfId="10" xr:uid="{72E8C261-0B7B-4154-8B6F-C9901D88251B}"/>
@@ -1322,6 +1345,23 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Regions"/>
+      <sheetName val="TRA"/>
+      <sheetName val="PWR"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2384,10 +2424,275 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B92B0C-7472-4C75-A119-CE0EE6C8A8E0}">
+  <dimension ref="A2:N14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="str">
+        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:AD3)</f>
+        <v>~UC_Sets: R_E: IE,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("",TRUE,"UC-PWR_MaxGrowth",A12)</f>
+        <v>UC-PWR_MaxGrowthCCS</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2018</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="33">
+        <f>1+$B12</f>
+        <v>1.2</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+      <c r="L6" s="34">
+        <f>-D12</f>
+        <v>-0.4</v>
+      </c>
+      <c r="M6" s="2">
+        <v>5</v>
+      </c>
+      <c r="N6" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,"PWR",A12, "maximum growth rate")</f>
+        <v>PWR CCS maximum growth rate</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="str">
+        <f t="shared" ref="B7:B8" si="0">_xlfn.TEXTJOIN("",TRUE,"UC-PWR_MaxGrowth",A13)</f>
+        <v>UC-PWR_MaxGrowthWave</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H7">
+        <v>2035</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="33">
+        <f t="shared" ref="J7:J8" si="1">1+$B13</f>
+        <v>1.2</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="34">
+        <f t="shared" ref="L7:L8" si="2">-D13</f>
+        <v>-0.4</v>
+      </c>
+      <c r="M7" s="2">
+        <v>5</v>
+      </c>
+      <c r="N7" s="2" t="str">
+        <f t="shared" ref="N7:N8" si="3">_xlfn.TEXTJOIN(" ",TRUE,"PWR",A13, "maximum growth rate")</f>
+        <v>PWR Wave maximum growth rate</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-PWR_MaxGrowthTidal</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H8">
+        <v>2035</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="33">
+        <f t="shared" si="1"/>
+        <v>1.2</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="34">
+        <f t="shared" si="2"/>
+        <v>-0.1</v>
+      </c>
+      <c r="M8" s="2">
+        <v>5</v>
+      </c>
+      <c r="N8" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>PWR Tidal maximum growth rate</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D13">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>163</v>
+      </c>
+      <c r="B14" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D14">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
   <dimension ref="A2:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
@@ -3225,7 +3530,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="32" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -3243,7 +3548,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
+      <c r="A30" s="32"/>
       <c r="B30" s="3" t="s">
         <v>25</v>
       </c>
@@ -3259,7 +3564,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="3" t="s">
         <v>24</v>
       </c>
@@ -3275,7 +3580,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
+      <c r="A32" s="32"/>
       <c r="B32" s="3" t="s">
         <v>23</v>
       </c>
@@ -3291,7 +3596,7 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="3" t="s">
         <v>22</v>
       </c>
@@ -3307,7 +3612,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
+      <c r="A34" s="32"/>
       <c r="B34" s="3" t="s">
         <v>21</v>
       </c>
@@ -3393,7 +3698,7 @@
         <v>33</v>
       </c>
       <c r="C45" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -3445,7 +3750,7 @@
         <v>2030</v>
       </c>
       <c r="P47" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -3509,7 +3814,7 @@
         <v>341.54999999999995</v>
       </c>
       <c r="E49" s="20">
-        <f t="shared" ref="D49:L49" si="3">D49*(1+$B$46)</f>
+        <f t="shared" ref="E49:H49" si="3">D49*(1+$B$46)</f>
         <v>512.32499999999993</v>
       </c>
       <c r="F49" s="14">
@@ -3548,7 +3853,7 @@
         <f t="shared" ref="N49" si="9">M49*(1+$B$46)</f>
         <v>19695.494091796874</v>
       </c>
-      <c r="O49" s="32">
+      <c r="O49" s="31">
         <f>N49*(1+$B$46)</f>
         <v>29543.24113769531</v>
       </c>
@@ -3606,15 +3911,15 @@
         <v>3056.2470703125</v>
       </c>
       <c r="M50" s="14">
-        <f t="shared" ref="M49:M52" si="11">L50*(1+$B$46)</f>
+        <f t="shared" ref="M50:M52" si="11">L50*(1+$B$46)</f>
         <v>4584.37060546875</v>
       </c>
       <c r="N50" s="14">
-        <f t="shared" ref="N49:N52" si="12">M50*(1+$B$46)</f>
+        <f t="shared" ref="N50:N52" si="12">M50*(1+$B$46)</f>
         <v>6876.555908203125</v>
       </c>
-      <c r="O50" s="32">
-        <f t="shared" ref="O49:O52" si="13">N50*(1+$B$46)</f>
+      <c r="O50" s="31">
+        <f t="shared" ref="O50:O52" si="13">N50*(1+$B$46)</f>
         <v>10314.833862304688</v>
       </c>
       <c r="P50" s="15">
@@ -3678,7 +3983,7 @@
         <f t="shared" si="12"/>
         <v>214587.46823730465</v>
       </c>
-      <c r="O51" s="32">
+      <c r="O51" s="31">
         <f t="shared" si="13"/>
         <v>321881.20235595701</v>
       </c>
@@ -3743,7 +4048,7 @@
         <f t="shared" si="12"/>
         <v>1571500.6191650389</v>
       </c>
-      <c r="O52" s="32">
+      <c r="O52" s="31">
         <f t="shared" si="13"/>
         <v>2357250.9287475585</v>
       </c>
@@ -3762,171 +4067,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A87F6E-94AE-4E0F-A04E-E84AF9E35740}">
-  <dimension ref="B2:N12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="str">
-        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:AD3)</f>
-        <v>~UC_Sets: R_E: IE,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="H6" s="18">
-        <v>2018</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="29">
-        <f>1+$B$12</f>
-        <v>1.2</v>
-      </c>
-      <c r="K6" s="18">
-        <v>1</v>
-      </c>
-      <c r="L6" s="19">
-        <f>-D12</f>
-        <v>-0.4</v>
-      </c>
-      <c r="M6" s="18">
-        <v>5</v>
-      </c>
-      <c r="N6" s="18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>155</v>
-      </c>
-      <c r="D11" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="D12">
-        <v>0.4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -4137,12 +4284,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4153,6 +4294,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4171,15 +4321,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Add max growth rate constraints for HPs in SRV
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,36 +8,43 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87645595-8646-4B9E-9D14-B92A1A4C22D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A179693-C30D-43DC-8BD4-BBCD21DEDB8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
     <sheet name="PWR" sheetId="4" r:id="rId2"/>
     <sheet name="TRA" sheetId="1" r:id="rId3"/>
+    <sheet name="SRV" sheetId="5" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="1" hidden="1">#REF!</definedName>
+    <definedName name="__123Graph_AEUMILKPN" localSheetId="3" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
     <definedName name="_Regression_Y" localSheetId="1" hidden="1">#REF!</definedName>
+    <definedName name="_Regression_Y" localSheetId="3" hidden="1">#REF!</definedName>
     <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
     <definedName name="aa" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="aa" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="table6" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -81,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="171">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -315,9 +322,6 @@
   </si>
   <si>
     <t>IE</t>
-  </si>
-  <si>
-    <t>*National</t>
   </si>
   <si>
     <t>Single-region</t>
@@ -593,6 +597,30 @@
   </si>
   <si>
     <t>Tidal</t>
+  </si>
+  <si>
+    <t>National</t>
+  </si>
+  <si>
+    <t>HPs</t>
+  </si>
+  <si>
+    <t>PWR</t>
+  </si>
+  <si>
+    <t>SRV-PU</t>
+  </si>
+  <si>
+    <t>SRV-CS</t>
+  </si>
+  <si>
+    <t>SRVAHT</t>
+  </si>
+  <si>
+    <t>S-SH*PU*</t>
+  </si>
+  <si>
+    <t>S-SH*CS*</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1030,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1042,11 +1070,12 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="217">
     <cellStyle name="20% - Accent5 2" xfId="10" xr:uid="{72E8C261-0B7B-4154-8B6F-C9901D88251B}"/>
@@ -1345,23 +1374,6 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Regions"/>
-      <sheetName val="TRA"/>
-      <sheetName val="PWR"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1664,7 +1676,7 @@
   <dimension ref="A3:AD37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1706,7 +1718,7 @@
       </c>
       <c r="D3" s="23" t="str" cm="1">
         <f t="array" ref="D3">IF(LEFT(INDEX(D5:D7,$A$4),1)&lt;&gt;"*",INDEX(D5:D7,$A$4),"")</f>
-        <v/>
+        <v>National</v>
       </c>
       <c r="E3" s="23" t="str" cm="1">
         <f t="array" ref="E3">IF(LEFT(INDEX(E5:E7,$A$4),1)&lt;&gt;"*",INDEX(E5:E7,$A$4),"")</f>
@@ -1826,7 +1838,7 @@
         <v>77</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>78</v>
+        <v>163</v>
       </c>
       <c r="E5" s="23" t="str">
         <f>Regions!A11</f>
@@ -1935,7 +1947,7 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="23" t="str">
         <f>C5</f>
@@ -2052,7 +2064,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="23" t="str">
         <f>"*"&amp;C5</f>
@@ -2060,7 +2072,7 @@
       </c>
       <c r="D7" s="23" t="str">
         <f>D5</f>
-        <v>*National</v>
+        <v>National</v>
       </c>
       <c r="E7" s="23" t="str">
         <f t="shared" ref="E7:AD7" si="1">E5</f>
@@ -2169,223 +2181,223 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="25" t="s">
         <v>81</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="26" t="s">
         <v>83</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="27" t="s">
         <v>85</v>
-      </c>
-      <c r="B12" s="27" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="27" t="s">
         <v>87</v>
-      </c>
-      <c r="B13" s="27" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="27" t="s">
         <v>89</v>
-      </c>
-      <c r="B14" s="27" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="27" t="s">
         <v>91</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="27" t="s">
         <v>93</v>
-      </c>
-      <c r="B16" s="27" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="27" t="s">
         <v>95</v>
-      </c>
-      <c r="B17" s="27" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="27" t="s">
         <v>97</v>
-      </c>
-      <c r="B18" s="27" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="27" t="s">
         <v>99</v>
-      </c>
-      <c r="B19" s="27" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="27" t="s">
         <v>101</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="27" t="s">
         <v>103</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="27" t="s">
         <v>105</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" s="27" t="s">
         <v>107</v>
-      </c>
-      <c r="B23" s="27" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="27" t="s">
         <v>109</v>
-      </c>
-      <c r="B24" s="27" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="27" t="s">
         <v>111</v>
-      </c>
-      <c r="B25" s="27" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="27" t="s">
         <v>113</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="27" t="s">
         <v>115</v>
-      </c>
-      <c r="B27" s="27" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="B28" s="27" t="s">
         <v>117</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="27" t="s">
         <v>119</v>
-      </c>
-      <c r="B29" s="27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="27" t="s">
         <v>121</v>
-      </c>
-      <c r="B30" s="27" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="27" t="s">
         <v>123</v>
-      </c>
-      <c r="B31" s="27" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" s="27" t="s">
         <v>125</v>
-      </c>
-      <c r="B32" s="27" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" s="27" t="s">
         <v>127</v>
-      </c>
-      <c r="B33" s="27" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="B34" s="27" t="s">
         <v>129</v>
-      </c>
-      <c r="B34" s="27" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="27" t="s">
         <v>131</v>
-      </c>
-      <c r="B35" s="27" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="27" t="s">
         <v>133</v>
-      </c>
-      <c r="B36" s="27" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2427,21 +2439,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B92B0C-7472-4C75-A119-CE0EE6C8A8E0}">
   <dimension ref="A2:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="str">
-        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:AD3)</f>
-        <v>~UC_Sets: R_E: IE,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
+        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
+        <v>~UC_Sets: R_E: IE,National</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2533,8 +2547,8 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("",TRUE,"UC-PWR_MaxGrowth",A12)</f>
-        <v>UC-PWR_MaxGrowthCCS</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A12,"MaxGrowth",B12)</f>
+        <v>UC_PWR_MaxGrowth_CCS</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
@@ -2543,7 +2557,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H6" s="2">
         <v>2018</v>
@@ -2551,14 +2565,14 @@
       <c r="I6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="33">
-        <f>1+$B12</f>
+      <c r="J6" s="32">
+        <f>1+$C12</f>
         <v>1.2</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
       </c>
-      <c r="L6" s="34">
+      <c r="L6" s="33">
         <f>-D12</f>
         <v>-0.4</v>
       </c>
@@ -2566,20 +2580,20 @@
         <v>5</v>
       </c>
       <c r="N6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,"PWR",A12, "maximum growth rate")</f>
-        <v>PWR CCS maximum growth rate</v>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A12, "maximum growth rate of",B12)</f>
+        <v>PWR maximum growth rate of CCS</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="str">
-        <f t="shared" ref="B7:B8" si="0">_xlfn.TEXTJOIN("",TRUE,"UC-PWR_MaxGrowth",A13)</f>
-        <v>UC-PWR_MaxGrowthWave</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A13,"MaxGrowth",B13)</f>
+        <v>UC_PWR_MaxGrowth_Wave</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H7">
         <v>2035</v>
@@ -2587,35 +2601,35 @@
       <c r="I7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="33">
-        <f t="shared" ref="J7:J8" si="1">1+$B13</f>
+      <c r="J7" s="32">
+        <f>1+$C13</f>
         <v>1.2</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
       </c>
-      <c r="L7" s="34">
-        <f t="shared" ref="L7:L8" si="2">-D13</f>
+      <c r="L7" s="33">
+        <f t="shared" ref="L7:L8" si="0">-D13</f>
         <v>-0.4</v>
       </c>
       <c r="M7" s="2">
         <v>5</v>
       </c>
       <c r="N7" s="2" t="str">
-        <f t="shared" ref="N7:N8" si="3">_xlfn.TEXTJOIN(" ",TRUE,"PWR",A13, "maximum growth rate")</f>
-        <v>PWR Wave maximum growth rate</v>
+        <f t="shared" ref="N7:N8" si="1">_xlfn.TEXTJOIN(" ",TRUE,A13, "maximum growth rate of",B13)</f>
+        <v>PWR maximum growth rate of Wave</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UC-PWR_MaxGrowthTidal</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
+        <v>UC_PWR_MaxGrowth_Tidal</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H8">
         <v>2035</v>
@@ -2623,38 +2637,41 @@
       <c r="I8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="33">
-        <f t="shared" si="1"/>
+      <c r="J8" s="32">
+        <f>1+$C14</f>
         <v>1.2</v>
       </c>
       <c r="K8" s="2">
         <v>1</v>
       </c>
-      <c r="L8" s="34">
-        <f t="shared" si="2"/>
+      <c r="L8" s="33">
+        <f t="shared" si="0"/>
         <v>-0.1</v>
       </c>
       <c r="M8" s="2">
         <v>5</v>
       </c>
       <c r="N8" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>PWR Tidal maximum growth rate</v>
+        <f t="shared" si="1"/>
+        <v>PWR maximum growth rate of Tidal</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>154</v>
+      <c r="C11" t="s">
+        <v>153</v>
       </c>
       <c r="D11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B12" s="13">
+        <v>165</v>
+      </c>
+      <c r="B12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="13">
         <v>0.2</v>
       </c>
       <c r="D12">
@@ -2663,9 +2680,12 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>162</v>
-      </c>
-      <c r="B13" s="13">
+        <v>165</v>
+      </c>
+      <c r="B13" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" s="13">
         <v>0.2</v>
       </c>
       <c r="D13">
@@ -2674,9 +2694,12 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>163</v>
-      </c>
-      <c r="B14" s="13">
+        <v>165</v>
+      </c>
+      <c r="B14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="13">
         <v>0.2</v>
       </c>
       <c r="D14">
@@ -2692,8 +2715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
   <dimension ref="A2:P52"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2715,7 +2738,7 @@
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:AD3)</f>
-        <v>~UC_Sets: R_E: IE,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
+        <v>~UC_Sets: R_E: IE,National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2888,7 +2911,7 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>13</v>
@@ -2899,7 +2922,7 @@
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H8" s="18">
         <v>2018</v>
@@ -2922,7 +2945,7 @@
         <v>5</v>
       </c>
       <c r="N8" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
@@ -3044,7 +3067,7 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>13</v>
@@ -3055,7 +3078,7 @@
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H12" s="18">
         <v>2018</v>
@@ -3078,7 +3101,7 @@
         <v>5</v>
       </c>
       <c r="N12" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
@@ -3161,7 +3184,7 @@
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>13</v>
@@ -3172,7 +3195,7 @@
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H15" s="18">
         <v>2018</v>
@@ -3195,12 +3218,12 @@
         <v>5</v>
       </c>
       <c r="N15" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>13</v>
@@ -3211,7 +3234,7 @@
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="G16" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H16" s="18">
         <v>2018</v>
@@ -3234,7 +3257,7 @@
         <v>5</v>
       </c>
       <c r="N16" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -3356,7 +3379,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>13</v>
@@ -3367,7 +3390,7 @@
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H20" s="18">
         <v>2018</v>
@@ -3390,12 +3413,12 @@
         <v>5</v>
       </c>
       <c r="N20" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>13</v>
@@ -3406,7 +3429,7 @@
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H21" s="18">
         <v>2018</v>
@@ -3429,7 +3452,7 @@
         <v>5</v>
       </c>
       <c r="N21" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -3530,7 +3553,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="35" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -3548,7 +3571,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="3" t="s">
         <v>25</v>
       </c>
@@ -3564,7 +3587,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="3" t="s">
         <v>24</v>
       </c>
@@ -3580,7 +3603,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="3" t="s">
         <v>23</v>
       </c>
@@ -3596,7 +3619,7 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
+      <c r="A33" s="35"/>
       <c r="B33" s="3" t="s">
         <v>22</v>
       </c>
@@ -3612,7 +3635,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
+      <c r="A34" s="35"/>
       <c r="B34" s="3" t="s">
         <v>21</v>
       </c>
@@ -3698,7 +3721,7 @@
         <v>33</v>
       </c>
       <c r="C45" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -3750,7 +3773,7 @@
         <v>2030</v>
       </c>
       <c r="P47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -4067,13 +4090,257 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5F46D0-BFBE-459D-AD94-C3EBC85EC70F}">
+  <dimension ref="A2:N13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" customWidth="1"/>
+    <col min="14" max="14" width="34.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="str">
+        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
+        <v>~UC_Sets: R_E: IE,National</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A12,"MaxGrowth",B12)</f>
+        <v>UC_SRV-PU_MaxGrowth_HPs</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2018</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="34">
+        <f>1+C12</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+      <c r="L6" s="33">
+        <f>-D12</f>
+        <v>-0.5</v>
+      </c>
+      <c r="M6" s="2">
+        <v>5</v>
+      </c>
+      <c r="N6" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A12, "maximum growth rate of",B12)</f>
+        <v>SRV-PU maximum growth rate of HPs</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A13,"MaxGrowth",B13)</f>
+        <v>UC_SRV-CS_MaxGrowth_HPs</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2018</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="34">
+        <f>1+C13</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="33">
+        <f>-D13</f>
+        <v>-0.5</v>
+      </c>
+      <c r="M7" s="2">
+        <v>5</v>
+      </c>
+      <c r="N7" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A13, "maximum growth rate of",B13)</f>
+        <v>SRV-CS maximum growth rate of HPs</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C12" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D13">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -4284,16 +4551,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4302,7 +4568,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4319,12 +4585,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Swap growth constraints for wave and tidal
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HannahD\Documents\GitHub\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A179693-C30D-43DC-8BD4-BBCD21DEDB8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE785B60-5900-4F9D-A39C-6D6F662DB714}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="4530" yWindow="16050" windowWidth="19650" windowHeight="11070" activeTab="1" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -2439,8 +2439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B92B0C-7472-4C75-A119-CE0EE6C8A8E0}">
   <dimension ref="A2:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2593,7 +2593,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H7">
         <v>2035</v>
@@ -2629,7 +2629,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H8">
         <v>2035</v>
@@ -4094,8 +4094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5F46D0-BFBE-459D-AD94-C3EBC85EC70F}">
   <dimension ref="A2:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4326,21 +4326,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -4551,24 +4536,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4585,4 +4568,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Include H2 PWR max growth in Scen_MaxGrowthRates
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HannahD\Documents\GitHub\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292BDC36-4078-40E9-8F39-9ACFBAB9B77B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1430D98-5773-4D91-BF28-D1567031F5C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="4575" yWindow="16050" windowWidth="19650" windowHeight="11070" activeTab="1" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="191">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -673,12 +673,22 @@
   <si>
     <t>FT*</t>
   </si>
+  <si>
+    <t>UC-PWR_MaxGrowthH2GT</t>
+  </si>
+  <si>
+    <t>P-TH*H2-*</t>
+  </si>
+  <si>
+    <t>PWR H2 Gas turbine maximum growth rate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
@@ -862,7 +872,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="217">
+  <cellStyleXfs count="264">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1080,8 +1090,55 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1127,8 +1184,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="217">
+  <cellStyles count="264">
     <cellStyle name="20% - Accent5 2" xfId="10" xr:uid="{72E8C261-0B7B-4154-8B6F-C9901D88251B}"/>
     <cellStyle name="20% - Accent5 2 2" xfId="25" xr:uid="{11984554-9BCD-4991-A26E-8E4E32B379F3}"/>
     <cellStyle name="20% - Accent5 2 2 2" xfId="80" xr:uid="{4053E826-B16E-4797-8175-121DE6309698}"/>
@@ -1180,49 +1240,96 @@
     <cellStyle name="Comma 2 2" xfId="23" xr:uid="{6FD8625A-7619-4301-8188-1E0AF0841F5E}"/>
     <cellStyle name="Comma 2 2 2" xfId="78" xr:uid="{A71FA496-1E4A-4D5C-95F9-C213403D1372}"/>
     <cellStyle name="Comma 2 2 2 2" xfId="183" xr:uid="{356500B6-3D45-44B3-9B7E-3AAB43000148}"/>
+    <cellStyle name="Comma 2 2 2 2 2" xfId="256" xr:uid="{E21A9A1E-5BDB-45AC-B8EF-33A6FE1A1F6E}"/>
+    <cellStyle name="Comma 2 2 2 3" xfId="232" xr:uid="{25994862-9FAF-40FE-94E8-E465DFF183D5}"/>
     <cellStyle name="Comma 2 2 3" xfId="130" xr:uid="{CB4D2CEB-63D1-4770-9880-AD8E6C8E36DB}"/>
+    <cellStyle name="Comma 2 2 3 2" xfId="244" xr:uid="{E4CBEE47-7757-4B4E-91F2-79CC1DD59CFB}"/>
+    <cellStyle name="Comma 2 2 4" xfId="220" xr:uid="{2B7C6BBC-4333-46B9-AA47-BC580583A7B3}"/>
     <cellStyle name="Comma 2 3" xfId="36" xr:uid="{90DE3579-1977-4C6B-847E-E92F15F9E0F1}"/>
     <cellStyle name="Comma 2 3 2" xfId="91" xr:uid="{3CA1604E-8A06-4062-9104-8340F7183A16}"/>
     <cellStyle name="Comma 2 3 2 2" xfId="196" xr:uid="{A7F5DA55-53CE-4422-BA06-89ABB3409010}"/>
+    <cellStyle name="Comma 2 3 2 2 2" xfId="259" xr:uid="{A96C2CD5-8E01-4B21-8934-F50B072E6EC8}"/>
+    <cellStyle name="Comma 2 3 2 3" xfId="235" xr:uid="{3B7722B8-02F8-41A7-87A7-E426BE2799EF}"/>
     <cellStyle name="Comma 2 3 3" xfId="143" xr:uid="{B8F801FD-5FC7-4F0B-88EC-EA43AE0A79B7}"/>
+    <cellStyle name="Comma 2 3 3 2" xfId="247" xr:uid="{E1341025-4BFA-4E26-9A3A-837ED0143EEC}"/>
+    <cellStyle name="Comma 2 3 4" xfId="223" xr:uid="{8B09463B-1F7D-43BA-B83F-672EE886B8CD}"/>
     <cellStyle name="Comma 2 4" xfId="49" xr:uid="{59FC5B72-FAAC-4300-9DF1-2048D9CFC09A}"/>
     <cellStyle name="Comma 2 4 2" xfId="104" xr:uid="{7F9BEF86-F7C9-47F6-B638-E029087F62EC}"/>
     <cellStyle name="Comma 2 4 2 2" xfId="209" xr:uid="{DC4C781B-3ECA-42B1-94E6-01303C20BCE0}"/>
+    <cellStyle name="Comma 2 4 2 2 2" xfId="262" xr:uid="{CAB82D8B-BCAB-40B6-A062-87F61BA717A2}"/>
+    <cellStyle name="Comma 2 4 2 3" xfId="238" xr:uid="{45C89678-BB79-43F7-A61E-560F0BA503B8}"/>
     <cellStyle name="Comma 2 4 3" xfId="156" xr:uid="{928DA526-D1B2-4D7C-A0C2-989B566BF2CF}"/>
+    <cellStyle name="Comma 2 4 3 2" xfId="250" xr:uid="{DB04CA2D-4B70-40EB-88C8-30BFFBC59B5C}"/>
+    <cellStyle name="Comma 2 4 4" xfId="226" xr:uid="{1ACB5DA1-6958-49CB-9B83-AFA8D5A4EF43}"/>
     <cellStyle name="Comma 2 5" xfId="64" xr:uid="{18203036-49E3-4111-A041-C15EF8392F11}"/>
     <cellStyle name="Comma 2 5 2" xfId="170" xr:uid="{69F7F36D-3C18-4C61-8F9E-13F178F3D6A0}"/>
+    <cellStyle name="Comma 2 5 2 2" xfId="253" xr:uid="{74F25553-17D5-48B7-A200-A29EAE9A8EBA}"/>
+    <cellStyle name="Comma 2 5 3" xfId="229" xr:uid="{18236CB7-8F48-4937-B8EB-575D735EF5F1}"/>
     <cellStyle name="Comma 2 6" xfId="117" xr:uid="{38D21344-41A3-4171-A298-3C4D16D5781D}"/>
+    <cellStyle name="Comma 2 6 2" xfId="241" xr:uid="{F8BC8039-F121-4F10-BE7F-B8895A058790}"/>
+    <cellStyle name="Comma 2 7" xfId="217" xr:uid="{D4547780-9645-45C1-B7DD-86548E32B7F4}"/>
     <cellStyle name="Comma 3" xfId="12" xr:uid="{B4F90DA6-3CEF-4B5E-8E10-A29DAAC7E6E1}"/>
     <cellStyle name="Comma 3 2" xfId="27" xr:uid="{22BBC824-B041-4306-BF3D-112FE089A6E4}"/>
     <cellStyle name="Comma 3 2 2" xfId="82" xr:uid="{3B2B509C-A915-437B-8267-A638DE5102EC}"/>
     <cellStyle name="Comma 3 2 2 2" xfId="187" xr:uid="{57955E9D-94F0-49A6-9F3F-5B3A06C4A25F}"/>
+    <cellStyle name="Comma 3 2 2 2 2" xfId="257" xr:uid="{E9D5217D-296E-4A8B-8987-6DC11C7D2653}"/>
+    <cellStyle name="Comma 3 2 2 3" xfId="233" xr:uid="{5B47EE65-88F0-4357-99B3-A59DD595C668}"/>
     <cellStyle name="Comma 3 2 3" xfId="134" xr:uid="{B597C21C-04D6-4E66-99E2-E7521C0BF552}"/>
+    <cellStyle name="Comma 3 2 3 2" xfId="245" xr:uid="{0E88E68C-584A-4D73-ABCC-52A7B9AD4C98}"/>
+    <cellStyle name="Comma 3 2 4" xfId="221" xr:uid="{4FAD0494-700A-4600-ADBE-258F1F25A79A}"/>
     <cellStyle name="Comma 3 3" xfId="40" xr:uid="{BD92A8CD-1B04-42B0-A5EE-AD5991DE5F2B}"/>
     <cellStyle name="Comma 3 3 2" xfId="95" xr:uid="{5B05ABBD-7F05-4B95-8433-D04FC429FFF6}"/>
     <cellStyle name="Comma 3 3 2 2" xfId="200" xr:uid="{1181A999-A111-41F5-A8B6-A0A329A6282A}"/>
+    <cellStyle name="Comma 3 3 2 2 2" xfId="260" xr:uid="{E480DA3A-708A-496A-BC81-E7D118899B0E}"/>
+    <cellStyle name="Comma 3 3 2 3" xfId="236" xr:uid="{471EB2E0-26E0-4DDB-9746-FCC08824EDFF}"/>
     <cellStyle name="Comma 3 3 3" xfId="147" xr:uid="{431A9580-1EFC-4ADD-975F-AF3215B5DB60}"/>
+    <cellStyle name="Comma 3 3 3 2" xfId="248" xr:uid="{53CC4246-E3D8-42FA-BA88-8D818BC24BDE}"/>
+    <cellStyle name="Comma 3 3 4" xfId="224" xr:uid="{FA3C3B94-AFDF-443F-8DA5-38DA5C6A427A}"/>
     <cellStyle name="Comma 3 4" xfId="53" xr:uid="{74EF9D46-89F5-4B02-BA6A-F228F73BCD51}"/>
     <cellStyle name="Comma 3 4 2" xfId="108" xr:uid="{6E59CA5A-5039-4947-9E29-BC415D8C6D0E}"/>
     <cellStyle name="Comma 3 4 2 2" xfId="213" xr:uid="{AC91527F-1468-44EF-99F2-A6476A77388E}"/>
+    <cellStyle name="Comma 3 4 2 2 2" xfId="263" xr:uid="{D4343070-0E2C-4363-AF9D-857E2F009D77}"/>
+    <cellStyle name="Comma 3 4 2 3" xfId="239" xr:uid="{8602B698-5F48-44B6-A65B-DE5FB67CE3DA}"/>
     <cellStyle name="Comma 3 4 3" xfId="160" xr:uid="{64ADE26D-B709-46AB-B1ED-D98440A98F28}"/>
+    <cellStyle name="Comma 3 4 3 2" xfId="251" xr:uid="{3F893459-A25C-4744-92AC-C3771F7CE88F}"/>
+    <cellStyle name="Comma 3 4 4" xfId="227" xr:uid="{D9A88900-2D59-4F82-968A-B31755DFEF4F}"/>
     <cellStyle name="Comma 3 5" xfId="68" xr:uid="{A984BC4E-032F-4E6C-8A39-C87842CFF2C7}"/>
     <cellStyle name="Comma 3 5 2" xfId="174" xr:uid="{7839EEA7-157F-4562-A4BB-29503D37EA90}"/>
+    <cellStyle name="Comma 3 5 2 2" xfId="254" xr:uid="{7E546453-CA11-4CFD-8E9A-0ACC7F262C58}"/>
+    <cellStyle name="Comma 3 5 3" xfId="230" xr:uid="{79CACC4C-835D-4A6F-AF5D-0BDDADAD36FF}"/>
     <cellStyle name="Comma 3 6" xfId="121" xr:uid="{5E507840-1D65-4E87-8D7F-4DEAC0461FD0}"/>
+    <cellStyle name="Comma 3 6 2" xfId="242" xr:uid="{BC3E7AAA-142F-4F6C-A15D-D43413687800}"/>
+    <cellStyle name="Comma 3 7" xfId="218" xr:uid="{64275CC4-A9B1-4FBD-AC13-A313740B785D}"/>
     <cellStyle name="Comma 4" xfId="16" xr:uid="{CD4C481F-9382-4616-8DC5-80BECD555C1F}"/>
     <cellStyle name="Comma 4 2" xfId="72" xr:uid="{1E03F2A1-21D4-49FC-B60C-E51F6DD1E52E}"/>
     <cellStyle name="Comma 4 2 2" xfId="178" xr:uid="{5EE973C0-E52B-4051-8B2B-A870AF88C918}"/>
+    <cellStyle name="Comma 4 2 2 2" xfId="255" xr:uid="{4B8F96A7-F793-418D-AB0E-E8EA459CA1DB}"/>
+    <cellStyle name="Comma 4 2 3" xfId="231" xr:uid="{596BE320-84F8-4ABD-8D95-FD3C0FD2FE71}"/>
     <cellStyle name="Comma 4 3" xfId="125" xr:uid="{BA46819D-2274-4B63-9822-8B2920FDE4A6}"/>
+    <cellStyle name="Comma 4 3 2" xfId="243" xr:uid="{B071A1A9-D818-4806-9902-0D0A00922682}"/>
+    <cellStyle name="Comma 4 4" xfId="219" xr:uid="{7F4248B7-57E5-4AF8-A95F-79CE75478A01}"/>
     <cellStyle name="Comma 5" xfId="31" xr:uid="{8948A309-0A0B-4EDB-897E-DC68ADC888E5}"/>
     <cellStyle name="Comma 5 2" xfId="86" xr:uid="{5F4FD49D-B720-479C-9506-386B5E33CC68}"/>
     <cellStyle name="Comma 5 2 2" xfId="191" xr:uid="{9555B528-480C-43E9-848D-C76431DBFCDC}"/>
+    <cellStyle name="Comma 5 2 2 2" xfId="258" xr:uid="{EC6A7C29-D73E-4C58-94C2-201EA434AA99}"/>
+    <cellStyle name="Comma 5 2 3" xfId="234" xr:uid="{27398D0E-6044-438C-90F4-A2EA8E428F96}"/>
     <cellStyle name="Comma 5 3" xfId="138" xr:uid="{F3A3DFF2-0391-488D-B790-383EFEFC2E88}"/>
+    <cellStyle name="Comma 5 3 2" xfId="246" xr:uid="{5DAA8A63-6F32-44E7-8435-3C9B68AEEC92}"/>
+    <cellStyle name="Comma 5 4" xfId="222" xr:uid="{C73D6361-4CB8-4194-8873-DBB6B27617BA}"/>
     <cellStyle name="Comma 6" xfId="44" xr:uid="{D215E70F-4FC9-4641-915E-57F29291582D}"/>
     <cellStyle name="Comma 6 2" xfId="99" xr:uid="{A33A6D59-2FDE-4498-B148-2742AAA886D8}"/>
     <cellStyle name="Comma 6 2 2" xfId="204" xr:uid="{8CB077BA-9B0C-4E28-B8F2-3F8DA5F6644F}"/>
+    <cellStyle name="Comma 6 2 2 2" xfId="261" xr:uid="{DBB084FA-A286-42A1-991A-7F0A5A8654FA}"/>
+    <cellStyle name="Comma 6 2 3" xfId="237" xr:uid="{03E5344F-DEC6-490A-BE2D-F2F1C107C234}"/>
     <cellStyle name="Comma 6 3" xfId="151" xr:uid="{5FE6D830-212B-46FA-9213-E06AE57FD613}"/>
+    <cellStyle name="Comma 6 3 2" xfId="249" xr:uid="{6A865773-C429-49A9-B39E-5E61553C7126}"/>
+    <cellStyle name="Comma 6 4" xfId="225" xr:uid="{48DCD399-A00A-4001-9B03-4A5D841EC0AE}"/>
     <cellStyle name="Comma 7" xfId="57" xr:uid="{B07F94D8-52D2-4210-96DC-5BE939614702}"/>
     <cellStyle name="Comma 7 2" xfId="165" xr:uid="{59CC3575-535F-4640-8AA9-6860CE88644D}"/>
+    <cellStyle name="Comma 7 2 2" xfId="252" xr:uid="{41169135-0D22-446B-BB01-DBE36489F6AA}"/>
+    <cellStyle name="Comma 7 3" xfId="228" xr:uid="{490F63AF-9113-4969-8993-34FA22F7624F}"/>
     <cellStyle name="Comma 8" xfId="113" xr:uid="{D3049B2C-D006-4A03-BB47-B9A6F9D46786}"/>
+    <cellStyle name="Comma 8 2" xfId="240" xr:uid="{A2775F03-1691-4769-BF1C-8A3FD1025287}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="56" xr:uid="{8FD9948C-E924-46F1-8C3F-BE68079CF0FB}"/>
     <cellStyle name="Normal 10 2" xfId="164" xr:uid="{6EC5393C-9EE8-492E-83F0-05CD88BCF795}"/>
@@ -2490,8 +2597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B92B0C-7472-4C75-A119-CE0EE6C8A8E0}">
   <dimension ref="A2:N14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2705,6 +2812,42 @@
       <c r="N8" s="2" t="str">
         <f t="shared" si="1"/>
         <v>PWR maximum growth rate of Tidal</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="36" t="s">
+        <v>188</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="H9" s="36">
+        <v>2020</v>
+      </c>
+      <c r="I9" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="38">
+        <v>1.2</v>
+      </c>
+      <c r="K9" s="36">
+        <v>1</v>
+      </c>
+      <c r="L9" s="37">
+        <f>L6</f>
+        <v>-0.4</v>
+      </c>
+      <c r="M9" s="36">
+        <v>5</v>
+      </c>
+      <c r="N9" s="36" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -4285,8 +4428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5F46D0-BFBE-459D-AD94-C3EBC85EC70F}">
   <dimension ref="A2:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4625,21 +4768,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -4850,24 +4978,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4884,4 +5010,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
SRV: Use ACT instead of CAP for growth constraints for biomass and biogas
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HannahD\Documents\GitHub\Irish-TIMES-model\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1430D98-5773-4D91-BF28-D1567031F5C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF063FDE-65FF-4A7C-9AAC-954508DFE292}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="16050" windowWidth="19650" windowHeight="11070" activeTab="1" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="194">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -681,6 +681,15 @@
   </si>
   <si>
     <t>PWR H2 Gas turbine maximum growth rate</t>
+  </si>
+  <si>
+    <t>ACT, GROWTH</t>
+  </si>
+  <si>
+    <t>UC_ACT</t>
+  </si>
+  <si>
+    <t>UC_ACT~RHS</t>
   </si>
 </sst>
 </file>
@@ -1181,12 +1190,12 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="264">
     <cellStyle name="20% - Accent5 2" xfId="10" xr:uid="{72E8C261-0B7B-4154-8B6F-C9901D88251B}"/>
@@ -2597,7 +2606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B92B0C-7472-4C75-A119-CE0EE6C8A8E0}">
   <dimension ref="A2:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -2815,38 +2824,38 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="35" t="s">
         <v>188</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36" t="s">
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35" t="s">
         <v>189</v>
       </c>
-      <c r="H9" s="36">
+      <c r="H9" s="35">
         <v>2020</v>
       </c>
-      <c r="I9" s="36" t="s">
+      <c r="I9" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="38">
+      <c r="J9" s="37">
         <v>1.2</v>
       </c>
-      <c r="K9" s="36">
+      <c r="K9" s="35">
         <v>1</v>
       </c>
-      <c r="L9" s="37">
+      <c r="L9" s="36">
         <f>L6</f>
         <v>-0.4</v>
       </c>
-      <c r="M9" s="36">
+      <c r="M9" s="35">
         <v>5</v>
       </c>
-      <c r="N9" s="36" t="s">
+      <c r="N9" s="35" t="s">
         <v>190</v>
       </c>
     </row>
@@ -3775,7 +3784,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="38" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -3799,7 +3808,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
+      <c r="A31" s="38"/>
       <c r="B31" s="3" t="s">
         <v>25</v>
       </c>
@@ -3824,7 +3833,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="35"/>
+      <c r="A32" s="38"/>
       <c r="B32" s="3" t="s">
         <v>24</v>
       </c>
@@ -3846,7 +3855,7 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
+      <c r="A33" s="38"/>
       <c r="B33" s="3" t="s">
         <v>23</v>
       </c>
@@ -3868,7 +3877,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
+      <c r="A34" s="38"/>
       <c r="B34" s="3" t="s">
         <v>22</v>
       </c>
@@ -3890,7 +3899,7 @@
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="35"/>
+      <c r="A35" s="38"/>
       <c r="B35" s="3" t="s">
         <v>21</v>
       </c>
@@ -4426,10 +4435,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5F46D0-BFBE-459D-AD94-C3EBC85EC70F}">
-  <dimension ref="A2:N15"/>
+  <dimension ref="A2:N18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4538,7 +4547,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A12,"MaxGrowth",B12)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A15,"MaxGrowth",B15)</f>
         <v>UC_SRV-PU_MaxGrowth_HPs</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -4559,27 +4568,27 @@
         <v>15</v>
       </c>
       <c r="J6" s="34">
-        <f>1+C12</f>
+        <f>1+C15</f>
         <v>1.05</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
       </c>
       <c r="L6" s="33">
-        <f>-D12</f>
+        <f>-D15</f>
         <v>-0.3</v>
       </c>
       <c r="M6" s="2">
         <v>5</v>
       </c>
       <c r="N6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A12, "maximum growth rate of",B12)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A15, "maximum growth rate of",B15)</f>
         <v>SRV-PU maximum growth rate of HPs</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A13,"MaxGrowth",B13)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A16,"MaxGrowth",B16)</f>
         <v>UC_SRV-CS_MaxGrowth_HPs</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -4600,165 +4609,238 @@
         <v>15</v>
       </c>
       <c r="J7" s="34">
-        <f>1+C13</f>
+        <f>1+C16</f>
         <v>1.05</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
       </c>
       <c r="L7" s="33">
-        <f>-D13</f>
+        <f>-D16</f>
         <v>-0.3</v>
       </c>
       <c r="M7" s="2">
         <v>5</v>
       </c>
       <c r="N7" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A13, "maximum growth rate of",B13)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A16, "maximum growth rate of",B16)</f>
         <v>SRV-CS maximum growth rate of HPs</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A17,"MaxGrowth",B17)</f>
         <v>UC_SRV_MaxGrowth_Biomass</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="F8" s="2" t="s">
+      <c r="C11" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="F11" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H11" s="2">
         <v>2018</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="34">
-        <f>1+C14</f>
+      <c r="J11" s="34">
+        <f>1+C17</f>
         <v>1.05</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K11" s="2">
         <v>1</v>
       </c>
-      <c r="L8" s="33">
-        <f>-D14</f>
+      <c r="L11" s="33">
+        <f>-D17</f>
         <v>-0.1</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M11" s="2">
         <v>5</v>
       </c>
-      <c r="N8" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A14, "maximum growth rate of",B14)</f>
+      <c r="N11" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A17, "maximum growth rate of",B17)</f>
         <v>SRV maximum growth rate of Biomass</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A15,"MaxGrowth",B15)</f>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
         <v>UC_SRV_MaxGrowth_Biogas</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="F9" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="F12" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H12" s="2">
         <v>2018</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="34">
-        <f>1+C15</f>
+      <c r="J12" s="34">
+        <f>1+C18</f>
         <v>1.05</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K12" s="2">
         <v>1</v>
       </c>
-      <c r="L9" s="33">
-        <f>-D15</f>
+      <c r="L12" s="33">
+        <f>-D18</f>
         <v>-0.1</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M12" s="2">
         <v>5</v>
       </c>
-      <c r="N9" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A15, "maximum growth rate of",B15)</f>
+      <c r="N12" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A18, "maximum growth rate of",B18)</f>
         <v>SRV maximum growth rate of Biogas</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>153</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D14" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>166</v>
-      </c>
-      <c r="B12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C12" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="D12">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>167</v>
-      </c>
-      <c r="B13" t="s">
-        <v>164</v>
-      </c>
-      <c r="C13" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="D13">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>184</v>
-      </c>
-      <c r="B14" t="s">
-        <v>182</v>
-      </c>
-      <c r="C14" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="D14">
-        <v>0.1</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="B15" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="C15" s="13">
         <v>0.05</v>
       </c>
       <c r="D15">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C16" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="D16">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="D17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>184</v>
+      </c>
+      <c r="B18" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="D18">
         <v>0.1</v>
       </c>
     </row>
@@ -4768,6 +4850,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -4978,12 +5066,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4994,6 +5076,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5012,15 +5103,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
SRV: use the same seed value for biomass, biogas and HPs
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF063FDE-65FF-4A7C-9AAC-954508DFE292}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393EC184-907A-4881-972A-027EF8CC88DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -4438,7 +4438,7 @@
   <dimension ref="A2:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4730,7 +4730,7 @@
       </c>
       <c r="L11" s="33">
         <f>-D17</f>
-        <v>-0.1</v>
+        <v>-0.3</v>
       </c>
       <c r="M11" s="2">
         <v>5</v>
@@ -4770,7 +4770,7 @@
       </c>
       <c r="L12" s="33">
         <f>-D18</f>
-        <v>-0.1</v>
+        <v>-0.3</v>
       </c>
       <c r="M12" s="2">
         <v>5</v>
@@ -4827,7 +4827,7 @@
         <v>0.05</v>
       </c>
       <c r="D17">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4841,7 +4841,7 @@
         <v>0.05</v>
       </c>
       <c r="D18">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>
@@ -4850,12 +4850,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -5066,6 +5060,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5076,15 +5076,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5103,6 +5094,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Disable maximum growth rate for BEVs
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393EC184-907A-4881-972A-027EF8CC88DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB2D5AF-0627-4C6D-B5E7-F6A47FBF6647}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="162">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -225,97 +225,25 @@
     <t>T-CAR-PHEV*</t>
   </si>
   <si>
-    <t>HGT-Maximum growth rate of HEVs</t>
-  </si>
-  <si>
-    <t>HGT-Maximum growth rate of BEVs</t>
-  </si>
-  <si>
-    <t>UC-HGT_MaxGrowthBEV</t>
-  </si>
-  <si>
-    <t>UC-HGT_MaxGrowthHEV</t>
-  </si>
-  <si>
     <t>T-HGT-HEV*</t>
   </si>
   <si>
     <t>T-MGT-HEV*</t>
   </si>
   <si>
-    <t>UC-MGT-MaxGrowthBEV</t>
-  </si>
-  <si>
-    <t>UC-MGT-MaxGrowthHEV</t>
-  </si>
-  <si>
-    <t>MGT-Maximum growth rate of BEVs</t>
-  </si>
-  <si>
-    <t>MGT-Maximum growth rate of HEVs</t>
-  </si>
-  <si>
-    <t>UC-LGT_MaxGrowthBEV</t>
-  </si>
-  <si>
-    <t>LGT-Maximum growth rate of BEVs</t>
-  </si>
-  <si>
-    <t>UC-CAR_MaxGrowthBEV</t>
-  </si>
-  <si>
-    <t>UC-CAR_MaxGrowthPHEV</t>
-  </si>
-  <si>
-    <t>Cars-Maximum growth rate of BEVs</t>
-  </si>
-  <si>
-    <t>Cars-Maximum growth rate of PHEVs</t>
-  </si>
-  <si>
-    <t>UC-HGT_MaxGrowthFCV</t>
-  </si>
-  <si>
     <t>T-HGT-FCV*</t>
   </si>
   <si>
-    <t>HGT-Maximum growth rate of FCVs</t>
-  </si>
-  <si>
-    <t>MGT-Maximum growth rate of FCVs</t>
-  </si>
-  <si>
     <t>T-MGT-FCV*</t>
   </si>
   <si>
-    <t>UC-MGT-MaxGrowthFCV</t>
-  </si>
-  <si>
     <t>T-CAR-FCV*</t>
   </si>
   <si>
-    <t>UC-CAR_MaxGrowthFCV</t>
-  </si>
-  <si>
-    <t>Cars-Maximum growth rate of FCVs</t>
-  </si>
-  <si>
-    <t>LGT-Maximum growth rate of PHEVs</t>
-  </si>
-  <si>
-    <t>LGT-Maximum growth rate of FCVs</t>
-  </si>
-  <si>
     <t>T-LGT-PHEV*</t>
   </si>
   <si>
     <t>T-LGT-FCV*</t>
-  </si>
-  <si>
-    <t>UC-LGT_MaxGrowthPHEV</t>
-  </si>
-  <si>
-    <t>UC-LGT_MaxGrowthFCV</t>
   </si>
   <si>
     <t>Development</t>
@@ -515,60 +443,24 @@
     </r>
   </si>
   <si>
-    <t>UC-HGT_MaxGrowthNGICE</t>
-  </si>
-  <si>
-    <t>UC-MGT-MaxGrowthNGICE</t>
-  </si>
-  <si>
     <t>T-MGT-ICE_NG*</t>
   </si>
   <si>
-    <t>MGT-Maximum growth rate of NG-ICEs</t>
-  </si>
-  <si>
-    <t>HGT-Maximum growth rate of NG-ICEs</t>
-  </si>
-  <si>
-    <t>UC-HGT_MaxGrowthLNGICE</t>
-  </si>
-  <si>
-    <t>HGT-Maximum growth rate of LNG-ICEs</t>
-  </si>
-  <si>
-    <t>UC-MGT-MaxGrowthLNGICE</t>
-  </si>
-  <si>
     <t>T-MGT-ICE_LNG*</t>
   </si>
   <si>
-    <t>MGT-Maximum growth rate of LNG-ICEs</t>
-  </si>
-  <si>
     <t>T-HGT-ICE_NG*</t>
   </si>
   <si>
     <t>T-HGT-ICE_LNG*</t>
   </si>
   <si>
-    <t>UC-CAR_MaxGrowthNGICE</t>
-  </si>
-  <si>
     <t>T-CAR-ICE_NG*</t>
   </si>
   <si>
-    <t>Cars-Maximum growth rate of NG-ICEs</t>
-  </si>
-  <si>
-    <t>UC-LGT_MaxGrowthNGICE</t>
-  </si>
-  <si>
     <t>T-LGT-ICE_NG*</t>
   </si>
   <si>
-    <t>LGT-Maximum growth rate of NG-ICEs</t>
-  </si>
-  <si>
     <t>Max growth rate</t>
   </si>
   <si>
@@ -623,18 +515,12 @@
     <t>S-SH*CS*</t>
   </si>
   <si>
-    <t>Cars</t>
-  </si>
-  <si>
     <t>BEV</t>
   </si>
   <si>
     <t>PHEV</t>
   </si>
   <si>
-    <t>NG-ICEs</t>
-  </si>
-  <si>
     <t>FCV</t>
   </si>
   <si>
@@ -650,9 +536,6 @@
     <t>HGT</t>
   </si>
   <si>
-    <t>LNG-ICEs</t>
-  </si>
-  <si>
     <t>Playground</t>
   </si>
   <si>
@@ -690,6 +573,27 @@
   </si>
   <si>
     <t>UC_ACT~RHS</t>
+  </si>
+  <si>
+    <t>CAR</t>
+  </si>
+  <si>
+    <t>NG-ICE</t>
+  </si>
+  <si>
+    <t>LNG-ICE</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>On/Off</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -1999,13 +1903,13 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>163</v>
+        <v>127</v>
       </c>
       <c r="E5" s="23" t="str">
         <f>Regions!A11</f>
@@ -2114,7 +2018,7 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="C6" s="23" t="str">
         <f>C5</f>
@@ -2231,7 +2135,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="C7" s="23" t="str">
         <f>"*"&amp;C5</f>
@@ -2348,223 +2252,223 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2724,7 +2628,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="H6" s="2">
         <v>2018</v>
@@ -2760,7 +2664,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="H7">
         <v>2035</v>
@@ -2796,7 +2700,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>158</v>
+        <v>122</v>
       </c>
       <c r="H8">
         <v>2035</v>
@@ -2825,7 +2729,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="35" t="s">
-        <v>188</v>
+        <v>149</v>
       </c>
       <c r="C9" s="35" t="s">
         <v>13</v>
@@ -2834,7 +2738,7 @@
       <c r="E9" s="35"/>
       <c r="F9" s="35"/>
       <c r="G9" s="35" t="s">
-        <v>189</v>
+        <v>150</v>
       </c>
       <c r="H9" s="35">
         <v>2020</v>
@@ -2856,23 +2760,23 @@
         <v>5</v>
       </c>
       <c r="N9" s="35" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="D11" t="s">
-        <v>155</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="B12" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
       <c r="C12" s="13">
         <v>0.2</v>
@@ -2883,10 +2787,10 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s">
-        <v>161</v>
+        <v>125</v>
       </c>
       <c r="C13" s="13">
         <v>0.2</v>
@@ -2897,10 +2801,10 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s">
-        <v>162</v>
+        <v>126</v>
       </c>
       <c r="C14" s="13">
         <v>0.2</v>
@@ -2918,8 +2822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
   <dimension ref="A2:P53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3035,8 +2939,9 @@
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
-        <v>57</v>
+      <c r="B6" s="18" t="str">
+        <f t="shared" ref="B6:B23" si="0">IF(H27="*","*",_xlfn.TEXTJOIN("",TRUE,"UC-",I27,"_MaxGrowth",J27))</f>
+        <v>*</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>13</v>
@@ -3056,7 +2961,7 @@
         <v>15</v>
       </c>
       <c r="J6" s="29">
-        <f t="shared" ref="J6:J23" si="0">1+$K27</f>
+        <f t="shared" ref="J6:J23" si="1">1+$K27</f>
         <v>1.8</v>
       </c>
       <c r="K6" s="18">
@@ -3069,13 +2974,15 @@
       <c r="M6" s="18">
         <v>5</v>
       </c>
-      <c r="N6" s="18" t="s">
-        <v>59</v>
+      <c r="N6" s="18" t="str">
+        <f t="shared" ref="N6:N23" si="2">_xlfn.TEXTJOIN(" ", TRUE,I27&amp;"s","maximum growth rate of",J27&amp;"s")</f>
+        <v>CARs maximum growth rate of BEVs</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
-        <v>58</v>
+      <c r="B7" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-CAR_MaxGrowthPHEV</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>13</v>
@@ -3095,7 +3002,7 @@
         <v>15</v>
       </c>
       <c r="J7" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8</v>
       </c>
       <c r="K7" s="18">
@@ -3108,13 +3015,15 @@
       <c r="M7" s="18">
         <v>5</v>
       </c>
-      <c r="N7" s="18" t="s">
-        <v>60</v>
+      <c r="N7" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>CARs maximum growth rate of PHEVs</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="18" t="s">
-        <v>147</v>
+      <c r="B8" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-CAR_MaxGrowthNG-ICE</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>13</v>
@@ -3125,7 +3034,7 @@
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="18" t="s">
-        <v>148</v>
+        <v>115</v>
       </c>
       <c r="H8" s="18">
         <v>2018</v>
@@ -3134,7 +3043,7 @@
         <v>15</v>
       </c>
       <c r="J8" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K8" s="18">
@@ -3147,13 +3056,15 @@
       <c r="M8" s="18">
         <v>5</v>
       </c>
-      <c r="N8" s="18" t="s">
-        <v>149</v>
+      <c r="N8" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>CARs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
-        <v>68</v>
+      <c r="B9" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-CAR_MaxGrowthFCV</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>13</v>
@@ -3164,7 +3075,7 @@
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="H9" s="21">
         <v>2018</v>
@@ -3173,7 +3084,7 @@
         <v>15</v>
       </c>
       <c r="J9" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K9" s="21">
@@ -3186,13 +3097,15 @@
       <c r="M9" s="21">
         <v>5</v>
       </c>
-      <c r="N9" s="21" t="s">
-        <v>69</v>
+      <c r="N9" s="21" t="str">
+        <f t="shared" si="2"/>
+        <v>CARs maximum growth rate of FCVs</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
-        <v>55</v>
+      <c r="B10" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-LGT_MaxGrowthBEV</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>13</v>
@@ -3212,7 +3125,7 @@
         <v>15</v>
       </c>
       <c r="J10" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K10" s="18">
@@ -3225,13 +3138,15 @@
       <c r="M10" s="18">
         <v>5</v>
       </c>
-      <c r="N10" s="18" t="s">
-        <v>56</v>
+      <c r="N10" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>LGTs maximum growth rate of BEVs</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
-        <v>74</v>
+      <c r="B11" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-LGT_MaxGrowthPHEV</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>13</v>
@@ -3242,7 +3157,7 @@
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="H11" s="18">
         <v>2018</v>
@@ -3251,7 +3166,7 @@
         <v>15</v>
       </c>
       <c r="J11" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K11" s="18">
@@ -3264,13 +3179,15 @@
       <c r="M11" s="18">
         <v>5</v>
       </c>
-      <c r="N11" s="18" t="s">
-        <v>70</v>
+      <c r="N11" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>LGTs maximum growth rate of PHEVs</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="18" t="s">
-        <v>150</v>
+      <c r="B12" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-LGT_MaxGrowthNG-ICE</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>13</v>
@@ -3281,7 +3198,7 @@
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="H12" s="18">
         <v>2018</v>
@@ -3290,7 +3207,7 @@
         <v>15</v>
       </c>
       <c r="J12" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K12" s="18">
@@ -3303,13 +3220,15 @@
       <c r="M12" s="18">
         <v>5</v>
       </c>
-      <c r="N12" s="18" t="s">
-        <v>152</v>
+      <c r="N12" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>LGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
-        <v>75</v>
+      <c r="B13" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-LGT_MaxGrowthFCV</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>13</v>
@@ -3320,7 +3239,7 @@
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
       <c r="G13" s="21" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="H13" s="21">
         <v>2018</v>
@@ -3329,7 +3248,7 @@
         <v>15</v>
       </c>
       <c r="J13" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K13" s="21">
@@ -3342,13 +3261,15 @@
       <c r="M13" s="21">
         <v>5</v>
       </c>
-      <c r="N13" s="21" t="s">
-        <v>71</v>
+      <c r="N13" s="21" t="str">
+        <f t="shared" si="2"/>
+        <v>LGTs maximum growth rate of FCVs</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="18" t="s">
-        <v>51</v>
+      <c r="B14" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-MGT_MaxGrowthBEV</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>13</v>
@@ -3368,7 +3289,7 @@
         <v>15</v>
       </c>
       <c r="J14" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K14" s="18">
@@ -3381,13 +3302,15 @@
       <c r="M14" s="18">
         <v>5</v>
       </c>
-      <c r="N14" s="18" t="s">
-        <v>53</v>
+      <c r="N14" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>MGTs maximum growth rate of BEVs</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="18" t="s">
-        <v>136</v>
+      <c r="B15" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-MGT_MaxGrowthNG-ICE</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>13</v>
@@ -3398,7 +3321,7 @@
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="18" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="H15" s="18">
         <v>2018</v>
@@ -3407,7 +3330,7 @@
         <v>15</v>
       </c>
       <c r="J15" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K15" s="18">
@@ -3420,13 +3343,15 @@
       <c r="M15" s="18">
         <v>5</v>
       </c>
-      <c r="N15" s="18" t="s">
-        <v>138</v>
+      <c r="N15" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>MGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
-        <v>142</v>
+      <c r="B16" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-MGT_MaxGrowthLNG-ICE</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>13</v>
@@ -3437,7 +3362,7 @@
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="G16" s="18" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="H16" s="18">
         <v>2018</v>
@@ -3446,7 +3371,7 @@
         <v>15</v>
       </c>
       <c r="J16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K16" s="18">
@@ -3459,13 +3384,15 @@
       <c r="M16" s="18">
         <v>5</v>
       </c>
-      <c r="N16" s="18" t="s">
-        <v>144</v>
+      <c r="N16" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>MGTs maximum growth rate of LNG-ICEs</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="s">
-        <v>52</v>
+      <c r="B17" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-MGT_MaxGrowthHEV</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>13</v>
@@ -3476,7 +3403,7 @@
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
       <c r="G17" s="18" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H17" s="18">
         <v>2018</v>
@@ -3485,7 +3412,7 @@
         <v>15</v>
       </c>
       <c r="J17" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K17" s="18">
@@ -3498,13 +3425,15 @@
       <c r="M17" s="18">
         <v>5</v>
       </c>
-      <c r="N17" s="18" t="s">
-        <v>54</v>
+      <c r="N17" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>MGTs maximum growth rate of HEVs</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="21" t="s">
-        <v>66</v>
+      <c r="B18" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-MGT_MaxGrowthFCV</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>13</v>
@@ -3515,7 +3444,7 @@
       <c r="E18" s="21"/>
       <c r="F18" s="21"/>
       <c r="G18" s="21" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="H18" s="21">
         <v>2018</v>
@@ -3524,7 +3453,7 @@
         <v>15</v>
       </c>
       <c r="J18" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K18" s="21">
@@ -3537,13 +3466,15 @@
       <c r="M18" s="21">
         <v>5</v>
       </c>
-      <c r="N18" s="21" t="s">
-        <v>64</v>
+      <c r="N18" s="21" t="str">
+        <f t="shared" si="2"/>
+        <v>MGTs maximum growth rate of FCVs</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="18" t="s">
-        <v>47</v>
+      <c r="B19" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-HGT_MaxGrowthBEV</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>13</v>
@@ -3563,7 +3494,7 @@
         <v>15</v>
       </c>
       <c r="J19" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K19" s="18">
@@ -3576,13 +3507,15 @@
       <c r="M19" s="18">
         <v>5</v>
       </c>
-      <c r="N19" s="18" t="s">
-        <v>46</v>
+      <c r="N19" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>HGTs maximum growth rate of BEVs</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="18" t="s">
-        <v>135</v>
+      <c r="B20" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-HGT_MaxGrowthNG-ICE</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>13</v>
@@ -3593,7 +3526,7 @@
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="18" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="H20" s="18">
         <v>2018</v>
@@ -3602,7 +3535,7 @@
         <v>15</v>
       </c>
       <c r="J20" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K20" s="18">
@@ -3615,13 +3548,15 @@
       <c r="M20" s="18">
         <v>5</v>
       </c>
-      <c r="N20" s="18" t="s">
-        <v>139</v>
+      <c r="N20" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>HGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="18" t="s">
-        <v>140</v>
+      <c r="B21" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-HGT_MaxGrowthLNG-ICE</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>13</v>
@@ -3632,7 +3567,7 @@
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="18" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="H21" s="18">
         <v>2018</v>
@@ -3641,7 +3576,7 @@
         <v>15</v>
       </c>
       <c r="J21" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K21" s="18">
@@ -3654,13 +3589,15 @@
       <c r="M21" s="18">
         <v>5</v>
       </c>
-      <c r="N21" s="18" t="s">
-        <v>141</v>
+      <c r="N21" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>HGTs maximum growth rate of LNG-ICEs</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="18" t="s">
-        <v>48</v>
+      <c r="B22" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-HGT_MaxGrowthHEV</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>13</v>
@@ -3671,7 +3608,7 @@
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
       <c r="G22" s="18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H22" s="18">
         <v>2018</v>
@@ -3680,7 +3617,7 @@
         <v>15</v>
       </c>
       <c r="J22" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K22" s="18">
@@ -3693,14 +3630,16 @@
       <c r="M22" s="18">
         <v>5</v>
       </c>
-      <c r="N22" s="18" t="s">
-        <v>45</v>
+      <c r="N22" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>HGTs maximum growth rate of HEVs</v>
       </c>
       <c r="O22" s="2"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
-        <v>61</v>
+      <c r="B23" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-HGT_MaxGrowthFCV</v>
       </c>
       <c r="C23" s="21" t="s">
         <v>13</v>
@@ -3711,7 +3650,7 @@
       <c r="E23" s="21"/>
       <c r="F23" s="21"/>
       <c r="G23" s="21" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="H23" s="21">
         <v>2018</v>
@@ -3720,7 +3659,7 @@
         <v>15</v>
       </c>
       <c r="J23" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K23" s="21">
@@ -3733,21 +3672,34 @@
       <c r="M23" s="21">
         <v>5</v>
       </c>
-      <c r="N23" s="21" t="s">
-        <v>63</v>
+      <c r="N23" s="21" t="str">
+        <f t="shared" si="2"/>
+        <v>HGTs maximum growth rate of FCVs</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>160</v>
+      </c>
+      <c r="I26" t="s">
+        <v>158</v>
+      </c>
+      <c r="J26" t="s">
+        <v>159</v>
+      </c>
       <c r="K26" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>161</v>
+      </c>
       <c r="I27" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="J27" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
       <c r="K27" s="13">
         <v>0.8</v>
@@ -3757,8 +3709,11 @@
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="I28" t="s">
+        <v>155</v>
+      </c>
       <c r="J28" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
       <c r="K28" s="13">
         <v>0.8</v>
@@ -3776,8 +3731,11 @@
       <c r="E29" s="10" t="s">
         <v>32</v>
       </c>
+      <c r="I29" t="s">
+        <v>155</v>
+      </c>
       <c r="J29" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="K29" s="13">
         <v>0.5</v>
@@ -3797,11 +3755,14 @@
         <v>9959</v>
       </c>
       <c r="E30" s="11">
-        <f t="shared" ref="E30:E35" si="1">D30/C30</f>
+        <f t="shared" ref="E30:E35" si="3">D30/C30</f>
         <v>4.3671013742841359E-2</v>
       </c>
+      <c r="I30" t="s">
+        <v>155</v>
+      </c>
       <c r="J30" t="s">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="K30" s="13">
         <v>0.5</v>
@@ -3819,14 +3780,14 @@
         <v>6580</v>
       </c>
       <c r="E31" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.5375711631511485E-2</v>
       </c>
       <c r="I31" t="s">
-        <v>176</v>
+        <v>138</v>
       </c>
       <c r="J31" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
       <c r="K31" s="13">
         <v>0.5</v>
@@ -3844,11 +3805,14 @@
         <v>201</v>
       </c>
       <c r="E32" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.4214694236691596E-2</v>
       </c>
+      <c r="I32" t="s">
+        <v>138</v>
+      </c>
       <c r="J32" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
       <c r="K32" s="13">
         <v>0.5</v>
@@ -3866,11 +3830,14 @@
         <v>329</v>
       </c>
       <c r="E33" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.9391983185707852E-2</v>
       </c>
+      <c r="I33" t="s">
+        <v>138</v>
+      </c>
       <c r="J33" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="K33" s="13">
         <v>0.5</v>
@@ -3888,11 +3855,14 @@
         <v>485</v>
       </c>
       <c r="E34" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.7573599240265907E-2</v>
       </c>
+      <c r="I34" t="s">
+        <v>138</v>
+      </c>
       <c r="J34" t="s">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="K34" s="13">
         <v>0.5</v>
@@ -3910,14 +3880,14 @@
         <v>1033</v>
       </c>
       <c r="E35" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.187086899046824E-2</v>
       </c>
       <c r="I35" t="s">
-        <v>177</v>
+        <v>139</v>
       </c>
       <c r="J35" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
       <c r="K35" s="13">
         <v>0.5</v>
@@ -3937,8 +3907,11 @@
         <f>D36/C36</f>
         <v>5.5865068892149296E-2</v>
       </c>
+      <c r="I36" t="s">
+        <v>139</v>
+      </c>
       <c r="J36" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="K36" s="13">
         <v>0.5</v>
@@ -3955,11 +3928,14 @@
         <v>2566</v>
       </c>
       <c r="E37" s="11">
-        <f t="shared" ref="E37:E39" si="2">D37/C37</f>
+        <f t="shared" ref="E37:E39" si="4">D37/C37</f>
         <v>6.1874562947601935E-2</v>
       </c>
+      <c r="I37" t="s">
+        <v>139</v>
+      </c>
       <c r="J37" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="K37" s="13">
         <v>0.5</v>
@@ -3976,11 +3952,14 @@
         <v>1224</v>
       </c>
       <c r="E38" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.7044321200540614E-2</v>
       </c>
+      <c r="I38" t="s">
+        <v>139</v>
+      </c>
       <c r="J38" t="s">
-        <v>178</v>
+        <v>140</v>
       </c>
       <c r="K38" s="13">
         <v>0.5</v>
@@ -3998,11 +3977,14 @@
         <v>551</v>
       </c>
       <c r="E39" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9170087453150095E-2</v>
       </c>
+      <c r="I39" t="s">
+        <v>139</v>
+      </c>
       <c r="J39" t="s">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="K39" s="13">
         <v>0.5</v>
@@ -4013,42 +3995,54 @@
         <v>28</v>
       </c>
       <c r="I40" t="s">
-        <v>179</v>
+        <v>141</v>
       </c>
       <c r="J40" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
       <c r="K40" s="13">
         <v>0.5</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I41" t="s">
+        <v>141</v>
+      </c>
       <c r="J41" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="K41" s="13">
         <v>0.5</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I42" t="s">
+        <v>141</v>
+      </c>
       <c r="J42" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="K42" s="13">
         <v>0.5</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>141</v>
+      </c>
       <c r="J43" t="s">
-        <v>178</v>
+        <v>140</v>
       </c>
       <c r="K43" s="13">
         <v>0.5</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I44" t="s">
+        <v>141</v>
+      </c>
       <c r="J44" t="s">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="K44" s="13">
         <v>0.5</v>
@@ -4056,7 +4050,7 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>181</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -4064,7 +4058,7 @@
         <v>33</v>
       </c>
       <c r="C46" t="s">
-        <v>156</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -4116,7 +4110,7 @@
         <v>2030</v>
       </c>
       <c r="P48" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -4180,43 +4174,43 @@
         <v>341.54999999999995</v>
       </c>
       <c r="E50" s="20">
-        <f t="shared" ref="E50:H50" si="3">D50*(1+$B$47)</f>
+        <f t="shared" ref="E50:H50" si="5">D50*(1+$B$47)</f>
         <v>512.32499999999993</v>
       </c>
       <c r="F50" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>768.48749999999995</v>
       </c>
       <c r="G50" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1152.7312499999998</v>
       </c>
       <c r="H50" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1729.0968749999997</v>
       </c>
       <c r="I50" s="14">
-        <f t="shared" ref="I50" si="4">H50*(1+$B$47)</f>
+        <f t="shared" ref="I50" si="6">H50*(1+$B$47)</f>
         <v>2593.6453124999998</v>
       </c>
       <c r="J50" s="14">
-        <f t="shared" ref="J50" si="5">I50*(1+$B$47)</f>
+        <f t="shared" ref="J50" si="7">I50*(1+$B$47)</f>
         <v>3890.4679687499997</v>
       </c>
       <c r="K50" s="14">
-        <f t="shared" ref="K50" si="6">J50*(1+$B$47)</f>
+        <f t="shared" ref="K50" si="8">J50*(1+$B$47)</f>
         <v>5835.7019531249998</v>
       </c>
       <c r="L50" s="14">
-        <f t="shared" ref="L50" si="7">K50*(1+$B$47)</f>
+        <f t="shared" ref="L50" si="9">K50*(1+$B$47)</f>
         <v>8753.5529296874993</v>
       </c>
       <c r="M50" s="14">
-        <f t="shared" ref="M50" si="8">L50*(1+$B$47)</f>
+        <f t="shared" ref="M50" si="10">L50*(1+$B$47)</f>
         <v>13130.329394531249</v>
       </c>
       <c r="N50" s="14">
-        <f t="shared" ref="N50" si="9">M50*(1+$B$47)</f>
+        <f t="shared" ref="N50" si="11">M50*(1+$B$47)</f>
         <v>19695.494091796874</v>
       </c>
       <c r="O50" s="31">
@@ -4241,51 +4235,51 @@
         <v>79.5</v>
       </c>
       <c r="D51" s="14">
-        <f t="shared" ref="D51:L51" si="10">C51*(1+$B$47)</f>
+        <f t="shared" ref="D51:L51" si="12">C51*(1+$B$47)</f>
         <v>119.25</v>
       </c>
       <c r="E51" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>178.875</v>
       </c>
       <c r="F51" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>268.3125</v>
       </c>
       <c r="G51" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>402.46875</v>
       </c>
       <c r="H51" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>603.703125</v>
       </c>
       <c r="I51" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>905.5546875</v>
       </c>
       <c r="J51" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1358.33203125</v>
       </c>
       <c r="K51" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2037.498046875</v>
       </c>
       <c r="L51" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3056.2470703125</v>
       </c>
       <c r="M51" s="14">
-        <f t="shared" ref="M51:M53" si="11">L51*(1+$B$47)</f>
+        <f t="shared" ref="M51:M53" si="13">L51*(1+$B$47)</f>
         <v>4584.37060546875</v>
       </c>
       <c r="N51" s="14">
-        <f t="shared" ref="N51:N53" si="12">M51*(1+$B$47)</f>
+        <f t="shared" ref="N51:N53" si="14">M51*(1+$B$47)</f>
         <v>6876.555908203125</v>
       </c>
       <c r="O51" s="31">
-        <f t="shared" ref="O51:O53" si="13">N51*(1+$B$47)</f>
+        <f t="shared" ref="O51:O53" si="15">N51*(1+$B$47)</f>
         <v>10314.833862304688</v>
       </c>
       <c r="P51" s="15">
@@ -4310,47 +4304,47 @@
         <v>3721.2749999999996</v>
       </c>
       <c r="E52" s="20">
-        <f t="shared" ref="E52:L52" si="14">D52*(1+$B$47)</f>
+        <f t="shared" ref="E52:L52" si="16">D52*(1+$B$47)</f>
         <v>5581.9124999999995</v>
       </c>
       <c r="F52" s="14">
+        <f t="shared" si="16"/>
+        <v>8372.8687499999996</v>
+      </c>
+      <c r="G52" s="14">
+        <f t="shared" si="16"/>
+        <v>12559.303124999999</v>
+      </c>
+      <c r="H52" s="14">
+        <f t="shared" si="16"/>
+        <v>18838.954687499998</v>
+      </c>
+      <c r="I52" s="14">
+        <f t="shared" si="16"/>
+        <v>28258.432031249999</v>
+      </c>
+      <c r="J52" s="14">
+        <f t="shared" si="16"/>
+        <v>42387.648046874994</v>
+      </c>
+      <c r="K52" s="14">
+        <f t="shared" si="16"/>
+        <v>63581.472070312491</v>
+      </c>
+      <c r="L52" s="14">
+        <f t="shared" si="16"/>
+        <v>95372.208105468744</v>
+      </c>
+      <c r="M52" s="14">
+        <f t="shared" si="13"/>
+        <v>143058.3121582031</v>
+      </c>
+      <c r="N52" s="14">
         <f t="shared" si="14"/>
-        <v>8372.8687499999996</v>
-      </c>
-      <c r="G52" s="14">
-        <f t="shared" si="14"/>
-        <v>12559.303124999999</v>
-      </c>
-      <c r="H52" s="14">
-        <f t="shared" si="14"/>
-        <v>18838.954687499998</v>
-      </c>
-      <c r="I52" s="14">
-        <f t="shared" si="14"/>
-        <v>28258.432031249999</v>
-      </c>
-      <c r="J52" s="14">
-        <f t="shared" si="14"/>
-        <v>42387.648046874994</v>
-      </c>
-      <c r="K52" s="14">
-        <f t="shared" si="14"/>
-        <v>63581.472070312491</v>
-      </c>
-      <c r="L52" s="14">
-        <f t="shared" si="14"/>
-        <v>95372.208105468744</v>
-      </c>
-      <c r="M52" s="14">
-        <f t="shared" si="11"/>
-        <v>143058.3121582031</v>
-      </c>
-      <c r="N52" s="14">
-        <f t="shared" si="12"/>
         <v>214587.46823730465</v>
       </c>
       <c r="O52" s="31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>321881.20235595701</v>
       </c>
       <c r="P52" s="15">
@@ -4371,51 +4365,51 @@
         <v>18168.149999999998</v>
       </c>
       <c r="D53" s="14">
-        <f t="shared" ref="D53:L53" si="15">C53*(1+$B$47)</f>
+        <f t="shared" ref="D53:L53" si="17">C53*(1+$B$47)</f>
         <v>27252.224999999999</v>
       </c>
       <c r="E53" s="20">
+        <f t="shared" si="17"/>
+        <v>40878.337499999994</v>
+      </c>
+      <c r="F53" s="14">
+        <f t="shared" si="17"/>
+        <v>61317.506249999991</v>
+      </c>
+      <c r="G53" s="14">
+        <f t="shared" si="17"/>
+        <v>91976.259374999994</v>
+      </c>
+      <c r="H53" s="14">
+        <f t="shared" si="17"/>
+        <v>137964.38906249998</v>
+      </c>
+      <c r="I53" s="14">
+        <f t="shared" si="17"/>
+        <v>206946.58359374997</v>
+      </c>
+      <c r="J53" s="14">
+        <f t="shared" si="17"/>
+        <v>310419.87539062498</v>
+      </c>
+      <c r="K53" s="14">
+        <f t="shared" si="17"/>
+        <v>465629.81308593747</v>
+      </c>
+      <c r="L53" s="14">
+        <f t="shared" si="17"/>
+        <v>698444.71962890623</v>
+      </c>
+      <c r="M53" s="14">
+        <f t="shared" si="13"/>
+        <v>1047667.0794433593</v>
+      </c>
+      <c r="N53" s="14">
+        <f t="shared" si="14"/>
+        <v>1571500.6191650389</v>
+      </c>
+      <c r="O53" s="31">
         <f t="shared" si="15"/>
-        <v>40878.337499999994</v>
-      </c>
-      <c r="F53" s="14">
-        <f t="shared" si="15"/>
-        <v>61317.506249999991</v>
-      </c>
-      <c r="G53" s="14">
-        <f t="shared" si="15"/>
-        <v>91976.259374999994</v>
-      </c>
-      <c r="H53" s="14">
-        <f t="shared" si="15"/>
-        <v>137964.38906249998</v>
-      </c>
-      <c r="I53" s="14">
-        <f t="shared" si="15"/>
-        <v>206946.58359374997</v>
-      </c>
-      <c r="J53" s="14">
-        <f t="shared" si="15"/>
-        <v>310419.87539062498</v>
-      </c>
-      <c r="K53" s="14">
-        <f t="shared" si="15"/>
-        <v>465629.81308593747</v>
-      </c>
-      <c r="L53" s="14">
-        <f t="shared" si="15"/>
-        <v>698444.71962890623</v>
-      </c>
-      <c r="M53" s="14">
-        <f t="shared" si="11"/>
-        <v>1047667.0794433593</v>
-      </c>
-      <c r="N53" s="14">
-        <f t="shared" si="12"/>
-        <v>1571500.6191650389</v>
-      </c>
-      <c r="O53" s="31">
-        <f t="shared" si="13"/>
         <v>2357250.9287475585</v>
       </c>
       <c r="P53" s="15">
@@ -4437,7 +4431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5F46D0-BFBE-459D-AD94-C3EBC85EC70F}">
   <dimension ref="A2:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -4555,11 +4549,11 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
       <c r="H6" s="2">
         <v>2018</v>
@@ -4596,11 +4590,11 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>170</v>
+        <v>134</v>
       </c>
       <c r="H7" s="2">
         <v>2018</v>
@@ -4685,10 +4679,10 @@
         <v>8</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>192</v>
+        <v>153</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>193</v>
+        <v>154</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>43</v>
@@ -4706,14 +4700,14 @@
         <v>UC_SRV_MaxGrowth_Biomass</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>191</v>
+        <v>152</v>
       </c>
       <c r="D11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>185</v>
+        <v>146</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="H11" s="2">
         <v>2018</v>
@@ -4746,14 +4740,14 @@
         <v>UC_SRV_MaxGrowth_Biogas</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>191</v>
+        <v>152</v>
       </c>
       <c r="D12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>186</v>
+        <v>147</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="H12" s="2">
         <v>2018</v>
@@ -4782,18 +4776,18 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="D14" t="s">
-        <v>155</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>130</v>
       </c>
       <c r="B15" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
       <c r="C15" s="13">
         <v>0.05</v>
@@ -4804,10 +4798,10 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>167</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
       <c r="C16" s="13">
         <v>0.05</v>
@@ -4818,10 +4812,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>184</v>
+        <v>145</v>
       </c>
       <c r="B17" t="s">
-        <v>182</v>
+        <v>143</v>
       </c>
       <c r="C17" s="13">
         <v>0.05</v>
@@ -4832,10 +4826,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>184</v>
+        <v>145</v>
       </c>
       <c r="B18" t="s">
-        <v>183</v>
+        <v>144</v>
       </c>
       <c r="C18" s="13">
         <v>0.05</v>
@@ -4850,6 +4844,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -5060,12 +5060,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5076,6 +5070,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5094,15 +5097,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Make the max growth constraint for BEVs more flexible
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393EC184-907A-4881-972A-027EF8CC88DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF98D62-AB3E-4693-BA8A-F2DB9F3886FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="162">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -225,97 +225,25 @@
     <t>T-CAR-PHEV*</t>
   </si>
   <si>
-    <t>HGT-Maximum growth rate of HEVs</t>
-  </si>
-  <si>
-    <t>HGT-Maximum growth rate of BEVs</t>
-  </si>
-  <si>
-    <t>UC-HGT_MaxGrowthBEV</t>
-  </si>
-  <si>
-    <t>UC-HGT_MaxGrowthHEV</t>
-  </si>
-  <si>
     <t>T-HGT-HEV*</t>
   </si>
   <si>
     <t>T-MGT-HEV*</t>
   </si>
   <si>
-    <t>UC-MGT-MaxGrowthBEV</t>
-  </si>
-  <si>
-    <t>UC-MGT-MaxGrowthHEV</t>
-  </si>
-  <si>
-    <t>MGT-Maximum growth rate of BEVs</t>
-  </si>
-  <si>
-    <t>MGT-Maximum growth rate of HEVs</t>
-  </si>
-  <si>
-    <t>UC-LGT_MaxGrowthBEV</t>
-  </si>
-  <si>
-    <t>LGT-Maximum growth rate of BEVs</t>
-  </si>
-  <si>
-    <t>UC-CAR_MaxGrowthBEV</t>
-  </si>
-  <si>
-    <t>UC-CAR_MaxGrowthPHEV</t>
-  </si>
-  <si>
-    <t>Cars-Maximum growth rate of BEVs</t>
-  </si>
-  <si>
-    <t>Cars-Maximum growth rate of PHEVs</t>
-  </si>
-  <si>
-    <t>UC-HGT_MaxGrowthFCV</t>
-  </si>
-  <si>
     <t>T-HGT-FCV*</t>
   </si>
   <si>
-    <t>HGT-Maximum growth rate of FCVs</t>
-  </si>
-  <si>
-    <t>MGT-Maximum growth rate of FCVs</t>
-  </si>
-  <si>
     <t>T-MGT-FCV*</t>
   </si>
   <si>
-    <t>UC-MGT-MaxGrowthFCV</t>
-  </si>
-  <si>
     <t>T-CAR-FCV*</t>
   </si>
   <si>
-    <t>UC-CAR_MaxGrowthFCV</t>
-  </si>
-  <si>
-    <t>Cars-Maximum growth rate of FCVs</t>
-  </si>
-  <si>
-    <t>LGT-Maximum growth rate of PHEVs</t>
-  </si>
-  <si>
-    <t>LGT-Maximum growth rate of FCVs</t>
-  </si>
-  <si>
     <t>T-LGT-PHEV*</t>
   </si>
   <si>
     <t>T-LGT-FCV*</t>
-  </si>
-  <si>
-    <t>UC-LGT_MaxGrowthPHEV</t>
-  </si>
-  <si>
-    <t>UC-LGT_MaxGrowthFCV</t>
   </si>
   <si>
     <t>Development</t>
@@ -515,60 +443,24 @@
     </r>
   </si>
   <si>
-    <t>UC-HGT_MaxGrowthNGICE</t>
-  </si>
-  <si>
-    <t>UC-MGT-MaxGrowthNGICE</t>
-  </si>
-  <si>
     <t>T-MGT-ICE_NG*</t>
   </si>
   <si>
-    <t>MGT-Maximum growth rate of NG-ICEs</t>
-  </si>
-  <si>
-    <t>HGT-Maximum growth rate of NG-ICEs</t>
-  </si>
-  <si>
-    <t>UC-HGT_MaxGrowthLNGICE</t>
-  </si>
-  <si>
-    <t>HGT-Maximum growth rate of LNG-ICEs</t>
-  </si>
-  <si>
-    <t>UC-MGT-MaxGrowthLNGICE</t>
-  </si>
-  <si>
     <t>T-MGT-ICE_LNG*</t>
   </si>
   <si>
-    <t>MGT-Maximum growth rate of LNG-ICEs</t>
-  </si>
-  <si>
     <t>T-HGT-ICE_NG*</t>
   </si>
   <si>
     <t>T-HGT-ICE_LNG*</t>
   </si>
   <si>
-    <t>UC-CAR_MaxGrowthNGICE</t>
-  </si>
-  <si>
     <t>T-CAR-ICE_NG*</t>
   </si>
   <si>
-    <t>Cars-Maximum growth rate of NG-ICEs</t>
-  </si>
-  <si>
-    <t>UC-LGT_MaxGrowthNGICE</t>
-  </si>
-  <si>
     <t>T-LGT-ICE_NG*</t>
   </si>
   <si>
-    <t>LGT-Maximum growth rate of NG-ICEs</t>
-  </si>
-  <si>
     <t>Max growth rate</t>
   </si>
   <si>
@@ -623,18 +515,12 @@
     <t>S-SH*CS*</t>
   </si>
   <si>
-    <t>Cars</t>
-  </si>
-  <si>
     <t>BEV</t>
   </si>
   <si>
     <t>PHEV</t>
   </si>
   <si>
-    <t>NG-ICEs</t>
-  </si>
-  <si>
     <t>FCV</t>
   </si>
   <si>
@@ -650,9 +536,6 @@
     <t>HGT</t>
   </si>
   <si>
-    <t>LNG-ICEs</t>
-  </si>
-  <si>
     <t>Playground</t>
   </si>
   <si>
@@ -690,6 +573,27 @@
   </si>
   <si>
     <t>UC_ACT~RHS</t>
+  </si>
+  <si>
+    <t>CAR</t>
+  </si>
+  <si>
+    <t>NG-ICE</t>
+  </si>
+  <si>
+    <t>LNG-ICE</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>On/Off</t>
+  </si>
+  <si>
+    <t>Seed Value</t>
   </si>
 </sst>
 </file>
@@ -1999,13 +1903,13 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>163</v>
+        <v>127</v>
       </c>
       <c r="E5" s="23" t="str">
         <f>Regions!A11</f>
@@ -2114,7 +2018,7 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="C6" s="23" t="str">
         <f>C5</f>
@@ -2231,7 +2135,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="C7" s="23" t="str">
         <f>"*"&amp;C5</f>
@@ -2348,223 +2252,223 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2724,7 +2628,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="H6" s="2">
         <v>2018</v>
@@ -2760,7 +2664,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="H7">
         <v>2035</v>
@@ -2796,7 +2700,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>158</v>
+        <v>122</v>
       </c>
       <c r="H8">
         <v>2035</v>
@@ -2825,7 +2729,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="35" t="s">
-        <v>188</v>
+        <v>149</v>
       </c>
       <c r="C9" s="35" t="s">
         <v>13</v>
@@ -2834,7 +2738,7 @@
       <c r="E9" s="35"/>
       <c r="F9" s="35"/>
       <c r="G9" s="35" t="s">
-        <v>189</v>
+        <v>150</v>
       </c>
       <c r="H9" s="35">
         <v>2020</v>
@@ -2856,23 +2760,23 @@
         <v>5</v>
       </c>
       <c r="N9" s="35" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="D11" t="s">
-        <v>155</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="B12" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
       <c r="C12" s="13">
         <v>0.2</v>
@@ -2883,10 +2787,10 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s">
-        <v>161</v>
+        <v>125</v>
       </c>
       <c r="C13" s="13">
         <v>0.2</v>
@@ -2897,10 +2801,10 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s">
-        <v>162</v>
+        <v>126</v>
       </c>
       <c r="C14" s="13">
         <v>0.2</v>
@@ -2918,8 +2822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
   <dimension ref="A2:P53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2928,12 +2832,12 @@
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.5703125" customWidth="1"/>
-    <col min="14" max="14" width="34" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" customWidth="1"/>
     <col min="15" max="15" width="10.7109375" customWidth="1"/>
     <col min="16" max="16" width="11.140625" customWidth="1"/>
   </cols>
@@ -3035,8 +2939,9 @@
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
-        <v>57</v>
+      <c r="B6" s="18" t="str">
+        <f t="shared" ref="B6:B23" si="0">IF(H27="*","*",_xlfn.TEXTJOIN("",TRUE,"UC-",I27,"_MaxGrowth",J27))</f>
+        <v>UC-CAR_MaxGrowthBEV</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>13</v>
@@ -3056,26 +2961,28 @@
         <v>15</v>
       </c>
       <c r="J6" s="29">
-        <f t="shared" ref="J6:J23" si="0">1+$K27</f>
+        <f t="shared" ref="J6:J23" si="1">1+$K27</f>
         <v>1.8</v>
       </c>
       <c r="K6" s="18">
         <v>1</v>
       </c>
       <c r="L6" s="19">
-        <f>-C53/1000</f>
+        <f t="shared" ref="L6:L9" si="2">-$B$53*L27/1000</f>
         <v>-18.168149999999997</v>
       </c>
       <c r="M6" s="18">
         <v>5</v>
       </c>
-      <c r="N6" s="18" t="s">
-        <v>59</v>
+      <c r="N6" s="18" t="str">
+        <f t="shared" ref="N6:N23" si="3">_xlfn.TEXTJOIN(" ", TRUE,I27&amp;"s","maximum growth rate of",J27&amp;"s")</f>
+        <v>CARs maximum growth rate of BEVs</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
-        <v>58</v>
+      <c r="B7" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-CAR_MaxGrowthPHEV</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>13</v>
@@ -3095,26 +3002,28 @@
         <v>15</v>
       </c>
       <c r="J7" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8</v>
       </c>
       <c r="K7" s="18">
         <v>1</v>
       </c>
       <c r="L7" s="19">
-        <f>-C53/1000</f>
+        <f t="shared" si="2"/>
         <v>-18.168149999999997</v>
       </c>
       <c r="M7" s="18">
         <v>5</v>
       </c>
-      <c r="N7" s="18" t="s">
-        <v>60</v>
+      <c r="N7" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>CARs maximum growth rate of PHEVs</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="18" t="s">
-        <v>147</v>
+      <c r="B8" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-CAR_MaxGrowthNG-ICE</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>13</v>
@@ -3125,7 +3034,7 @@
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="18" t="s">
-        <v>148</v>
+        <v>115</v>
       </c>
       <c r="H8" s="18">
         <v>2018</v>
@@ -3134,26 +3043,28 @@
         <v>15</v>
       </c>
       <c r="J8" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K8" s="18">
         <v>1</v>
       </c>
       <c r="L8" s="19">
-        <f>-C53/1000</f>
+        <f t="shared" si="2"/>
         <v>-18.168149999999997</v>
       </c>
       <c r="M8" s="18">
         <v>5</v>
       </c>
-      <c r="N8" s="18" t="s">
-        <v>149</v>
+      <c r="N8" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>CARs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
-        <v>68</v>
+      <c r="B9" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-CAR_MaxGrowthFCV</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>13</v>
@@ -3164,7 +3075,7 @@
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="H9" s="21">
         <v>2018</v>
@@ -3173,26 +3084,28 @@
         <v>15</v>
       </c>
       <c r="J9" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K9" s="21">
         <v>1</v>
       </c>
       <c r="L9" s="22">
-        <f>-C53/1000</f>
+        <f t="shared" ref="L9:L10" si="4">-$B$53*L30/1000</f>
         <v>-18.168149999999997</v>
       </c>
       <c r="M9" s="21">
         <v>5</v>
       </c>
-      <c r="N9" s="21" t="s">
-        <v>69</v>
+      <c r="N9" s="21" t="str">
+        <f t="shared" si="3"/>
+        <v>CARs maximum growth rate of FCVs</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
-        <v>55</v>
+      <c r="B10" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-LGT_MaxGrowthBEV</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>13</v>
@@ -3212,26 +3125,28 @@
         <v>15</v>
       </c>
       <c r="J10" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K10" s="18">
         <v>1</v>
       </c>
       <c r="L10" s="19">
-        <f>-C52/1000</f>
+        <f t="shared" ref="L10:L13" si="5">-$B$52*L31/1000</f>
         <v>-2.4808499999999998</v>
       </c>
       <c r="M10" s="18">
         <v>5</v>
       </c>
-      <c r="N10" s="18" t="s">
-        <v>56</v>
+      <c r="N10" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>LGTs maximum growth rate of BEVs</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
-        <v>74</v>
+      <c r="B11" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-LGT_MaxGrowthPHEV</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>13</v>
@@ -3242,7 +3157,7 @@
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="H11" s="18">
         <v>2018</v>
@@ -3251,26 +3166,28 @@
         <v>15</v>
       </c>
       <c r="J11" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K11" s="18">
         <v>1</v>
       </c>
       <c r="L11" s="19">
-        <f>-C52/1000</f>
+        <f t="shared" si="5"/>
         <v>-2.4808499999999998</v>
       </c>
       <c r="M11" s="18">
         <v>5</v>
       </c>
-      <c r="N11" s="18" t="s">
-        <v>70</v>
+      <c r="N11" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>LGTs maximum growth rate of PHEVs</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="18" t="s">
-        <v>150</v>
+      <c r="B12" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-LGT_MaxGrowthNG-ICE</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>13</v>
@@ -3281,7 +3198,7 @@
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="H12" s="18">
         <v>2018</v>
@@ -3290,26 +3207,28 @@
         <v>15</v>
       </c>
       <c r="J12" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K12" s="18">
         <v>1</v>
       </c>
       <c r="L12" s="19">
-        <f>-C52/1000</f>
+        <f t="shared" si="5"/>
         <v>-2.4808499999999998</v>
       </c>
       <c r="M12" s="18">
         <v>5</v>
       </c>
-      <c r="N12" s="18" t="s">
-        <v>152</v>
+      <c r="N12" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>LGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
-        <v>75</v>
+      <c r="B13" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-LGT_MaxGrowthFCV</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>13</v>
@@ -3320,7 +3239,7 @@
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
       <c r="G13" s="21" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="H13" s="21">
         <v>2018</v>
@@ -3329,26 +3248,28 @@
         <v>15</v>
       </c>
       <c r="J13" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K13" s="21">
         <v>1</v>
       </c>
       <c r="L13" s="22">
-        <f>-C52/1000</f>
+        <f t="shared" ref="L13:L14" si="6">-$B$52*L34/1000</f>
         <v>-2.4808499999999998</v>
       </c>
       <c r="M13" s="21">
         <v>5</v>
       </c>
-      <c r="N13" s="21" t="s">
-        <v>71</v>
+      <c r="N13" s="21" t="str">
+        <f t="shared" si="3"/>
+        <v>LGTs maximum growth rate of FCVs</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="18" t="s">
-        <v>51</v>
+      <c r="B14" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-MGT_MaxGrowthBEV</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>13</v>
@@ -3368,26 +3289,28 @@
         <v>15</v>
       </c>
       <c r="J14" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K14" s="18">
         <v>1</v>
       </c>
       <c r="L14" s="19">
-        <f>-C51/1000</f>
+        <f t="shared" ref="L14:L18" si="7">-$B$51*L35/1000</f>
         <v>-7.9500000000000001E-2</v>
       </c>
       <c r="M14" s="18">
         <v>5</v>
       </c>
-      <c r="N14" s="18" t="s">
-        <v>53</v>
+      <c r="N14" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>MGTs maximum growth rate of BEVs</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="18" t="s">
-        <v>136</v>
+      <c r="B15" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-MGT_MaxGrowthNG-ICE</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>13</v>
@@ -3398,7 +3321,7 @@
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="18" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="H15" s="18">
         <v>2018</v>
@@ -3407,26 +3330,28 @@
         <v>15</v>
       </c>
       <c r="J15" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K15" s="18">
         <v>1</v>
       </c>
       <c r="L15" s="19">
-        <f>-C51/1000</f>
+        <f t="shared" si="7"/>
         <v>-7.9500000000000001E-2</v>
       </c>
       <c r="M15" s="18">
         <v>5</v>
       </c>
-      <c r="N15" s="18" t="s">
-        <v>138</v>
+      <c r="N15" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>MGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
-        <v>142</v>
+      <c r="B16" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-MGT_MaxGrowthLNG-ICE</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>13</v>
@@ -3437,7 +3362,7 @@
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="G16" s="18" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="H16" s="18">
         <v>2018</v>
@@ -3446,26 +3371,28 @@
         <v>15</v>
       </c>
       <c r="J16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K16" s="18">
         <v>1</v>
       </c>
       <c r="L16" s="19">
-        <f>-C51/1000</f>
+        <f t="shared" si="7"/>
         <v>-7.9500000000000001E-2</v>
       </c>
       <c r="M16" s="18">
         <v>5</v>
       </c>
-      <c r="N16" s="18" t="s">
-        <v>144</v>
+      <c r="N16" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>MGTs maximum growth rate of LNG-ICEs</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="s">
-        <v>52</v>
+      <c r="B17" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-MGT_MaxGrowthHEV</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>13</v>
@@ -3476,7 +3403,7 @@
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
       <c r="G17" s="18" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H17" s="18">
         <v>2018</v>
@@ -3485,26 +3412,28 @@
         <v>15</v>
       </c>
       <c r="J17" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K17" s="18">
         <v>1</v>
       </c>
       <c r="L17" s="19">
-        <f>-C51/1000</f>
+        <f t="shared" si="7"/>
         <v>-7.9500000000000001E-2</v>
       </c>
       <c r="M17" s="18">
         <v>5</v>
       </c>
-      <c r="N17" s="18" t="s">
-        <v>54</v>
+      <c r="N17" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>MGTs maximum growth rate of HEVs</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="21" t="s">
-        <v>66</v>
+      <c r="B18" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-MGT_MaxGrowthFCV</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>13</v>
@@ -3515,7 +3444,7 @@
       <c r="E18" s="21"/>
       <c r="F18" s="21"/>
       <c r="G18" s="21" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="H18" s="21">
         <v>2018</v>
@@ -3524,26 +3453,28 @@
         <v>15</v>
       </c>
       <c r="J18" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K18" s="21">
         <v>1</v>
       </c>
       <c r="L18" s="22">
-        <f>-C51/1000</f>
+        <f t="shared" ref="L18:L19" si="8">-$B$51*L39/1000</f>
         <v>-7.9500000000000001E-2</v>
       </c>
       <c r="M18" s="21">
         <v>5</v>
       </c>
-      <c r="N18" s="21" t="s">
-        <v>64</v>
+      <c r="N18" s="21" t="str">
+        <f t="shared" si="3"/>
+        <v>MGTs maximum growth rate of FCVs</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="18" t="s">
-        <v>47</v>
+      <c r="B19" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-HGT_MaxGrowthBEV</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>13</v>
@@ -3563,26 +3494,28 @@
         <v>15</v>
       </c>
       <c r="J19" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K19" s="18">
         <v>1</v>
       </c>
       <c r="L19" s="19">
-        <f>-C50/1000</f>
+        <f t="shared" ref="L19:L23" si="9">-$B$50*L40/1000</f>
         <v>-0.22769999999999999</v>
       </c>
       <c r="M19" s="18">
         <v>5</v>
       </c>
-      <c r="N19" s="18" t="s">
-        <v>46</v>
+      <c r="N19" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>HGTs maximum growth rate of BEVs</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="18" t="s">
-        <v>135</v>
+      <c r="B20" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-HGT_MaxGrowthNG-ICE</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>13</v>
@@ -3593,7 +3526,7 @@
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="18" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="H20" s="18">
         <v>2018</v>
@@ -3602,26 +3535,28 @@
         <v>15</v>
       </c>
       <c r="J20" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K20" s="18">
         <v>1</v>
       </c>
       <c r="L20" s="19">
-        <f>-C50/1000</f>
+        <f t="shared" si="9"/>
         <v>-0.22769999999999999</v>
       </c>
       <c r="M20" s="18">
         <v>5</v>
       </c>
-      <c r="N20" s="18" t="s">
-        <v>139</v>
+      <c r="N20" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>HGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="18" t="s">
-        <v>140</v>
+      <c r="B21" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-HGT_MaxGrowthLNG-ICE</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>13</v>
@@ -3632,7 +3567,7 @@
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="18" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="H21" s="18">
         <v>2018</v>
@@ -3641,26 +3576,28 @@
         <v>15</v>
       </c>
       <c r="J21" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K21" s="18">
         <v>1</v>
       </c>
       <c r="L21" s="19">
-        <f>-C50/1000</f>
+        <f t="shared" si="9"/>
         <v>-0.22769999999999999</v>
       </c>
       <c r="M21" s="18">
         <v>5</v>
       </c>
-      <c r="N21" s="18" t="s">
-        <v>141</v>
+      <c r="N21" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>HGTs maximum growth rate of LNG-ICEs</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="18" t="s">
-        <v>48</v>
+      <c r="B22" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-HGT_MaxGrowthHEV</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>13</v>
@@ -3671,7 +3608,7 @@
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
       <c r="G22" s="18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H22" s="18">
         <v>2018</v>
@@ -3680,27 +3617,29 @@
         <v>15</v>
       </c>
       <c r="J22" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K22" s="18">
         <v>1</v>
       </c>
       <c r="L22" s="19">
-        <f>-C50/1000</f>
+        <f t="shared" si="9"/>
         <v>-0.22769999999999999</v>
       </c>
       <c r="M22" s="18">
         <v>5</v>
       </c>
-      <c r="N22" s="18" t="s">
-        <v>45</v>
+      <c r="N22" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>HGTs maximum growth rate of HEVs</v>
       </c>
       <c r="O22" s="2"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
-        <v>61</v>
+      <c r="B23" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>UC-HGT_MaxGrowthFCV</v>
       </c>
       <c r="C23" s="21" t="s">
         <v>13</v>
@@ -3711,7 +3650,7 @@
       <c r="E23" s="21"/>
       <c r="F23" s="21"/>
       <c r="G23" s="21" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="H23" s="21">
         <v>2018</v>
@@ -3720,48 +3659,70 @@
         <v>15</v>
       </c>
       <c r="J23" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="K23" s="21">
         <v>1</v>
       </c>
       <c r="L23" s="22">
-        <f>-C50/1000</f>
+        <f t="shared" si="9"/>
         <v>-0.22769999999999999</v>
       </c>
       <c r="M23" s="21">
         <v>5</v>
       </c>
-      <c r="N23" s="21" t="s">
-        <v>63</v>
+      <c r="N23" s="21" t="str">
+        <f t="shared" si="3"/>
+        <v>HGTs maximum growth rate of FCVs</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>160</v>
+      </c>
+      <c r="I26" t="s">
+        <v>158</v>
+      </c>
+      <c r="J26" t="s">
+        <v>159</v>
+      </c>
       <c r="K26" t="s">
-        <v>153</v>
+        <v>117</v>
+      </c>
+      <c r="L26" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I27" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="J27" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
       <c r="K27" s="13">
         <v>0.8</v>
+      </c>
+      <c r="L27" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="I28" t="s">
+        <v>155</v>
+      </c>
       <c r="J28" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
       <c r="K28" s="13">
         <v>0.8</v>
+      </c>
+      <c r="L28" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -3776,11 +3737,17 @@
       <c r="E29" s="10" t="s">
         <v>32</v>
       </c>
+      <c r="I29" t="s">
+        <v>155</v>
+      </c>
       <c r="J29" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="K29" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L29" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -3797,14 +3764,20 @@
         <v>9959</v>
       </c>
       <c r="E30" s="11">
-        <f t="shared" ref="E30:E35" si="1">D30/C30</f>
+        <f t="shared" ref="E30:E35" si="10">D30/C30</f>
         <v>4.3671013742841359E-2</v>
       </c>
+      <c r="I30" t="s">
+        <v>155</v>
+      </c>
       <c r="J30" t="s">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="K30" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L30" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -3819,17 +3792,20 @@
         <v>6580</v>
       </c>
       <c r="E31" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>6.5375711631511485E-2</v>
       </c>
       <c r="I31" t="s">
-        <v>176</v>
+        <v>138</v>
       </c>
       <c r="J31" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
       <c r="K31" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L31" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -3844,14 +3820,20 @@
         <v>201</v>
       </c>
       <c r="E32" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>4.4214694236691596E-2</v>
       </c>
+      <c r="I32" t="s">
+        <v>138</v>
+      </c>
       <c r="J32" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
       <c r="K32" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L32" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -3866,14 +3848,20 @@
         <v>329</v>
       </c>
       <c r="E33" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>4.9391983185707852E-2</v>
       </c>
+      <c r="I33" t="s">
+        <v>138</v>
+      </c>
       <c r="J33" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="K33" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L33" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -3888,14 +3876,20 @@
         <v>485</v>
       </c>
       <c r="E34" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>5.7573599240265907E-2</v>
       </c>
+      <c r="I34" t="s">
+        <v>138</v>
+      </c>
       <c r="J34" t="s">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="K34" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L34" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -3910,17 +3904,20 @@
         <v>1033</v>
       </c>
       <c r="E35" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>7.187086899046824E-2</v>
       </c>
       <c r="I35" t="s">
-        <v>177</v>
+        <v>139</v>
       </c>
       <c r="J35" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
       <c r="K35" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L35" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -3937,11 +3934,17 @@
         <f>D36/C36</f>
         <v>5.5865068892149296E-2</v>
       </c>
+      <c r="I36" t="s">
+        <v>139</v>
+      </c>
       <c r="J36" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="K36" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L36" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -3955,14 +3958,20 @@
         <v>2566</v>
       </c>
       <c r="E37" s="11">
-        <f t="shared" ref="E37:E39" si="2">D37/C37</f>
+        <f t="shared" ref="E37:E39" si="11">D37/C37</f>
         <v>6.1874562947601935E-2</v>
       </c>
+      <c r="I37" t="s">
+        <v>139</v>
+      </c>
       <c r="J37" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="K37" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L37" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -3976,14 +3985,20 @@
         <v>1224</v>
       </c>
       <c r="E38" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>5.7044321200540614E-2</v>
       </c>
+      <c r="I38" t="s">
+        <v>139</v>
+      </c>
       <c r="J38" t="s">
-        <v>178</v>
+        <v>140</v>
       </c>
       <c r="K38" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L38" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -3998,14 +4013,20 @@
         <v>551</v>
       </c>
       <c r="E39" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4.9170087453150095E-2</v>
       </c>
+      <c r="I39" t="s">
+        <v>139</v>
+      </c>
       <c r="J39" t="s">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="K39" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L39" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -4013,50 +4034,77 @@
         <v>28</v>
       </c>
       <c r="I40" t="s">
-        <v>179</v>
+        <v>141</v>
       </c>
       <c r="J40" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
       <c r="K40" s="13">
         <v>0.5</v>
       </c>
+      <c r="L40" s="13">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I41" t="s">
+        <v>141</v>
+      </c>
       <c r="J41" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="K41" s="13">
         <v>0.5</v>
       </c>
+      <c r="L41" s="13">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I42" t="s">
+        <v>141</v>
+      </c>
       <c r="J42" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="K42" s="13">
         <v>0.5</v>
       </c>
+      <c r="L42" s="13">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>141</v>
+      </c>
       <c r="J43" t="s">
-        <v>178</v>
+        <v>140</v>
       </c>
       <c r="K43" s="13">
         <v>0.5</v>
       </c>
+      <c r="L43" s="13">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I44" t="s">
+        <v>141</v>
+      </c>
       <c r="J44" t="s">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="K44" s="13">
         <v>0.5</v>
       </c>
+      <c r="L44" s="13">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>181</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -4064,7 +4112,7 @@
         <v>33</v>
       </c>
       <c r="C46" t="s">
-        <v>156</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -4072,7 +4120,7 @@
         <v>0.5</v>
       </c>
       <c r="C47" s="13">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -4116,7 +4164,7 @@
         <v>2030</v>
       </c>
       <c r="P48" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -4173,55 +4221,55 @@
       </c>
       <c r="C50" s="14">
         <f>B50*$C$47</f>
-        <v>227.7</v>
+        <v>303.60000000000002</v>
       </c>
       <c r="D50" s="14">
         <f>C50*(1+$B$47)</f>
-        <v>341.54999999999995</v>
+        <v>455.40000000000003</v>
       </c>
       <c r="E50" s="20">
-        <f t="shared" ref="E50:H50" si="3">D50*(1+$B$47)</f>
-        <v>512.32499999999993</v>
+        <f t="shared" ref="E50:H50" si="12">D50*(1+$B$47)</f>
+        <v>683.1</v>
       </c>
       <c r="F50" s="14">
-        <f t="shared" si="3"/>
-        <v>768.48749999999995</v>
+        <f t="shared" si="12"/>
+        <v>1024.6500000000001</v>
       </c>
       <c r="G50" s="14">
-        <f t="shared" si="3"/>
-        <v>1152.7312499999998</v>
+        <f t="shared" si="12"/>
+        <v>1536.9750000000001</v>
       </c>
       <c r="H50" s="14">
-        <f t="shared" si="3"/>
-        <v>1729.0968749999997</v>
+        <f t="shared" si="12"/>
+        <v>2305.4625000000001</v>
       </c>
       <c r="I50" s="14">
-        <f t="shared" ref="I50" si="4">H50*(1+$B$47)</f>
-        <v>2593.6453124999998</v>
+        <f t="shared" ref="I50" si="13">H50*(1+$B$47)</f>
+        <v>3458.1937500000004</v>
       </c>
       <c r="J50" s="14">
-        <f t="shared" ref="J50" si="5">I50*(1+$B$47)</f>
-        <v>3890.4679687499997</v>
+        <f t="shared" ref="J50" si="14">I50*(1+$B$47)</f>
+        <v>5187.2906250000005</v>
       </c>
       <c r="K50" s="14">
-        <f t="shared" ref="K50" si="6">J50*(1+$B$47)</f>
-        <v>5835.7019531249998</v>
+        <f t="shared" ref="K50" si="15">J50*(1+$B$47)</f>
+        <v>7780.9359375000004</v>
       </c>
       <c r="L50" s="14">
-        <f t="shared" ref="L50" si="7">K50*(1+$B$47)</f>
-        <v>8753.5529296874993</v>
+        <f t="shared" ref="L50" si="16">K50*(1+$B$47)</f>
+        <v>11671.403906250001</v>
       </c>
       <c r="M50" s="14">
-        <f t="shared" ref="M50" si="8">L50*(1+$B$47)</f>
-        <v>13130.329394531249</v>
+        <f t="shared" ref="M50" si="17">L50*(1+$B$47)</f>
+        <v>17507.105859375002</v>
       </c>
       <c r="N50" s="14">
-        <f t="shared" ref="N50" si="9">M50*(1+$B$47)</f>
-        <v>19695.494091796874</v>
+        <f t="shared" ref="N50" si="18">M50*(1+$B$47)</f>
+        <v>26260.658789062501</v>
       </c>
       <c r="O50" s="31">
         <f>N50*(1+$B$47)</f>
-        <v>29543.24113769531</v>
+        <v>39390.988183593756</v>
       </c>
       <c r="P50" s="15">
         <f>C35+C34</f>
@@ -4238,55 +4286,55 @@
       </c>
       <c r="C51" s="14">
         <f>B51*$C$47</f>
-        <v>79.5</v>
+        <v>106</v>
       </c>
       <c r="D51" s="14">
-        <f t="shared" ref="D51:L51" si="10">C51*(1+$B$47)</f>
-        <v>119.25</v>
+        <f t="shared" ref="D51:L51" si="19">C51*(1+$B$47)</f>
+        <v>159</v>
       </c>
       <c r="E51" s="20">
-        <f t="shared" si="10"/>
-        <v>178.875</v>
+        <f t="shared" si="19"/>
+        <v>238.5</v>
       </c>
       <c r="F51" s="14">
-        <f t="shared" si="10"/>
-        <v>268.3125</v>
+        <f t="shared" si="19"/>
+        <v>357.75</v>
       </c>
       <c r="G51" s="14">
-        <f t="shared" si="10"/>
-        <v>402.46875</v>
+        <f t="shared" si="19"/>
+        <v>536.625</v>
       </c>
       <c r="H51" s="14">
-        <f t="shared" si="10"/>
-        <v>603.703125</v>
+        <f t="shared" si="19"/>
+        <v>804.9375</v>
       </c>
       <c r="I51" s="14">
-        <f t="shared" si="10"/>
-        <v>905.5546875</v>
+        <f t="shared" si="19"/>
+        <v>1207.40625</v>
       </c>
       <c r="J51" s="14">
-        <f t="shared" si="10"/>
-        <v>1358.33203125</v>
+        <f t="shared" si="19"/>
+        <v>1811.109375</v>
       </c>
       <c r="K51" s="14">
-        <f t="shared" si="10"/>
-        <v>2037.498046875</v>
+        <f t="shared" si="19"/>
+        <v>2716.6640625</v>
       </c>
       <c r="L51" s="14">
-        <f t="shared" si="10"/>
-        <v>3056.2470703125</v>
+        <f t="shared" si="19"/>
+        <v>4074.99609375</v>
       </c>
       <c r="M51" s="14">
-        <f t="shared" ref="M51:M53" si="11">L51*(1+$B$47)</f>
-        <v>4584.37060546875</v>
+        <f t="shared" ref="M51:M53" si="20">L51*(1+$B$47)</f>
+        <v>6112.494140625</v>
       </c>
       <c r="N51" s="14">
-        <f t="shared" ref="N51:N53" si="12">M51*(1+$B$47)</f>
-        <v>6876.555908203125</v>
+        <f t="shared" ref="N51:N53" si="21">M51*(1+$B$47)</f>
+        <v>9168.7412109375</v>
       </c>
       <c r="O51" s="31">
-        <f t="shared" ref="O51:O53" si="13">N51*(1+$B$47)</f>
-        <v>10314.833862304688</v>
+        <f t="shared" ref="O51:O53" si="22">N51*(1+$B$47)</f>
+        <v>13753.11181640625</v>
       </c>
       <c r="P51" s="15">
         <f>C33+C32</f>
@@ -4303,55 +4351,55 @@
       </c>
       <c r="C52" s="14">
         <f>B52*$C$47</f>
-        <v>2480.85</v>
+        <v>3307.8</v>
       </c>
       <c r="D52" s="14">
         <f>C52*(1+$B$47)</f>
-        <v>3721.2749999999996</v>
+        <v>4961.7000000000007</v>
       </c>
       <c r="E52" s="20">
-        <f t="shared" ref="E52:L52" si="14">D52*(1+$B$47)</f>
-        <v>5581.9124999999995</v>
+        <f t="shared" ref="E52:L52" si="23">D52*(1+$B$47)</f>
+        <v>7442.5500000000011</v>
       </c>
       <c r="F52" s="14">
-        <f t="shared" si="14"/>
-        <v>8372.8687499999996</v>
+        <f t="shared" si="23"/>
+        <v>11163.825000000001</v>
       </c>
       <c r="G52" s="14">
-        <f t="shared" si="14"/>
-        <v>12559.303124999999</v>
+        <f t="shared" si="23"/>
+        <v>16745.737500000003</v>
       </c>
       <c r="H52" s="14">
-        <f t="shared" si="14"/>
-        <v>18838.954687499998</v>
+        <f t="shared" si="23"/>
+        <v>25118.606250000004</v>
       </c>
       <c r="I52" s="14">
-        <f t="shared" si="14"/>
-        <v>28258.432031249999</v>
+        <f t="shared" si="23"/>
+        <v>37677.909375000003</v>
       </c>
       <c r="J52" s="14">
-        <f t="shared" si="14"/>
-        <v>42387.648046874994</v>
+        <f t="shared" si="23"/>
+        <v>56516.864062500004</v>
       </c>
       <c r="K52" s="14">
-        <f t="shared" si="14"/>
-        <v>63581.472070312491</v>
+        <f t="shared" si="23"/>
+        <v>84775.296093750003</v>
       </c>
       <c r="L52" s="14">
-        <f t="shared" si="14"/>
-        <v>95372.208105468744</v>
+        <f t="shared" si="23"/>
+        <v>127162.94414062501</v>
       </c>
       <c r="M52" s="14">
-        <f t="shared" si="11"/>
-        <v>143058.3121582031</v>
+        <f t="shared" si="20"/>
+        <v>190744.41621093752</v>
       </c>
       <c r="N52" s="14">
-        <f t="shared" si="12"/>
-        <v>214587.46823730465</v>
+        <f t="shared" si="21"/>
+        <v>286116.62431640626</v>
       </c>
       <c r="O52" s="31">
-        <f t="shared" si="13"/>
-        <v>321881.20235595701</v>
+        <f t="shared" si="22"/>
+        <v>429174.93647460942</v>
       </c>
       <c r="P52" s="15">
         <f>C31+C30</f>
@@ -4368,55 +4416,55 @@
       </c>
       <c r="C53" s="14">
         <f>B53*$C$47</f>
-        <v>18168.149999999998</v>
+        <v>24224.2</v>
       </c>
       <c r="D53" s="14">
-        <f t="shared" ref="D53:L53" si="15">C53*(1+$B$47)</f>
-        <v>27252.224999999999</v>
+        <f t="shared" ref="D53:L53" si="24">C53*(1+$B$47)</f>
+        <v>36336.300000000003</v>
       </c>
       <c r="E53" s="20">
-        <f t="shared" si="15"/>
-        <v>40878.337499999994</v>
+        <f t="shared" si="24"/>
+        <v>54504.450000000004</v>
       </c>
       <c r="F53" s="14">
-        <f t="shared" si="15"/>
-        <v>61317.506249999991</v>
+        <f t="shared" si="24"/>
+        <v>81756.675000000003</v>
       </c>
       <c r="G53" s="14">
-        <f t="shared" si="15"/>
-        <v>91976.259374999994</v>
+        <f t="shared" si="24"/>
+        <v>122635.01250000001</v>
       </c>
       <c r="H53" s="14">
-        <f t="shared" si="15"/>
-        <v>137964.38906249998</v>
+        <f t="shared" si="24"/>
+        <v>183952.51875000002</v>
       </c>
       <c r="I53" s="14">
-        <f t="shared" si="15"/>
-        <v>206946.58359374997</v>
+        <f t="shared" si="24"/>
+        <v>275928.77812500001</v>
       </c>
       <c r="J53" s="14">
-        <f t="shared" si="15"/>
-        <v>310419.87539062498</v>
+        <f t="shared" si="24"/>
+        <v>413893.16718750005</v>
       </c>
       <c r="K53" s="14">
-        <f t="shared" si="15"/>
-        <v>465629.81308593747</v>
+        <f t="shared" si="24"/>
+        <v>620839.75078125007</v>
       </c>
       <c r="L53" s="14">
-        <f t="shared" si="15"/>
-        <v>698444.71962890623</v>
+        <f t="shared" si="24"/>
+        <v>931259.62617187505</v>
       </c>
       <c r="M53" s="14">
-        <f t="shared" si="11"/>
-        <v>1047667.0794433593</v>
+        <f t="shared" si="20"/>
+        <v>1396889.4392578127</v>
       </c>
       <c r="N53" s="14">
-        <f t="shared" si="12"/>
-        <v>1571500.6191650389</v>
+        <f t="shared" si="21"/>
+        <v>2095334.158886719</v>
       </c>
       <c r="O53" s="31">
-        <f t="shared" si="13"/>
-        <v>2357250.9287475585</v>
+        <f t="shared" si="22"/>
+        <v>3143001.2383300783</v>
       </c>
       <c r="P53" s="15">
         <f>C36</f>
@@ -4437,7 +4485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5F46D0-BFBE-459D-AD94-C3EBC85EC70F}">
   <dimension ref="A2:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -4555,11 +4603,11 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
       <c r="H6" s="2">
         <v>2018</v>
@@ -4596,11 +4644,11 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>170</v>
+        <v>134</v>
       </c>
       <c r="H7" s="2">
         <v>2018</v>
@@ -4685,10 +4733,10 @@
         <v>8</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>192</v>
+        <v>153</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>193</v>
+        <v>154</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>43</v>
@@ -4706,14 +4754,14 @@
         <v>UC_SRV_MaxGrowth_Biomass</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>191</v>
+        <v>152</v>
       </c>
       <c r="D11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>185</v>
+        <v>146</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="H11" s="2">
         <v>2018</v>
@@ -4746,14 +4794,14 @@
         <v>UC_SRV_MaxGrowth_Biogas</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>191</v>
+        <v>152</v>
       </c>
       <c r="D12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>186</v>
+        <v>147</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="H12" s="2">
         <v>2018</v>
@@ -4782,18 +4830,18 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="D14" t="s">
-        <v>155</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>130</v>
       </c>
       <c r="B15" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
       <c r="C15" s="13">
         <v>0.05</v>
@@ -4804,10 +4852,10 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>167</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
       <c r="C16" s="13">
         <v>0.05</v>
@@ -4818,10 +4866,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>184</v>
+        <v>145</v>
       </c>
       <c r="B17" t="s">
-        <v>182</v>
+        <v>143</v>
       </c>
       <c r="C17" s="13">
         <v>0.05</v>
@@ -4832,10 +4880,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>184</v>
+        <v>145</v>
       </c>
       <c r="B18" t="s">
-        <v>183</v>
+        <v>144</v>
       </c>
       <c r="C18" s="13">
         <v>0.05</v>

</xml_diff>

<commit_message>
Reactivate BEV growth constraint
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB2D5AF-0627-4C6D-B5E7-F6A47FBF6647}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF98D62-AB3E-4693-BA8A-F2DB9F3886FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -593,7 +593,7 @@
     <t>On/Off</t>
   </si>
   <si>
-    <t>*</t>
+    <t>Seed Value</t>
   </si>
 </sst>
 </file>
@@ -2823,7 +2823,7 @@
   <dimension ref="A2:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2832,12 +2832,12 @@
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.5703125" customWidth="1"/>
-    <col min="14" max="14" width="34" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" customWidth="1"/>
     <col min="15" max="15" width="10.7109375" customWidth="1"/>
     <col min="16" max="16" width="11.140625" customWidth="1"/>
   </cols>
@@ -2941,7 +2941,7 @@
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="str">
         <f t="shared" ref="B6:B23" si="0">IF(H27="*","*",_xlfn.TEXTJOIN("",TRUE,"UC-",I27,"_MaxGrowth",J27))</f>
-        <v>*</v>
+        <v>UC-CAR_MaxGrowthBEV</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>13</v>
@@ -2968,14 +2968,14 @@
         <v>1</v>
       </c>
       <c r="L6" s="19">
-        <f>-C53/1000</f>
+        <f t="shared" ref="L6:L9" si="2">-$B$53*L27/1000</f>
         <v>-18.168149999999997</v>
       </c>
       <c r="M6" s="18">
         <v>5</v>
       </c>
       <c r="N6" s="18" t="str">
-        <f t="shared" ref="N6:N23" si="2">_xlfn.TEXTJOIN(" ", TRUE,I27&amp;"s","maximum growth rate of",J27&amp;"s")</f>
+        <f t="shared" ref="N6:N23" si="3">_xlfn.TEXTJOIN(" ", TRUE,I27&amp;"s","maximum growth rate of",J27&amp;"s")</f>
         <v>CARs maximum growth rate of BEVs</v>
       </c>
     </row>
@@ -3009,14 +3009,14 @@
         <v>1</v>
       </c>
       <c r="L7" s="19">
-        <f>-C53/1000</f>
+        <f t="shared" si="2"/>
         <v>-18.168149999999997</v>
       </c>
       <c r="M7" s="18">
         <v>5</v>
       </c>
       <c r="N7" s="18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>CARs maximum growth rate of PHEVs</v>
       </c>
     </row>
@@ -3050,14 +3050,14 @@
         <v>1</v>
       </c>
       <c r="L8" s="19">
-        <f>-C53/1000</f>
+        <f t="shared" si="2"/>
         <v>-18.168149999999997</v>
       </c>
       <c r="M8" s="18">
         <v>5</v>
       </c>
       <c r="N8" s="18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>CARs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
@@ -3091,14 +3091,14 @@
         <v>1</v>
       </c>
       <c r="L9" s="22">
-        <f>-C53/1000</f>
+        <f t="shared" ref="L9:L10" si="4">-$B$53*L30/1000</f>
         <v>-18.168149999999997</v>
       </c>
       <c r="M9" s="21">
         <v>5</v>
       </c>
       <c r="N9" s="21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>CARs maximum growth rate of FCVs</v>
       </c>
     </row>
@@ -3132,14 +3132,14 @@
         <v>1</v>
       </c>
       <c r="L10" s="19">
-        <f>-C52/1000</f>
+        <f t="shared" ref="L10:L13" si="5">-$B$52*L31/1000</f>
         <v>-2.4808499999999998</v>
       </c>
       <c r="M10" s="18">
         <v>5</v>
       </c>
       <c r="N10" s="18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>LGTs maximum growth rate of BEVs</v>
       </c>
     </row>
@@ -3173,14 +3173,14 @@
         <v>1</v>
       </c>
       <c r="L11" s="19">
-        <f>-C52/1000</f>
+        <f t="shared" si="5"/>
         <v>-2.4808499999999998</v>
       </c>
       <c r="M11" s="18">
         <v>5</v>
       </c>
       <c r="N11" s="18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>LGTs maximum growth rate of PHEVs</v>
       </c>
     </row>
@@ -3214,14 +3214,14 @@
         <v>1</v>
       </c>
       <c r="L12" s="19">
-        <f>-C52/1000</f>
+        <f t="shared" si="5"/>
         <v>-2.4808499999999998</v>
       </c>
       <c r="M12" s="18">
         <v>5</v>
       </c>
       <c r="N12" s="18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>LGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
@@ -3255,14 +3255,14 @@
         <v>1</v>
       </c>
       <c r="L13" s="22">
-        <f>-C52/1000</f>
+        <f t="shared" ref="L13:L14" si="6">-$B$52*L34/1000</f>
         <v>-2.4808499999999998</v>
       </c>
       <c r="M13" s="21">
         <v>5</v>
       </c>
       <c r="N13" s="21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>LGTs maximum growth rate of FCVs</v>
       </c>
     </row>
@@ -3296,14 +3296,14 @@
         <v>1</v>
       </c>
       <c r="L14" s="19">
-        <f>-C51/1000</f>
+        <f t="shared" ref="L14:L18" si="7">-$B$51*L35/1000</f>
         <v>-7.9500000000000001E-2</v>
       </c>
       <c r="M14" s="18">
         <v>5</v>
       </c>
       <c r="N14" s="18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>MGTs maximum growth rate of BEVs</v>
       </c>
     </row>
@@ -3337,14 +3337,14 @@
         <v>1</v>
       </c>
       <c r="L15" s="19">
-        <f>-C51/1000</f>
+        <f t="shared" si="7"/>
         <v>-7.9500000000000001E-2</v>
       </c>
       <c r="M15" s="18">
         <v>5</v>
       </c>
       <c r="N15" s="18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>MGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
@@ -3378,14 +3378,14 @@
         <v>1</v>
       </c>
       <c r="L16" s="19">
-        <f>-C51/1000</f>
+        <f t="shared" si="7"/>
         <v>-7.9500000000000001E-2</v>
       </c>
       <c r="M16" s="18">
         <v>5</v>
       </c>
       <c r="N16" s="18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>MGTs maximum growth rate of LNG-ICEs</v>
       </c>
     </row>
@@ -3419,14 +3419,14 @@
         <v>1</v>
       </c>
       <c r="L17" s="19">
-        <f>-C51/1000</f>
+        <f t="shared" si="7"/>
         <v>-7.9500000000000001E-2</v>
       </c>
       <c r="M17" s="18">
         <v>5</v>
       </c>
       <c r="N17" s="18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>MGTs maximum growth rate of HEVs</v>
       </c>
     </row>
@@ -3460,14 +3460,14 @@
         <v>1</v>
       </c>
       <c r="L18" s="22">
-        <f>-C51/1000</f>
+        <f t="shared" ref="L18:L19" si="8">-$B$51*L39/1000</f>
         <v>-7.9500000000000001E-2</v>
       </c>
       <c r="M18" s="21">
         <v>5</v>
       </c>
       <c r="N18" s="21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>MGTs maximum growth rate of FCVs</v>
       </c>
     </row>
@@ -3501,14 +3501,14 @@
         <v>1</v>
       </c>
       <c r="L19" s="19">
-        <f>-C50/1000</f>
+        <f t="shared" ref="L19:L23" si="9">-$B$50*L40/1000</f>
         <v>-0.22769999999999999</v>
       </c>
       <c r="M19" s="18">
         <v>5</v>
       </c>
       <c r="N19" s="18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HGTs maximum growth rate of BEVs</v>
       </c>
     </row>
@@ -3542,14 +3542,14 @@
         <v>1</v>
       </c>
       <c r="L20" s="19">
-        <f>-C50/1000</f>
+        <f t="shared" si="9"/>
         <v>-0.22769999999999999</v>
       </c>
       <c r="M20" s="18">
         <v>5</v>
       </c>
       <c r="N20" s="18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
@@ -3583,14 +3583,14 @@
         <v>1</v>
       </c>
       <c r="L21" s="19">
-        <f>-C50/1000</f>
+        <f t="shared" si="9"/>
         <v>-0.22769999999999999</v>
       </c>
       <c r="M21" s="18">
         <v>5</v>
       </c>
       <c r="N21" s="18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HGTs maximum growth rate of LNG-ICEs</v>
       </c>
     </row>
@@ -3624,14 +3624,14 @@
         <v>1</v>
       </c>
       <c r="L22" s="19">
-        <f>-C50/1000</f>
+        <f t="shared" si="9"/>
         <v>-0.22769999999999999</v>
       </c>
       <c r="M22" s="18">
         <v>5</v>
       </c>
       <c r="N22" s="18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HGTs maximum growth rate of HEVs</v>
       </c>
       <c r="O22" s="2"/>
@@ -3666,14 +3666,14 @@
         <v>1</v>
       </c>
       <c r="L23" s="22">
-        <f>-C50/1000</f>
+        <f t="shared" si="9"/>
         <v>-0.22769999999999999</v>
       </c>
       <c r="M23" s="21">
         <v>5</v>
       </c>
       <c r="N23" s="21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HGTs maximum growth rate of FCVs</v>
       </c>
     </row>
@@ -3690,11 +3690,11 @@
       <c r="K26" t="s">
         <v>117</v>
       </c>
+      <c r="L26" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H27" t="s">
-        <v>161</v>
-      </c>
       <c r="I27" t="s">
         <v>155</v>
       </c>
@@ -3703,6 +3703,9 @@
       </c>
       <c r="K27" s="13">
         <v>0.8</v>
+      </c>
+      <c r="L27" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -3717,6 +3720,9 @@
       </c>
       <c r="K28" s="13">
         <v>0.8</v>
+      </c>
+      <c r="L28" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -3740,6 +3746,9 @@
       <c r="K29" s="13">
         <v>0.5</v>
       </c>
+      <c r="L29" s="13">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="38" t="s">
@@ -3755,7 +3764,7 @@
         <v>9959</v>
       </c>
       <c r="E30" s="11">
-        <f t="shared" ref="E30:E35" si="3">D30/C30</f>
+        <f t="shared" ref="E30:E35" si="10">D30/C30</f>
         <v>4.3671013742841359E-2</v>
       </c>
       <c r="I30" t="s">
@@ -3766,6 +3775,9 @@
       </c>
       <c r="K30" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L30" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -3780,7 +3792,7 @@
         <v>6580</v>
       </c>
       <c r="E31" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>6.5375711631511485E-2</v>
       </c>
       <c r="I31" t="s">
@@ -3791,6 +3803,9 @@
       </c>
       <c r="K31" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L31" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -3805,7 +3820,7 @@
         <v>201</v>
       </c>
       <c r="E32" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>4.4214694236691596E-2</v>
       </c>
       <c r="I32" t="s">
@@ -3816,6 +3831,9 @@
       </c>
       <c r="K32" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L32" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -3830,7 +3848,7 @@
         <v>329</v>
       </c>
       <c r="E33" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>4.9391983185707852E-2</v>
       </c>
       <c r="I33" t="s">
@@ -3841,6 +3859,9 @@
       </c>
       <c r="K33" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L33" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -3855,7 +3876,7 @@
         <v>485</v>
       </c>
       <c r="E34" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>5.7573599240265907E-2</v>
       </c>
       <c r="I34" t="s">
@@ -3866,6 +3887,9 @@
       </c>
       <c r="K34" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L34" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -3880,7 +3904,7 @@
         <v>1033</v>
       </c>
       <c r="E35" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>7.187086899046824E-2</v>
       </c>
       <c r="I35" t="s">
@@ -3891,6 +3915,9 @@
       </c>
       <c r="K35" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L35" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -3916,6 +3943,9 @@
       <c r="K36" s="13">
         <v>0.5</v>
       </c>
+      <c r="L36" s="13">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
@@ -3928,7 +3958,7 @@
         <v>2566</v>
       </c>
       <c r="E37" s="11">
-        <f t="shared" ref="E37:E39" si="4">D37/C37</f>
+        <f t="shared" ref="E37:E39" si="11">D37/C37</f>
         <v>6.1874562947601935E-2</v>
       </c>
       <c r="I37" t="s">
@@ -3939,6 +3969,9 @@
       </c>
       <c r="K37" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L37" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -3952,7 +3985,7 @@
         <v>1224</v>
       </c>
       <c r="E38" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>5.7044321200540614E-2</v>
       </c>
       <c r="I38" t="s">
@@ -3963,6 +3996,9 @@
       </c>
       <c r="K38" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L38" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -3977,7 +4013,7 @@
         <v>551</v>
       </c>
       <c r="E39" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>4.9170087453150095E-2</v>
       </c>
       <c r="I39" t="s">
@@ -3988,6 +4024,9 @@
       </c>
       <c r="K39" s="13">
         <v>0.5</v>
+      </c>
+      <c r="L39" s="13">
+        <v>0.15</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -4003,6 +4042,9 @@
       <c r="K40" s="13">
         <v>0.5</v>
       </c>
+      <c r="L40" s="13">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I41" t="s">
@@ -4014,6 +4056,9 @@
       <c r="K41" s="13">
         <v>0.5</v>
       </c>
+      <c r="L41" s="13">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I42" t="s">
@@ -4025,6 +4070,9 @@
       <c r="K42" s="13">
         <v>0.5</v>
       </c>
+      <c r="L42" s="13">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I43" t="s">
@@ -4036,6 +4084,9 @@
       <c r="K43" s="13">
         <v>0.5</v>
       </c>
+      <c r="L43" s="13">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I44" t="s">
@@ -4047,6 +4098,9 @@
       <c r="K44" s="13">
         <v>0.5</v>
       </c>
+      <c r="L44" s="13">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -4066,7 +4120,7 @@
         <v>0.5</v>
       </c>
       <c r="C47" s="13">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -4167,55 +4221,55 @@
       </c>
       <c r="C50" s="14">
         <f>B50*$C$47</f>
-        <v>227.7</v>
+        <v>303.60000000000002</v>
       </c>
       <c r="D50" s="14">
         <f>C50*(1+$B$47)</f>
-        <v>341.54999999999995</v>
+        <v>455.40000000000003</v>
       </c>
       <c r="E50" s="20">
-        <f t="shared" ref="E50:H50" si="5">D50*(1+$B$47)</f>
-        <v>512.32499999999993</v>
+        <f t="shared" ref="E50:H50" si="12">D50*(1+$B$47)</f>
+        <v>683.1</v>
       </c>
       <c r="F50" s="14">
-        <f t="shared" si="5"/>
-        <v>768.48749999999995</v>
+        <f t="shared" si="12"/>
+        <v>1024.6500000000001</v>
       </c>
       <c r="G50" s="14">
-        <f t="shared" si="5"/>
-        <v>1152.7312499999998</v>
+        <f t="shared" si="12"/>
+        <v>1536.9750000000001</v>
       </c>
       <c r="H50" s="14">
-        <f t="shared" si="5"/>
-        <v>1729.0968749999997</v>
+        <f t="shared" si="12"/>
+        <v>2305.4625000000001</v>
       </c>
       <c r="I50" s="14">
-        <f t="shared" ref="I50" si="6">H50*(1+$B$47)</f>
-        <v>2593.6453124999998</v>
+        <f t="shared" ref="I50" si="13">H50*(1+$B$47)</f>
+        <v>3458.1937500000004</v>
       </c>
       <c r="J50" s="14">
-        <f t="shared" ref="J50" si="7">I50*(1+$B$47)</f>
-        <v>3890.4679687499997</v>
+        <f t="shared" ref="J50" si="14">I50*(1+$B$47)</f>
+        <v>5187.2906250000005</v>
       </c>
       <c r="K50" s="14">
-        <f t="shared" ref="K50" si="8">J50*(1+$B$47)</f>
-        <v>5835.7019531249998</v>
+        <f t="shared" ref="K50" si="15">J50*(1+$B$47)</f>
+        <v>7780.9359375000004</v>
       </c>
       <c r="L50" s="14">
-        <f t="shared" ref="L50" si="9">K50*(1+$B$47)</f>
-        <v>8753.5529296874993</v>
+        <f t="shared" ref="L50" si="16">K50*(1+$B$47)</f>
+        <v>11671.403906250001</v>
       </c>
       <c r="M50" s="14">
-        <f t="shared" ref="M50" si="10">L50*(1+$B$47)</f>
-        <v>13130.329394531249</v>
+        <f t="shared" ref="M50" si="17">L50*(1+$B$47)</f>
+        <v>17507.105859375002</v>
       </c>
       <c r="N50" s="14">
-        <f t="shared" ref="N50" si="11">M50*(1+$B$47)</f>
-        <v>19695.494091796874</v>
+        <f t="shared" ref="N50" si="18">M50*(1+$B$47)</f>
+        <v>26260.658789062501</v>
       </c>
       <c r="O50" s="31">
         <f>N50*(1+$B$47)</f>
-        <v>29543.24113769531</v>
+        <v>39390.988183593756</v>
       </c>
       <c r="P50" s="15">
         <f>C35+C34</f>
@@ -4232,55 +4286,55 @@
       </c>
       <c r="C51" s="14">
         <f>B51*$C$47</f>
-        <v>79.5</v>
+        <v>106</v>
       </c>
       <c r="D51" s="14">
-        <f t="shared" ref="D51:L51" si="12">C51*(1+$B$47)</f>
-        <v>119.25</v>
+        <f t="shared" ref="D51:L51" si="19">C51*(1+$B$47)</f>
+        <v>159</v>
       </c>
       <c r="E51" s="20">
-        <f t="shared" si="12"/>
-        <v>178.875</v>
+        <f t="shared" si="19"/>
+        <v>238.5</v>
       </c>
       <c r="F51" s="14">
-        <f t="shared" si="12"/>
-        <v>268.3125</v>
+        <f t="shared" si="19"/>
+        <v>357.75</v>
       </c>
       <c r="G51" s="14">
-        <f t="shared" si="12"/>
-        <v>402.46875</v>
+        <f t="shared" si="19"/>
+        <v>536.625</v>
       </c>
       <c r="H51" s="14">
-        <f t="shared" si="12"/>
-        <v>603.703125</v>
+        <f t="shared" si="19"/>
+        <v>804.9375</v>
       </c>
       <c r="I51" s="14">
-        <f t="shared" si="12"/>
-        <v>905.5546875</v>
+        <f t="shared" si="19"/>
+        <v>1207.40625</v>
       </c>
       <c r="J51" s="14">
-        <f t="shared" si="12"/>
-        <v>1358.33203125</v>
+        <f t="shared" si="19"/>
+        <v>1811.109375</v>
       </c>
       <c r="K51" s="14">
-        <f t="shared" si="12"/>
-        <v>2037.498046875</v>
+        <f t="shared" si="19"/>
+        <v>2716.6640625</v>
       </c>
       <c r="L51" s="14">
-        <f t="shared" si="12"/>
-        <v>3056.2470703125</v>
+        <f t="shared" si="19"/>
+        <v>4074.99609375</v>
       </c>
       <c r="M51" s="14">
-        <f t="shared" ref="M51:M53" si="13">L51*(1+$B$47)</f>
-        <v>4584.37060546875</v>
+        <f t="shared" ref="M51:M53" si="20">L51*(1+$B$47)</f>
+        <v>6112.494140625</v>
       </c>
       <c r="N51" s="14">
-        <f t="shared" ref="N51:N53" si="14">M51*(1+$B$47)</f>
-        <v>6876.555908203125</v>
+        <f t="shared" ref="N51:N53" si="21">M51*(1+$B$47)</f>
+        <v>9168.7412109375</v>
       </c>
       <c r="O51" s="31">
-        <f t="shared" ref="O51:O53" si="15">N51*(1+$B$47)</f>
-        <v>10314.833862304688</v>
+        <f t="shared" ref="O51:O53" si="22">N51*(1+$B$47)</f>
+        <v>13753.11181640625</v>
       </c>
       <c r="P51" s="15">
         <f>C33+C32</f>
@@ -4297,55 +4351,55 @@
       </c>
       <c r="C52" s="14">
         <f>B52*$C$47</f>
-        <v>2480.85</v>
+        <v>3307.8</v>
       </c>
       <c r="D52" s="14">
         <f>C52*(1+$B$47)</f>
-        <v>3721.2749999999996</v>
+        <v>4961.7000000000007</v>
       </c>
       <c r="E52" s="20">
-        <f t="shared" ref="E52:L52" si="16">D52*(1+$B$47)</f>
-        <v>5581.9124999999995</v>
+        <f t="shared" ref="E52:L52" si="23">D52*(1+$B$47)</f>
+        <v>7442.5500000000011</v>
       </c>
       <c r="F52" s="14">
-        <f t="shared" si="16"/>
-        <v>8372.8687499999996</v>
+        <f t="shared" si="23"/>
+        <v>11163.825000000001</v>
       </c>
       <c r="G52" s="14">
-        <f t="shared" si="16"/>
-        <v>12559.303124999999</v>
+        <f t="shared" si="23"/>
+        <v>16745.737500000003</v>
       </c>
       <c r="H52" s="14">
-        <f t="shared" si="16"/>
-        <v>18838.954687499998</v>
+        <f t="shared" si="23"/>
+        <v>25118.606250000004</v>
       </c>
       <c r="I52" s="14">
-        <f t="shared" si="16"/>
-        <v>28258.432031249999</v>
+        <f t="shared" si="23"/>
+        <v>37677.909375000003</v>
       </c>
       <c r="J52" s="14">
-        <f t="shared" si="16"/>
-        <v>42387.648046874994</v>
+        <f t="shared" si="23"/>
+        <v>56516.864062500004</v>
       </c>
       <c r="K52" s="14">
-        <f t="shared" si="16"/>
-        <v>63581.472070312491</v>
+        <f t="shared" si="23"/>
+        <v>84775.296093750003</v>
       </c>
       <c r="L52" s="14">
-        <f t="shared" si="16"/>
-        <v>95372.208105468744</v>
+        <f t="shared" si="23"/>
+        <v>127162.94414062501</v>
       </c>
       <c r="M52" s="14">
-        <f t="shared" si="13"/>
-        <v>143058.3121582031</v>
+        <f t="shared" si="20"/>
+        <v>190744.41621093752</v>
       </c>
       <c r="N52" s="14">
-        <f t="shared" si="14"/>
-        <v>214587.46823730465</v>
+        <f t="shared" si="21"/>
+        <v>286116.62431640626</v>
       </c>
       <c r="O52" s="31">
-        <f t="shared" si="15"/>
-        <v>321881.20235595701</v>
+        <f t="shared" si="22"/>
+        <v>429174.93647460942</v>
       </c>
       <c r="P52" s="15">
         <f>C31+C30</f>
@@ -4362,55 +4416,55 @@
       </c>
       <c r="C53" s="14">
         <f>B53*$C$47</f>
-        <v>18168.149999999998</v>
+        <v>24224.2</v>
       </c>
       <c r="D53" s="14">
-        <f t="shared" ref="D53:L53" si="17">C53*(1+$B$47)</f>
-        <v>27252.224999999999</v>
+        <f t="shared" ref="D53:L53" si="24">C53*(1+$B$47)</f>
+        <v>36336.300000000003</v>
       </c>
       <c r="E53" s="20">
-        <f t="shared" si="17"/>
-        <v>40878.337499999994</v>
+        <f t="shared" si="24"/>
+        <v>54504.450000000004</v>
       </c>
       <c r="F53" s="14">
-        <f t="shared" si="17"/>
-        <v>61317.506249999991</v>
+        <f t="shared" si="24"/>
+        <v>81756.675000000003</v>
       </c>
       <c r="G53" s="14">
-        <f t="shared" si="17"/>
-        <v>91976.259374999994</v>
+        <f t="shared" si="24"/>
+        <v>122635.01250000001</v>
       </c>
       <c r="H53" s="14">
-        <f t="shared" si="17"/>
-        <v>137964.38906249998</v>
+        <f t="shared" si="24"/>
+        <v>183952.51875000002</v>
       </c>
       <c r="I53" s="14">
-        <f t="shared" si="17"/>
-        <v>206946.58359374997</v>
+        <f t="shared" si="24"/>
+        <v>275928.77812500001</v>
       </c>
       <c r="J53" s="14">
-        <f t="shared" si="17"/>
-        <v>310419.87539062498</v>
+        <f t="shared" si="24"/>
+        <v>413893.16718750005</v>
       </c>
       <c r="K53" s="14">
-        <f t="shared" si="17"/>
-        <v>465629.81308593747</v>
+        <f t="shared" si="24"/>
+        <v>620839.75078125007</v>
       </c>
       <c r="L53" s="14">
-        <f t="shared" si="17"/>
-        <v>698444.71962890623</v>
+        <f t="shared" si="24"/>
+        <v>931259.62617187505</v>
       </c>
       <c r="M53" s="14">
-        <f t="shared" si="13"/>
-        <v>1047667.0794433593</v>
+        <f t="shared" si="20"/>
+        <v>1396889.4392578127</v>
       </c>
       <c r="N53" s="14">
-        <f t="shared" si="14"/>
-        <v>1571500.6191650389</v>
+        <f t="shared" si="21"/>
+        <v>2095334.158886719</v>
       </c>
       <c r="O53" s="31">
-        <f t="shared" si="15"/>
-        <v>2357250.9287475585</v>
+        <f t="shared" si="22"/>
+        <v>3143001.2383300783</v>
       </c>
       <c r="P53" s="15">
         <f>C36</f>
@@ -4844,12 +4898,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -5060,6 +5108,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5070,15 +5124,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5097,6 +5142,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Modify existing scenarios and define multiple parametric scenario files
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HannahD\Documents\GitHub\Irish-TIMES-model\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\TRA_VA5\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1430D98-5773-4D91-BF28-D1567031F5C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E7F6E3-6112-497D-8646-B714E89913D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="16050" windowWidth="19650" windowHeight="11070" activeTab="1" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -688,8 +688,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
@@ -874,269 +874,269 @@
   </borders>
   <cellStyleXfs count="264">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1181,12 +1181,12 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="264">
     <cellStyle name="20% - Accent5 2" xfId="10" xr:uid="{72E8C261-0B7B-4154-8B6F-C9901D88251B}"/>
@@ -1837,39 +1837,39 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5546875" customWidth="1"/>
+    <col min="25" max="25" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C3" s="23" t="str" cm="1">
         <f t="array" ref="C3">IF(LEFT(INDEX(C5:C7,$A$4),1)&lt;&gt;"*",INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
@@ -1983,12 +1983,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>80</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>82</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
         <v>84</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
         <v>86</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
         <v>88</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
         <v>90</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
         <v>92</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>94</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>96</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>98</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
         <v>100</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
         <v>102</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
         <v>104</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
         <v>106</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="27" t="s">
         <v>108</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="27" t="s">
         <v>110</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="27" t="s">
         <v>112</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="27" t="s">
         <v>114</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
         <v>116</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
         <v>118</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
         <v>120</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="27" t="s">
         <v>122</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="27" t="s">
         <v>124</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="27" t="s">
         <v>126</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="27" t="s">
         <v>128</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
         <v>130</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="27" t="s">
         <v>132</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="28" t="s">
         <v>134</v>
       </c>
@@ -2597,20 +2597,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B92B0C-7472-4C75-A119-CE0EE6C8A8E0}">
   <dimension ref="A2:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
@@ -2628,7 +2628,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2645,7 +2645,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2662,7 +2662,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A12,"MaxGrowth",B12)</f>
         <v>UC_PWR_MaxGrowth_CCS</v>
@@ -2742,7 +2742,7 @@
         <v>PWR maximum growth rate of CCS</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A13,"MaxGrowth",B13)</f>
         <v>UC_PWR_MaxGrowth_Wave</v>
@@ -2778,7 +2778,7 @@
         <v>PWR maximum growth rate of Wave</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
         <v>UC_PWR_MaxGrowth_Tidal</v>
@@ -2814,43 +2814,43 @@
         <v>PWR maximum growth rate of Tidal</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="36" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B9" s="35" t="s">
         <v>188</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36" t="s">
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35" t="s">
         <v>189</v>
       </c>
-      <c r="H9" s="36">
+      <c r="H9" s="35">
         <v>2020</v>
       </c>
-      <c r="I9" s="36" t="s">
+      <c r="I9" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="38">
+      <c r="J9" s="37">
         <v>1.2</v>
       </c>
-      <c r="K9" s="36">
+      <c r="K9" s="35">
         <v>1</v>
       </c>
-      <c r="L9" s="37">
+      <c r="L9" s="36">
         <f>L6</f>
         <v>-0.4</v>
       </c>
-      <c r="M9" s="36">
+      <c r="M9" s="35">
         <v>5</v>
       </c>
-      <c r="N9" s="36" t="s">
+      <c r="N9" s="35" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>153</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>165</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>165</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>165</v>
       </c>
@@ -2909,27 +2909,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
   <dimension ref="A2:P53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="9" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
+    <col min="9" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" customWidth="1"/>
     <col min="14" max="14" width="34" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3,Regions!E3:AD3)</f>
         <v>~UC_Sets: R_E: IE,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
@@ -2948,7 +2948,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2966,7 +2966,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2984,7 +2984,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="18" t="s">
         <v>57</v>
       </c>
@@ -3047,15 +3047,15 @@
         <v>15</v>
       </c>
       <c r="J6" s="29">
-        <f t="shared" ref="J6:J23" si="0">1+$K27</f>
+        <f>1+$K27</f>
         <v>1.8</v>
       </c>
       <c r="K6" s="18">
         <v>1</v>
       </c>
       <c r="L6" s="19">
-        <f>-C53/1000</f>
-        <v>-18.168149999999997</v>
+        <f>-D53/1000</f>
+        <v>-27.252224999999999</v>
       </c>
       <c r="M6" s="18">
         <v>5</v>
@@ -3064,7 +3064,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="18" t="s">
         <v>58</v>
       </c>
@@ -3086,15 +3086,15 @@
         <v>15</v>
       </c>
       <c r="J7" s="29">
-        <f t="shared" si="0"/>
+        <f>1+$K28</f>
         <v>1.8</v>
       </c>
       <c r="K7" s="18">
         <v>1</v>
       </c>
       <c r="L7" s="19">
-        <f>-C53/1000</f>
-        <v>-18.168149999999997</v>
+        <f>-D53/1000</f>
+        <v>-27.252224999999999</v>
       </c>
       <c r="M7" s="18">
         <v>5</v>
@@ -3103,7 +3103,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
         <v>147</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>15</v>
       </c>
       <c r="J8" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J8:J23" si="0">1+$K29</f>
         <v>1.5</v>
       </c>
       <c r="K8" s="18">
@@ -3142,7 +3142,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" s="21" t="s">
         <v>68</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
         <v>55</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" s="18" t="s">
         <v>74</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" s="18" t="s">
         <v>150</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" s="21" t="s">
         <v>75</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" s="18" t="s">
         <v>51</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" s="18" t="s">
         <v>136</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" s="18" t="s">
         <v>142</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B17" s="18" t="s">
         <v>52</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B18" s="21" t="s">
         <v>66</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B19" s="18" t="s">
         <v>47</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B20" s="18" t="s">
         <v>135</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B21" s="18" t="s">
         <v>140</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B22" s="18" t="s">
         <v>48</v>
       </c>
@@ -3689,7 +3689,7 @@
       </c>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B23" s="21" t="s">
         <v>61</v>
       </c>
@@ -3728,12 +3728,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="K26" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I27" t="s">
         <v>171</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
@@ -3755,7 +3755,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="10" t="s">
@@ -3774,8 +3774,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="38" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -3798,8 +3798,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="38"/>
       <c r="B31" s="3" t="s">
         <v>25</v>
       </c>
@@ -3823,8 +3823,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="35"/>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" s="38"/>
       <c r="B32" s="3" t="s">
         <v>24</v>
       </c>
@@ -3845,8 +3845,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" s="38"/>
       <c r="B33" s="3" t="s">
         <v>23</v>
       </c>
@@ -3867,8 +3867,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34" s="38"/>
       <c r="B34" s="3" t="s">
         <v>22</v>
       </c>
@@ -3889,8 +3889,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="35"/>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35" s="38"/>
       <c r="B35" s="3" t="s">
         <v>21</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
         <v>20</v>
       </c>
@@ -3935,7 +3935,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
         <v>19</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
         <v>18</v>
       </c>
@@ -3977,7 +3977,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
       <c r="B39" s="7" t="s">
         <v>17</v>
@@ -3999,7 +3999,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -4013,7 +4013,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J41" t="s">
         <v>174</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J42" t="s">
         <v>180</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J43" t="s">
         <v>178</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J44" t="s">
         <v>175</v>
       </c>
@@ -4045,12 +4045,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>33</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B47" s="13">
         <v>0.5</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C48">
         <v>2018</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>34</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>35</v>
       </c>
@@ -4219,7 +4219,7 @@
         <v>22797</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>11207</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -4349,7 +4349,7 @@
         <v>328695</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>38</v>
       </c>
@@ -4432,18 +4432,18 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.140625" customWidth="1"/>
-    <col min="14" max="14" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.109375" customWidth="1"/>
+    <col min="14" max="14" width="34.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
@@ -4461,7 +4461,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -4478,7 +4478,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -4495,7 +4495,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -4536,7 +4536,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A12,"MaxGrowth",B12)</f>
         <v>UC_SRV-PU_MaxGrowth_HPs</v>
@@ -4577,7 +4577,7 @@
         <v>SRV-PU maximum growth rate of HPs</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A13,"MaxGrowth",B13)</f>
         <v>UC_SRV-CS_MaxGrowth_HPs</v>
@@ -4618,7 +4618,7 @@
         <v>SRV-CS maximum growth rate of HPs</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
         <v>UC_SRV_MaxGrowth_Biomass</v>
@@ -4658,7 +4658,7 @@
         <v>SRV maximum growth rate of Biomass</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A15,"MaxGrowth",B15)</f>
         <v>UC_SRV_MaxGrowth_Biogas</v>
@@ -4698,7 +4698,7 @@
         <v>SRV maximum growth rate of Biogas</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>153</v>
       </c>
@@ -4706,7 +4706,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>166</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>167</v>
       </c>
@@ -4734,7 +4734,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>184</v>
       </c>
@@ -4748,7 +4748,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>184</v>
       </c>

</xml_diff>

<commit_message>
Add 20% growth rate constraints for WON and WOF
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF98D62-AB3E-4693-BA8A-F2DB9F3886FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7923D03F-7684-48A2-974F-97898983D37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="166">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -594,6 +594,18 @@
   </si>
   <si>
     <t>Seed Value</t>
+  </si>
+  <si>
+    <t>WON</t>
+  </si>
+  <si>
+    <t>WOF</t>
+  </si>
+  <si>
+    <t>P*WIN*ON*</t>
+  </si>
+  <si>
+    <t>P*WIN*OF*</t>
   </si>
 </sst>
 </file>
@@ -673,7 +685,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -713,6 +725,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1094,12 +1112,12 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="264">
     <cellStyle name="20% - Accent5 2" xfId="10" xr:uid="{72E8C261-0B7B-4154-8B6F-C9901D88251B}"/>
@@ -2508,10 +2526,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B92B0C-7472-4C75-A119-CE0EE6C8A8E0}">
-  <dimension ref="A2:N14"/>
+  <dimension ref="A2:N19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2520,7 +2538,7 @@
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2618,7 +2636,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A12,"MaxGrowth",B12)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
         <v>UC_PWR_MaxGrowth_CCS</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -2637,27 +2655,27 @@
         <v>15</v>
       </c>
       <c r="J6" s="32">
-        <f>1+$C12</f>
+        <f>1+$C14</f>
         <v>1.2</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
       </c>
       <c r="L6" s="33">
-        <f>-D12</f>
+        <f>-D14</f>
         <v>-0.4</v>
       </c>
       <c r="M6" s="2">
         <v>5</v>
       </c>
       <c r="N6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A12, "maximum growth rate of",B12)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A14, "maximum growth rate of",B14)</f>
         <v>PWR maximum growth rate of CCS</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A13,"MaxGrowth",B13)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A15,"MaxGrowth",B15)</f>
         <v>UC_PWR_MaxGrowth_Wave</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -2673,27 +2691,27 @@
         <v>15</v>
       </c>
       <c r="J7" s="32">
-        <f>1+$C13</f>
+        <f>1+$C15</f>
         <v>1.2</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
       </c>
       <c r="L7" s="33">
-        <f t="shared" ref="L7:L8" si="0">-D13</f>
+        <f t="shared" ref="L7:L8" si="0">-D15</f>
         <v>-0.4</v>
       </c>
       <c r="M7" s="2">
         <v>5</v>
       </c>
       <c r="N7" s="2" t="str">
-        <f t="shared" ref="N7:N8" si="1">_xlfn.TEXTJOIN(" ",TRUE,A13, "maximum growth rate of",B13)</f>
+        <f t="shared" ref="N7:N8" si="1">_xlfn.TEXTJOIN(" ",TRUE,A15, "maximum growth rate of",B15)</f>
         <v>PWR maximum growth rate of Wave</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A16,"MaxGrowth",B16)</f>
         <v>UC_PWR_MaxGrowth_Tidal</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -2709,7 +2727,7 @@
         <v>15</v>
       </c>
       <c r="J8" s="32">
-        <f>1+$C14</f>
+        <f>1+$C16</f>
         <v>1.2</v>
       </c>
       <c r="K8" s="2">
@@ -2728,75 +2746,119 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35" t="s">
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="H9" s="35">
+      <c r="H9" s="36">
         <v>2020</v>
       </c>
-      <c r="I9" s="35" t="s">
+      <c r="I9" s="36" t="s">
         <v>15</v>
       </c>
       <c r="J9" s="37">
         <v>1.2</v>
       </c>
-      <c r="K9" s="35">
+      <c r="K9" s="36">
         <v>1</v>
       </c>
-      <c r="L9" s="36">
+      <c r="L9" s="38">
         <f>L6</f>
         <v>-0.4</v>
       </c>
-      <c r="M9" s="35">
+      <c r="M9" s="36">
         <v>5</v>
       </c>
-      <c r="N9" s="35" t="s">
+      <c r="N9" s="36" t="s">
         <v>151</v>
       </c>
     </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
+        <v>UC_PWR_MaxGrowth_WON</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H10">
+        <v>2018</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="32">
+        <f>1+$C18</f>
+        <v>1.2</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10" s="33">
+        <f t="shared" ref="L10" si="2">-D18</f>
+        <v>-0.5</v>
+      </c>
+      <c r="M10" s="2">
+        <v>5</v>
+      </c>
+      <c r="N10" s="2" t="str">
+        <f t="shared" ref="N10" si="3">_xlfn.TEXTJOIN(" ",TRUE,A18, "maximum growth rate of",B18)</f>
+        <v>PWR maximum growth rate of WON</v>
+      </c>
+    </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+      <c r="B11" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A19,"MaxGrowth",B19)</f>
+        <v>UC_PWR_MaxGrowth_WOF</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="H11">
+        <v>2018</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="32">
+        <f>1+$C19</f>
+        <v>1.2</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1</v>
+      </c>
+      <c r="L11" s="33">
+        <f t="shared" ref="L11" si="4">-D19</f>
+        <v>-0.5</v>
+      </c>
+      <c r="M11" s="2">
+        <v>5</v>
+      </c>
+      <c r="N11" s="2" t="str">
+        <f t="shared" ref="N11" si="5">_xlfn.TEXTJOIN(" ",TRUE,A19, "maximum growth rate of",B19)</f>
+        <v>PWR maximum growth rate of WOF</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
         <v>117</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D13" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>129</v>
-      </c>
-      <c r="B12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C12" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="D12">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>129</v>
-      </c>
-      <c r="B13" t="s">
-        <v>125</v>
-      </c>
-      <c r="C13" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="D13">
-        <v>0.4</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2804,13 +2866,72 @@
         <v>129</v>
       </c>
       <c r="B14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C14" s="13">
         <v>0.2</v>
       </c>
       <c r="D14">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D15">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D16">
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="13"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" t="s">
+        <v>163</v>
+      </c>
+      <c r="C19" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D19">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -2822,8 +2943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
   <dimension ref="A2:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2968,7 +3089,7 @@
         <v>1</v>
       </c>
       <c r="L6" s="19">
-        <f t="shared" ref="L6:L9" si="2">-$B$53*L27/1000</f>
+        <f t="shared" ref="L6:L8" si="2">-$B$53*L27/1000</f>
         <v>-18.168149999999997</v>
       </c>
       <c r="M6" s="18">
@@ -3091,7 +3212,7 @@
         <v>1</v>
       </c>
       <c r="L9" s="22">
-        <f t="shared" ref="L9:L10" si="4">-$B$53*L30/1000</f>
+        <f t="shared" ref="L9" si="4">-$B$53*L30/1000</f>
         <v>-18.168149999999997</v>
       </c>
       <c r="M9" s="21">
@@ -3132,7 +3253,7 @@
         <v>1</v>
       </c>
       <c r="L10" s="19">
-        <f t="shared" ref="L10:L13" si="5">-$B$52*L31/1000</f>
+        <f t="shared" ref="L10:L12" si="5">-$B$52*L31/1000</f>
         <v>-2.4808499999999998</v>
       </c>
       <c r="M10" s="18">
@@ -3255,7 +3376,7 @@
         <v>1</v>
       </c>
       <c r="L13" s="22">
-        <f t="shared" ref="L13:L14" si="6">-$B$52*L34/1000</f>
+        <f t="shared" ref="L13" si="6">-$B$52*L34/1000</f>
         <v>-2.4808499999999998</v>
       </c>
       <c r="M13" s="21">
@@ -3296,7 +3417,7 @@
         <v>1</v>
       </c>
       <c r="L14" s="19">
-        <f t="shared" ref="L14:L18" si="7">-$B$51*L35/1000</f>
+        <f t="shared" ref="L14:L17" si="7">-$B$51*L35/1000</f>
         <v>-7.9500000000000001E-2</v>
       </c>
       <c r="M14" s="18">
@@ -3460,7 +3581,7 @@
         <v>1</v>
       </c>
       <c r="L18" s="22">
-        <f t="shared" ref="L18:L19" si="8">-$B$51*L39/1000</f>
+        <f t="shared" ref="L18" si="8">-$B$51*L39/1000</f>
         <v>-7.9500000000000001E-2</v>
       </c>
       <c r="M18" s="21">
@@ -3751,7 +3872,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="35" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -3781,7 +3902,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="38"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="3" t="s">
         <v>25</v>
       </c>
@@ -3809,7 +3930,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="38"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="3" t="s">
         <v>24</v>
       </c>
@@ -3837,7 +3958,7 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="38"/>
+      <c r="A33" s="35"/>
       <c r="B33" s="3" t="s">
         <v>23</v>
       </c>
@@ -3865,7 +3986,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
+      <c r="A34" s="35"/>
       <c r="B34" s="3" t="s">
         <v>22</v>
       </c>
@@ -3893,7 +4014,7 @@
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="38"/>
+      <c r="A35" s="35"/>
       <c r="B35" s="3" t="s">
         <v>21</v>
       </c>
@@ -4898,6 +5019,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -5108,12 +5235,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5124,6 +5245,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5142,15 +5272,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Add 20% growth rate constraints for PV and CSP
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7923D03F-7684-48A2-974F-97898983D37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7612DDC-F2A0-41A5-8C2D-2D6405E0F784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="170">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -606,6 +606,18 @@
   </si>
   <si>
     <t>P*WIN*OF*</t>
+  </si>
+  <si>
+    <t>PV</t>
+  </si>
+  <si>
+    <t>CSP</t>
+  </si>
+  <si>
+    <t>P*SOL*PV*</t>
+  </si>
+  <si>
+    <t>P*SOL*CSP*</t>
   </si>
 </sst>
 </file>
@@ -1112,12 +1124,12 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="264">
     <cellStyle name="20% - Accent5 2" xfId="10" xr:uid="{72E8C261-0B7B-4154-8B6F-C9901D88251B}"/>
@@ -2526,10 +2538,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B92B0C-7472-4C75-A119-CE0EE6C8A8E0}">
-  <dimension ref="A2:N19"/>
+  <dimension ref="A2:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2636,7 +2648,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A16,"MaxGrowth",B16)</f>
         <v>UC_PWR_MaxGrowth_CCS</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -2655,27 +2667,27 @@
         <v>15</v>
       </c>
       <c r="J6" s="32">
-        <f>1+$C14</f>
+        <f>1+$C16</f>
         <v>1.2</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
       </c>
       <c r="L6" s="33">
-        <f>-D14</f>
+        <f>-D16</f>
         <v>-0.4</v>
       </c>
       <c r="M6" s="2">
         <v>5</v>
       </c>
       <c r="N6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A14, "maximum growth rate of",B14)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A16, "maximum growth rate of",B16)</f>
         <v>PWR maximum growth rate of CCS</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A15,"MaxGrowth",B15)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A17,"MaxGrowth",B17)</f>
         <v>UC_PWR_MaxGrowth_Wave</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -2691,27 +2703,27 @@
         <v>15</v>
       </c>
       <c r="J7" s="32">
-        <f>1+$C15</f>
+        <f>1+$C17</f>
         <v>1.2</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
       </c>
       <c r="L7" s="33">
-        <f t="shared" ref="L7:L8" si="0">-D15</f>
+        <f t="shared" ref="L7:L8" si="0">-D17</f>
         <v>-0.4</v>
       </c>
       <c r="M7" s="2">
         <v>5</v>
       </c>
       <c r="N7" s="2" t="str">
-        <f t="shared" ref="N7:N8" si="1">_xlfn.TEXTJOIN(" ",TRUE,A15, "maximum growth rate of",B15)</f>
+        <f t="shared" ref="N7:N8" si="1">_xlfn.TEXTJOIN(" ",TRUE,A17, "maximum growth rate of",B17)</f>
         <v>PWR maximum growth rate of Wave</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A16,"MaxGrowth",B16)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
         <v>UC_PWR_MaxGrowth_Tidal</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -2727,7 +2739,7 @@
         <v>15</v>
       </c>
       <c r="J8" s="32">
-        <f>1+$C16</f>
+        <f>1+$C18</f>
         <v>1.2</v>
       </c>
       <c r="K8" s="2">
@@ -2746,44 +2758,44 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36" t="s">
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="H9" s="36">
+      <c r="H9" s="35">
         <v>2020</v>
       </c>
-      <c r="I9" s="36" t="s">
+      <c r="I9" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="37">
+      <c r="J9" s="36">
         <v>1.2</v>
       </c>
-      <c r="K9" s="36">
+      <c r="K9" s="35">
         <v>1</v>
       </c>
-      <c r="L9" s="38">
+      <c r="L9" s="37">
         <f>L6</f>
         <v>-0.4</v>
       </c>
-      <c r="M9" s="36">
+      <c r="M9" s="35">
         <v>5</v>
       </c>
-      <c r="N9" s="36" t="s">
+      <c r="N9" s="35" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A20,"MaxGrowth",B20)</f>
         <v>UC_PWR_MaxGrowth_WON</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -2799,27 +2811,27 @@
         <v>15</v>
       </c>
       <c r="J10" s="32">
-        <f>1+$C18</f>
+        <f>1+$C20</f>
         <v>1.2</v>
       </c>
       <c r="K10" s="2">
         <v>1</v>
       </c>
       <c r="L10" s="33">
-        <f t="shared" ref="L10" si="2">-D18</f>
+        <f t="shared" ref="L10" si="2">-D20</f>
         <v>-0.5</v>
       </c>
       <c r="M10" s="2">
         <v>5</v>
       </c>
       <c r="N10" s="2" t="str">
-        <f t="shared" ref="N10" si="3">_xlfn.TEXTJOIN(" ",TRUE,A18, "maximum growth rate of",B18)</f>
+        <f t="shared" ref="N10" si="3">_xlfn.TEXTJOIN(" ",TRUE,A20, "maximum growth rate of",B20)</f>
         <v>PWR maximum growth rate of WON</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A19,"MaxGrowth",B19)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A21,"MaxGrowth",B21)</f>
         <v>UC_PWR_MaxGrowth_WOF</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -2835,58 +2847,102 @@
         <v>15</v>
       </c>
       <c r="J11" s="32">
-        <f>1+$C19</f>
+        <f>1+$C21</f>
         <v>1.2</v>
       </c>
       <c r="K11" s="2">
         <v>1</v>
       </c>
       <c r="L11" s="33">
-        <f t="shared" ref="L11" si="4">-D19</f>
+        <f t="shared" ref="L11" si="4">-D21</f>
         <v>-0.5</v>
       </c>
       <c r="M11" s="2">
         <v>5</v>
       </c>
       <c r="N11" s="2" t="str">
-        <f t="shared" ref="N11" si="5">_xlfn.TEXTJOIN(" ",TRUE,A19, "maximum growth rate of",B19)</f>
+        <f t="shared" ref="N11" si="5">_xlfn.TEXTJOIN(" ",TRUE,A21, "maximum growth rate of",B21)</f>
         <v>PWR maximum growth rate of WOF</v>
       </c>
     </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="str">
+        <f t="shared" ref="B12:B13" si="6">_xlfn.TEXTJOIN("_",TRUE,"UC",A22,"MaxGrowth",B22)</f>
+        <v>UC_PWR_MaxGrowth_PV</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H12">
+        <v>2018</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="32">
+        <f t="shared" ref="J12:J13" si="7">1+$C22</f>
+        <v>1.2</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+      <c r="L12" s="33">
+        <f t="shared" ref="L12:L13" si="8">-D22</f>
+        <v>-0.5</v>
+      </c>
+      <c r="M12" s="2">
+        <v>5</v>
+      </c>
+      <c r="N12" s="2" t="str">
+        <f t="shared" ref="N12:N13" si="9">_xlfn.TEXTJOIN(" ",TRUE,A22, "maximum growth rate of",B22)</f>
+        <v>PWR maximum growth rate of PV</v>
+      </c>
+    </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+      <c r="B13" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>UC_PWR_MaxGrowth_CSP</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H13">
+        <v>2018</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="32">
+        <f t="shared" si="7"/>
+        <v>1.2</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1</v>
+      </c>
+      <c r="L13" s="33">
+        <f t="shared" si="8"/>
+        <v>-0.5</v>
+      </c>
+      <c r="M13" s="2">
+        <v>5</v>
+      </c>
+      <c r="N13" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>PWR maximum growth rate of CSP</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>117</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>129</v>
-      </c>
-      <c r="B14" t="s">
-        <v>124</v>
-      </c>
-      <c r="C14" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="D14">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>129</v>
-      </c>
-      <c r="B15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C15" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="D15">
-        <v>0.4</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2894,43 +2950,99 @@
         <v>129</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C16" s="13">
         <v>0.2</v>
       </c>
       <c r="D16">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="13"/>
+      <c r="A17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C17" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D17">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>129</v>
       </c>
       <c r="B18" t="s">
-        <v>162</v>
+        <v>126</v>
       </c>
       <c r="C18" s="13">
         <v>0.2</v>
       </c>
       <c r="D18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="13"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" t="s">
+        <v>162</v>
+      </c>
+      <c r="C20" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D20">
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>129</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>163</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C21" s="13">
         <v>0.2</v>
       </c>
-      <c r="D19">
+      <c r="D21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>129</v>
+      </c>
+      <c r="B22" t="s">
+        <v>166</v>
+      </c>
+      <c r="C22" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" t="s">
+        <v>167</v>
+      </c>
+      <c r="C23" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D23">
         <v>0.5</v>
       </c>
     </row>
@@ -3872,7 +3984,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="38" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -3902,7 +4014,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
+      <c r="A31" s="38"/>
       <c r="B31" s="3" t="s">
         <v>25</v>
       </c>
@@ -3930,7 +4042,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="35"/>
+      <c r="A32" s="38"/>
       <c r="B32" s="3" t="s">
         <v>24</v>
       </c>
@@ -3958,7 +4070,7 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
+      <c r="A33" s="38"/>
       <c r="B33" s="3" t="s">
         <v>23</v>
       </c>
@@ -3986,7 +4098,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
+      <c r="A34" s="38"/>
       <c r="B34" s="3" t="s">
         <v>22</v>
       </c>
@@ -4014,7 +4126,7 @@
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="35"/>
+      <c r="A35" s="38"/>
       <c r="B35" s="3" t="s">
         <v>21</v>
       </c>
@@ -5019,12 +5131,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -5235,6 +5341,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5245,15 +5357,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5272,6 +5375,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Remove unused files and be more consistent in file naming
- remove files that are not part of any scenario group
- use SubRES instead of SubRes
- only capitalise acronyms
- remove BASE from Scen_B files
- include H2-GT_MaxGrowth in Scen_B_SYS_MaxGrowthRates.xlsx
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7612DDC-F2A0-41A5-8C2D-2D6405E0F784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6201583-C0F0-4806-848F-BA68AD82CDAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="169">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -557,15 +557,9 @@
     <t>FT*</t>
   </si>
   <si>
-    <t>UC-PWR_MaxGrowthH2GT</t>
-  </si>
-  <si>
     <t>P-TH*H2-*</t>
   </si>
   <si>
-    <t>PWR H2 Gas turbine maximum growth rate</t>
-  </si>
-  <si>
     <t>ACT, GROWTH</t>
   </si>
   <si>
@@ -618,6 +612,9 @@
   </si>
   <si>
     <t>P*SOL*CSP*</t>
+  </si>
+  <si>
+    <t>H2GT</t>
   </si>
 </sst>
 </file>
@@ -697,7 +694,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -737,12 +734,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1124,12 +1115,12 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="264">
     <cellStyle name="20% - Accent5 2" xfId="10" xr:uid="{72E8C261-0B7B-4154-8B6F-C9901D88251B}"/>
@@ -2541,7 +2532,7 @@
   <dimension ref="A2:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2710,14 +2701,14 @@
         <v>1</v>
       </c>
       <c r="L7" s="33">
-        <f t="shared" ref="L7:L8" si="0">-D17</f>
+        <f t="shared" ref="L7:L9" si="0">-D17</f>
         <v>-0.4</v>
       </c>
       <c r="M7" s="2">
         <v>5</v>
       </c>
       <c r="N7" s="2" t="str">
-        <f t="shared" ref="N7:N8" si="1">_xlfn.TEXTJOIN(" ",TRUE,A17, "maximum growth rate of",B17)</f>
+        <f t="shared" ref="N7:N9" si="1">_xlfn.TEXTJOIN(" ",TRUE,A17, "maximum growth rate of",B17)</f>
         <v>PWR maximum growth rate of Wave</v>
       </c>
     </row>
@@ -2758,39 +2749,42 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A19,"MaxGrowth",B19)</f>
+        <v>UC_PWR_MaxGrowth_H2GT</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="C9" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35" t="s">
-        <v>150</v>
-      </c>
-      <c r="H9" s="35">
+      <c r="H9" s="18">
         <v>2020</v>
       </c>
-      <c r="I9" s="35" t="s">
+      <c r="I9" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="36">
+      <c r="J9" s="37">
+        <f>1+$C19</f>
         <v>1.2</v>
       </c>
-      <c r="K9" s="35">
+      <c r="K9" s="36">
         <v>1</v>
       </c>
-      <c r="L9" s="37">
-        <f>L6</f>
-        <v>-0.4</v>
-      </c>
-      <c r="M9" s="35">
+      <c r="L9" s="38">
+        <f t="shared" si="0"/>
+        <v>-0.5</v>
+      </c>
+      <c r="M9" s="18">
         <v>5</v>
       </c>
-      <c r="N9" s="35" t="s">
-        <v>151</v>
+      <c r="N9" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>PWR maximum growth rate of H2GT</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -2802,7 +2796,7 @@
         <v>13</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H10">
         <v>2018</v>
@@ -2838,7 +2832,7 @@
         <v>13</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H11">
         <v>2018</v>
@@ -2874,7 +2868,7 @@
         <v>13</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H12">
         <v>2018</v>
@@ -2910,7 +2904,7 @@
         <v>13</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H13">
         <v>2018</v>
@@ -2988,14 +2982,25 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="13"/>
+      <c r="A19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C19" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D19">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>129</v>
       </c>
       <c r="B20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C20" s="13">
         <v>0.2</v>
@@ -3009,7 +3014,7 @@
         <v>129</v>
       </c>
       <c r="B21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C21" s="13">
         <v>0.2</v>
@@ -3023,7 +3028,7 @@
         <v>129</v>
       </c>
       <c r="B22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C22" s="13">
         <v>0.2</v>
@@ -3037,7 +3042,7 @@
         <v>129</v>
       </c>
       <c r="B23" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C23" s="13">
         <v>0.2</v>
@@ -3912,24 +3917,24 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J26" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K26" t="s">
         <v>117</v>
       </c>
       <c r="L26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I27" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J27" t="s">
         <v>135</v>
@@ -3946,7 +3951,7 @@
         <v>29</v>
       </c>
       <c r="I28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J28" t="s">
         <v>136</v>
@@ -3971,10 +3976,10 @@
         <v>32</v>
       </c>
       <c r="I29" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J29" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K29" s="13">
         <v>0.5</v>
@@ -3984,7 +3989,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="35" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -4001,7 +4006,7 @@
         <v>4.3671013742841359E-2</v>
       </c>
       <c r="I30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J30" t="s">
         <v>137</v>
@@ -4014,7 +4019,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="38"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="3" t="s">
         <v>25</v>
       </c>
@@ -4042,7 +4047,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="38"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="3" t="s">
         <v>24</v>
       </c>
@@ -4070,7 +4075,7 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="38"/>
+      <c r="A33" s="35"/>
       <c r="B33" s="3" t="s">
         <v>23</v>
       </c>
@@ -4088,7 +4093,7 @@
         <v>138</v>
       </c>
       <c r="J33" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K33" s="13">
         <v>0.5</v>
@@ -4098,7 +4103,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
+      <c r="A34" s="35"/>
       <c r="B34" s="3" t="s">
         <v>22</v>
       </c>
@@ -4126,7 +4131,7 @@
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="38"/>
+      <c r="A35" s="35"/>
       <c r="B35" s="3" t="s">
         <v>21</v>
       </c>
@@ -4171,7 +4176,7 @@
         <v>139</v>
       </c>
       <c r="J36" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K36" s="13">
         <v>0.5</v>
@@ -4198,7 +4203,7 @@
         <v>139</v>
       </c>
       <c r="J37" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K37" s="13">
         <v>0.5</v>
@@ -4284,7 +4289,7 @@
         <v>141</v>
       </c>
       <c r="J41" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K41" s="13">
         <v>0.5</v>
@@ -4298,7 +4303,7 @@
         <v>141</v>
       </c>
       <c r="J42" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K42" s="13">
         <v>0.5</v>
@@ -4966,10 +4971,10 @@
         <v>8</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>43</v>
@@ -4987,7 +4992,7 @@
         <v>UC_SRV_MaxGrowth_Biomass</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D11" s="2"/>
       <c r="F11" s="2" t="s">
@@ -5027,7 +5032,7 @@
         <v>UC_SRV_MaxGrowth_Biogas</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D12" s="2"/>
       <c r="F12" s="2" t="s">
@@ -5131,6 +5136,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -5341,12 +5352,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5357,6 +5362,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5375,15 +5389,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>

</xml_diff>